<commit_message>
Zmiana dot kolumny K. Kolumna przyjmuje wartości N lub K. Wartość == N gdy teskst zawarty w STW_TEKST zaczyna się od dużej litery, w przeciwnym razie przyjmuje wartość == K.
</commit_message>
<xml_diff>
--- a/UEFTA_Teksty.xlsx
+++ b/UEFTA_Teksty.xlsx
@@ -1635,11 +1635,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AE171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA1" sqref="AA1"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A148" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D159" sqref="D159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1647,9 +1648,9 @@
     <col min="1" max="1" width="6.5703125" style="3" customWidth="1"/>
     <col min="2" max="2" width="15.42578125" style="3" customWidth="1"/>
     <col min="3" max="3" width="6" style="3" customWidth="1"/>
-    <col min="4" max="4" width="13" style="3" customWidth="1"/>
+    <col min="4" max="4" width="29.42578125" style="3" customWidth="1"/>
     <col min="5" max="5" width="2" style="3" customWidth="1"/>
-    <col min="6" max="6" width="35" style="3" customWidth="1"/>
+    <col min="6" max="6" width="54.7109375" style="3" customWidth="1"/>
     <col min="7" max="7" width="11.28515625" style="3" customWidth="1"/>
     <col min="8" max="8" width="11" style="12" customWidth="1"/>
     <col min="9" max="9" width="14.42578125" style="12" customWidth="1"/>
@@ -1790,7 +1791,7 @@
         <v>3001</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L2" s="12" t="s">
         <v>202</v>
@@ -1806,7 +1807,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>134</v>
       </c>
@@ -1853,7 +1854,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="4" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>134</v>
       </c>
@@ -1882,7 +1883,7 @@
         <v>3001</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L4" s="12" t="s">
         <v>202</v>
@@ -1894,7 +1895,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="5" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>134</v>
       </c>
@@ -1926,7 +1927,7 @@
         <v>3</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L5" s="12" t="s">
         <v>202</v>
@@ -1947,7 +1948,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="6" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>134</v>
       </c>
@@ -1979,7 +1980,7 @@
         <v>3</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L6" s="13" t="s">
         <v>202</v>
@@ -2014,7 +2015,7 @@
       </c>
       <c r="AE6" s="13"/>
     </row>
-    <row r="7" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>134</v>
       </c>
@@ -2062,7 +2063,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="8" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>134</v>
       </c>
@@ -2091,7 +2092,7 @@
         <v>3072</v>
       </c>
       <c r="K8" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L8" s="12" t="s">
         <v>202</v>
@@ -2106,7 +2107,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="9" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>134</v>
       </c>
@@ -2135,7 +2136,7 @@
         <v>3072</v>
       </c>
       <c r="K9" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L9" s="12" t="s">
         <v>202</v>
@@ -2150,7 +2151,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="10" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>134</v>
       </c>
@@ -2182,7 +2183,7 @@
         <v>7</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L10" s="12" t="s">
         <v>202</v>
@@ -2206,7 +2207,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="11" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>134</v>
       </c>
@@ -2238,7 +2239,7 @@
         <v>7</v>
       </c>
       <c r="K11" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L11" s="12" t="s">
         <v>202</v>
@@ -2264,7 +2265,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="12" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>134</v>
       </c>
@@ -2296,7 +2297,7 @@
         <v>7</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L12" s="12" t="s">
         <v>202</v>
@@ -2315,7 +2316,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="13" spans="1:31" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" ht="49.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>134</v>
       </c>
@@ -2347,7 +2348,7 @@
         <v>7</v>
       </c>
       <c r="K13" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L13" s="12" t="s">
         <v>202</v>
@@ -2373,7 +2374,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="14" spans="1:31" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" ht="58.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>134</v>
       </c>
@@ -2405,7 +2406,7 @@
         <v>7</v>
       </c>
       <c r="K14" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L14" s="12" t="s">
         <v>202</v>
@@ -2434,7 +2435,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="15" spans="1:31" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" ht="70.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>134</v>
       </c>
@@ -2466,7 +2467,7 @@
         <v>7</v>
       </c>
       <c r="K15" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L15" s="12" t="s">
         <v>202</v>
@@ -2492,7 +2493,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="16" spans="1:31" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>134</v>
       </c>
@@ -2524,7 +2525,7 @@
         <v>7</v>
       </c>
       <c r="K16" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L16" s="12" t="s">
         <v>202</v>
@@ -2543,7 +2544,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="17" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>134</v>
       </c>
@@ -2575,7 +2576,7 @@
         <v>7</v>
       </c>
       <c r="K17" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L17" s="12" t="s">
         <v>202</v>
@@ -2594,7 +2595,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="18" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>134</v>
       </c>
@@ -2626,7 +2627,7 @@
         <v>7</v>
       </c>
       <c r="K18" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L18" s="12" t="s">
         <v>202</v>
@@ -2641,7 +2642,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="19" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>134</v>
       </c>
@@ -2673,7 +2674,7 @@
         <v>7</v>
       </c>
       <c r="K19" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L19" s="12" t="s">
         <v>202</v>
@@ -2694,7 +2695,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="20" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>134</v>
       </c>
@@ -2726,7 +2727,7 @@
         <v>7</v>
       </c>
       <c r="K20" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L20" s="12" t="s">
         <v>202</v>
@@ -2747,7 +2748,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="21" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>134</v>
       </c>
@@ -2777,7 +2778,7 @@
       </c>
       <c r="J21" s="13"/>
       <c r="K21" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L21" s="13"/>
       <c r="M21" s="13" t="s">
@@ -2810,7 +2811,7 @@
       <c r="AD21" s="13"/>
       <c r="AE21" s="13"/>
     </row>
-    <row r="22" spans="1:31" s="13" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31" s="13" customFormat="1" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>134</v>
       </c>
@@ -2840,7 +2841,7 @@
       </c>
       <c r="J22" s="12"/>
       <c r="K22" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L22" s="12"/>
       <c r="M22" s="12" t="s">
@@ -2873,7 +2874,7 @@
       <c r="AD22" s="12"/>
       <c r="AE22" s="12"/>
     </row>
-    <row r="23" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>134</v>
       </c>
@@ -2902,7 +2903,7 @@
         <v>3001</v>
       </c>
       <c r="K23" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L23" s="12" t="s">
         <v>202</v>
@@ -2952,7 +2953,7 @@
         <v>3049</v>
       </c>
       <c r="K24" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L24" s="12" t="s">
         <v>202</v>
@@ -2964,7 +2965,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="25" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>134</v>
       </c>
@@ -2994,7 +2995,7 @@
       </c>
       <c r="J25" s="13"/>
       <c r="K25" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L25" s="13" t="s">
         <v>202</v>
@@ -3025,7 +3026,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="26" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>134</v>
       </c>
@@ -3066,7 +3067,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="27" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>134</v>
       </c>
@@ -3098,7 +3099,7 @@
         <v>7</v>
       </c>
       <c r="K27" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L27" s="12" t="s">
         <v>202</v>
@@ -3114,7 +3115,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="28" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>134</v>
       </c>
@@ -3146,7 +3147,7 @@
         <v>7</v>
       </c>
       <c r="K28" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L28" s="12" t="s">
         <v>202</v>
@@ -3191,7 +3192,7 @@
         <v>3068</v>
       </c>
       <c r="K29" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L29" s="12" t="s">
         <v>202</v>
@@ -3203,7 +3204,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="30" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>134</v>
       </c>
@@ -3233,7 +3234,7 @@
       </c>
       <c r="J30" s="13"/>
       <c r="K30" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L30" s="13" t="s">
         <v>202</v>
@@ -3264,7 +3265,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="31" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>134</v>
       </c>
@@ -3305,7 +3306,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="32" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>134</v>
       </c>
@@ -3334,7 +3335,7 @@
         <v>3049</v>
       </c>
       <c r="K32" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L32" s="12" t="s">
         <v>202</v>
@@ -3350,7 +3351,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="33" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>134</v>
       </c>
@@ -3379,7 +3380,7 @@
         <v>3049</v>
       </c>
       <c r="K33" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L33" s="12" t="s">
         <v>202</v>
@@ -3424,7 +3425,7 @@
         <v>3003</v>
       </c>
       <c r="K34" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L34" s="12" t="s">
         <v>202</v>
@@ -3439,7 +3440,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="35" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>134</v>
       </c>
@@ -3468,7 +3469,7 @@
         <v>3068</v>
       </c>
       <c r="K35" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L35" s="12" t="s">
         <v>202</v>
@@ -3484,7 +3485,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="36" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>134</v>
       </c>
@@ -3531,7 +3532,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="37" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>134</v>
       </c>
@@ -3560,7 +3561,7 @@
         <v>3068</v>
       </c>
       <c r="K37" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L37" s="12" t="s">
         <v>202</v>
@@ -3576,7 +3577,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="38" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>134</v>
       </c>
@@ -3605,7 +3606,7 @@
         <v>3068</v>
       </c>
       <c r="K38" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L38" s="12" t="s">
         <v>202</v>
@@ -3620,7 +3621,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="39" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>134</v>
       </c>
@@ -3652,7 +3653,7 @@
         <v>3</v>
       </c>
       <c r="K39" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L39" s="12" t="s">
         <v>202</v>
@@ -3673,7 +3674,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="40" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>134</v>
       </c>
@@ -3705,7 +3706,7 @@
         <v>3</v>
       </c>
       <c r="K40" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L40" s="12" t="s">
         <v>202</v>
@@ -3726,7 +3727,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="41" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>134</v>
       </c>
@@ -3758,7 +3759,7 @@
         <v>3</v>
       </c>
       <c r="K41" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L41" s="12" t="s">
         <v>202</v>
@@ -3779,7 +3780,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="42" spans="1:31" s="13" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:31" s="13" customFormat="1" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>134</v>
       </c>
@@ -3811,7 +3812,7 @@
         <v>3</v>
       </c>
       <c r="K42" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L42" s="12" t="s">
         <v>202</v>
@@ -3846,7 +3847,7 @@
       <c r="AD42" s="12"/>
       <c r="AE42" s="12"/>
     </row>
-    <row r="43" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>134</v>
       </c>
@@ -3878,7 +3879,7 @@
         <v>3</v>
       </c>
       <c r="K43" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L43" s="12" t="s">
         <v>202</v>
@@ -3902,7 +3903,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="44" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>134</v>
       </c>
@@ -3934,7 +3935,7 @@
         <v>3</v>
       </c>
       <c r="K44" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L44" s="12" t="s">
         <v>202</v>
@@ -3958,7 +3959,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="45" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>134</v>
       </c>
@@ -3990,7 +3991,7 @@
         <v>3</v>
       </c>
       <c r="K45" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L45" s="12" t="s">
         <v>202</v>
@@ -4008,7 +4009,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="46" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>134</v>
       </c>
@@ -4040,7 +4041,7 @@
         <v>3</v>
       </c>
       <c r="K46" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L46" s="12" t="s">
         <v>202</v>
@@ -4058,7 +4059,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="47" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>134</v>
       </c>
@@ -4090,7 +4091,7 @@
         <v>3</v>
       </c>
       <c r="K47" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L47" s="12" t="s">
         <v>202</v>
@@ -4105,7 +4106,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="48" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>134</v>
       </c>
@@ -4137,7 +4138,7 @@
         <v>3</v>
       </c>
       <c r="K48" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L48" s="12" t="s">
         <v>202</v>
@@ -4158,7 +4159,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="49" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>134</v>
       </c>
@@ -4190,7 +4191,7 @@
         <v>3</v>
       </c>
       <c r="K49" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L49" s="12" t="s">
         <v>202</v>
@@ -4240,7 +4241,7 @@
         <v>3056</v>
       </c>
       <c r="K50" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L50" s="12" t="s">
         <v>202</v>
@@ -4252,7 +4253,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="51" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>134</v>
       </c>
@@ -4284,7 +4285,7 @@
         <v>1</v>
       </c>
       <c r="K51" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L51" s="12" t="s">
         <v>202</v>
@@ -4299,7 +4300,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="52" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>134</v>
       </c>
@@ -4340,7 +4341,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="53" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>134</v>
       </c>
@@ -4372,7 +4373,7 @@
         <v>3</v>
       </c>
       <c r="K53" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L53" s="12" t="s">
         <v>202</v>
@@ -4387,7 +4388,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="54" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>134</v>
       </c>
@@ -4419,7 +4420,7 @@
         <v>3</v>
       </c>
       <c r="K54" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L54" s="12" t="s">
         <v>202</v>
@@ -4434,7 +4435,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="55" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>134</v>
       </c>
@@ -4466,7 +4467,7 @@
         <v>1</v>
       </c>
       <c r="K55" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L55" s="12" t="s">
         <v>202</v>
@@ -4481,7 +4482,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="56" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>134</v>
       </c>
@@ -4513,7 +4514,7 @@
         <v>2</v>
       </c>
       <c r="K56" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L56" s="12" t="s">
         <v>202</v>
@@ -4560,7 +4561,7 @@
         <v>3058</v>
       </c>
       <c r="K57" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L57" s="12" t="s">
         <v>202</v>
@@ -4572,7 +4573,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="58" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>134</v>
       </c>
@@ -4601,7 +4602,7 @@
         <v>3058</v>
       </c>
       <c r="K58" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L58" s="12" t="s">
         <v>202</v>
@@ -4619,7 +4620,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="59" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>134</v>
       </c>
@@ -4648,7 +4649,7 @@
         <v>3058</v>
       </c>
       <c r="K59" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L59" s="12" t="s">
         <v>202</v>
@@ -4666,7 +4667,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="60" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>134</v>
       </c>
@@ -4695,7 +4696,7 @@
         <v>3058</v>
       </c>
       <c r="K60" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L60" s="12" t="s">
         <v>202</v>
@@ -4713,7 +4714,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="61" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>134</v>
       </c>
@@ -4742,7 +4743,7 @@
         <v>3058</v>
       </c>
       <c r="K61" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L61" s="12" t="s">
         <v>202</v>
@@ -4760,7 +4761,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="62" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>134</v>
       </c>
@@ -4792,7 +4793,7 @@
         <v>1</v>
       </c>
       <c r="K62" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L62" s="12" t="s">
         <v>202</v>
@@ -4807,7 +4808,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="63" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>134</v>
       </c>
@@ -4839,7 +4840,7 @@
         <v>2</v>
       </c>
       <c r="K63" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L63" s="12" t="s">
         <v>202</v>
@@ -4886,7 +4887,7 @@
         <v>3072</v>
       </c>
       <c r="K64" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="M64" s="19" t="s">
         <v>193</v>
@@ -4895,7 +4896,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="65" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>134</v>
       </c>
@@ -4962,7 +4963,7 @@
         <v>3023</v>
       </c>
       <c r="K66" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L66" s="12" t="s">
         <v>202</v>
@@ -4977,7 +4978,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="67" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>134</v>
       </c>
@@ -5006,7 +5007,7 @@
         <v>3023</v>
       </c>
       <c r="K67" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L67" s="12" t="s">
         <v>202</v>
@@ -5021,7 +5022,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="68" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>134</v>
       </c>
@@ -5062,7 +5063,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="69" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>134</v>
       </c>
@@ -5103,7 +5104,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="70" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>134</v>
       </c>
@@ -5135,7 +5136,7 @@
         <v>7</v>
       </c>
       <c r="K70" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L70" s="12" t="s">
         <v>202</v>
@@ -5150,7 +5151,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="71" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>134</v>
       </c>
@@ -5182,7 +5183,7 @@
         <v>7</v>
       </c>
       <c r="K71" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L71" s="12" t="s">
         <v>202</v>
@@ -5197,7 +5198,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="72" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>134</v>
       </c>
@@ -5229,7 +5230,7 @@
         <v>8</v>
       </c>
       <c r="K72" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L72" s="12" t="s">
         <v>202</v>
@@ -5247,7 +5248,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="73" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>134</v>
       </c>
@@ -5279,7 +5280,7 @@
         <v>8</v>
       </c>
       <c r="K73" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L73" s="12" t="s">
         <v>202</v>
@@ -5294,7 +5295,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="74" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>134</v>
       </c>
@@ -5326,7 +5327,7 @@
         <v>8</v>
       </c>
       <c r="K74" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L74" s="12" t="s">
         <v>202</v>
@@ -5341,7 +5342,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="75" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>134</v>
       </c>
@@ -5373,7 +5374,7 @@
         <v>8</v>
       </c>
       <c r="K75" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L75" s="12" t="s">
         <v>202</v>
@@ -5388,7 +5389,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="76" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>134</v>
       </c>
@@ -5420,7 +5421,7 @@
         <v>8</v>
       </c>
       <c r="K76" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L76" s="12" t="s">
         <v>202</v>
@@ -5435,7 +5436,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="77" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>134</v>
       </c>
@@ -5467,7 +5468,7 @@
         <v>8</v>
       </c>
       <c r="K77" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L77" s="12" t="s">
         <v>202</v>
@@ -5485,7 +5486,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="78" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>134</v>
       </c>
@@ -5517,7 +5518,7 @@
         <v>8</v>
       </c>
       <c r="K78" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L78" s="12" t="s">
         <v>202</v>
@@ -5535,7 +5536,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="79" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>134</v>
       </c>
@@ -5567,7 +5568,7 @@
         <v>8</v>
       </c>
       <c r="K79" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L79" s="12" t="s">
         <v>202</v>
@@ -5585,7 +5586,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="80" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>134</v>
       </c>
@@ -5617,7 +5618,7 @@
         <v>8</v>
       </c>
       <c r="K80" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L80" s="12" t="s">
         <v>202</v>
@@ -5635,7 +5636,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="81" spans="1:29" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:29" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>134</v>
       </c>
@@ -5667,7 +5668,7 @@
         <v>8</v>
       </c>
       <c r="K81" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L81" s="12" t="s">
         <v>202</v>
@@ -5682,7 +5683,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="82" spans="1:29" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:29" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>134</v>
       </c>
@@ -5714,7 +5715,7 @@
         <v>8</v>
       </c>
       <c r="K82" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L82" s="12" t="s">
         <v>202</v>
@@ -5735,7 +5736,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="83" spans="1:29" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:29" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>134</v>
       </c>
@@ -5767,7 +5768,7 @@
         <v>8</v>
       </c>
       <c r="K83" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L83" s="12" t="s">
         <v>202</v>
@@ -5788,7 +5789,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="84" spans="1:29" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:29" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>134</v>
       </c>
@@ -5820,7 +5821,7 @@
         <v>8</v>
       </c>
       <c r="K84" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L84" s="12" t="s">
         <v>202</v>
@@ -5841,7 +5842,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="85" spans="1:29" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:29" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>134</v>
       </c>
@@ -5873,7 +5874,7 @@
         <v>8</v>
       </c>
       <c r="K85" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L85" s="12" t="s">
         <v>202</v>
@@ -5894,7 +5895,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="86" spans="1:29" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:29" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>134</v>
       </c>
@@ -5923,7 +5924,7 @@
         <v>3023</v>
       </c>
       <c r="K86" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L86" s="12" t="s">
         <v>202</v>
@@ -5944,7 +5945,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="87" spans="1:29" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:29" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>134</v>
       </c>
@@ -5973,7 +5974,7 @@
         <v>3023</v>
       </c>
       <c r="K87" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L87" s="12" t="s">
         <v>202</v>
@@ -5994,7 +5995,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="88" spans="1:29" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:29" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>134</v>
       </c>
@@ -6023,7 +6024,7 @@
         <v>3023</v>
       </c>
       <c r="K88" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L88" s="12" t="s">
         <v>202</v>
@@ -6073,7 +6074,7 @@
         <v>3042</v>
       </c>
       <c r="K89" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L89" s="12" t="s">
         <v>202</v>
@@ -6085,7 +6086,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="90" spans="1:29" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:29" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>134</v>
       </c>
@@ -6117,7 +6118,7 @@
         <v>3</v>
       </c>
       <c r="K90" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L90" s="12" t="s">
         <v>202</v>
@@ -6138,7 +6139,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="91" spans="1:29" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:29" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>134</v>
       </c>
@@ -6170,7 +6171,7 @@
         <v>3</v>
       </c>
       <c r="K91" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L91" s="12" t="s">
         <v>202</v>
@@ -6191,7 +6192,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="92" spans="1:29" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:29" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>134</v>
       </c>
@@ -6223,7 +6224,7 @@
         <v>3</v>
       </c>
       <c r="K92" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L92" s="12" t="s">
         <v>202</v>
@@ -6241,7 +6242,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="93" spans="1:29" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:29" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>134</v>
       </c>
@@ -6273,7 +6274,7 @@
         <v>3</v>
       </c>
       <c r="K93" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L93" s="12" t="s">
         <v>202</v>
@@ -6291,7 +6292,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="94" spans="1:29" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:29" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>134</v>
       </c>
@@ -6323,7 +6324,7 @@
         <v>3</v>
       </c>
       <c r="K94" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L94" s="12" t="s">
         <v>202</v>
@@ -6341,7 +6342,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="95" spans="1:29" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:29" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>134</v>
       </c>
@@ -6373,7 +6374,7 @@
         <v>3</v>
       </c>
       <c r="K95" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L95" s="12" t="s">
         <v>202</v>
@@ -6391,7 +6392,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="96" spans="1:29" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:29" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>134</v>
       </c>
@@ -6423,7 +6424,7 @@
         <v>3</v>
       </c>
       <c r="K96" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L96" s="12" t="s">
         <v>202</v>
@@ -6438,7 +6439,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="97" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>134</v>
       </c>
@@ -6470,7 +6471,7 @@
         <v>3</v>
       </c>
       <c r="K97" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L97" s="12" t="s">
         <v>202</v>
@@ -6491,7 +6492,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="98" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>134</v>
       </c>
@@ -6523,7 +6524,7 @@
         <v>3</v>
       </c>
       <c r="K98" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L98" s="12" t="s">
         <v>202</v>
@@ -6544,7 +6545,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="99" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
         <v>134</v>
       </c>
@@ -6576,7 +6577,7 @@
         <v>3</v>
       </c>
       <c r="K99" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L99" s="12" t="s">
         <v>202</v>
@@ -6594,7 +6595,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="100" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>134</v>
       </c>
@@ -6626,7 +6627,7 @@
         <v>3</v>
       </c>
       <c r="K100" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L100" s="12" t="s">
         <v>202</v>
@@ -6644,7 +6645,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="101" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>134</v>
       </c>
@@ -6673,7 +6674,7 @@
         <v>3048</v>
       </c>
       <c r="K101" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L101" s="12" t="s">
         <v>202</v>
@@ -6714,7 +6715,7 @@
         <v>3041</v>
       </c>
       <c r="K102" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L102" s="12" t="s">
         <v>202</v>
@@ -6726,7 +6727,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="103" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
         <v>134</v>
       </c>
@@ -6755,7 +6756,7 @@
         <v>3056</v>
       </c>
       <c r="K103" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L103" s="12" t="s">
         <v>202</v>
@@ -6770,7 +6771,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="104" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>134</v>
       </c>
@@ -6814,7 +6815,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="105" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
         <v>134</v>
       </c>
@@ -6846,7 +6847,7 @@
         <v>1</v>
       </c>
       <c r="K105" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L105" s="12" t="s">
         <v>202</v>
@@ -6861,7 +6862,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="106" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
         <v>134</v>
       </c>
@@ -6893,7 +6894,7 @@
         <v>1</v>
       </c>
       <c r="K106" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L106" s="12" t="s">
         <v>202</v>
@@ -6908,7 +6909,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="107" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
         <v>134</v>
       </c>
@@ -6940,7 +6941,7 @@
         <v>4</v>
       </c>
       <c r="K107" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L107" s="12" t="s">
         <v>202</v>
@@ -6961,7 +6962,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="108" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
         <v>134</v>
       </c>
@@ -6993,7 +6994,7 @@
         <v>4</v>
       </c>
       <c r="K108" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L108" s="12" t="s">
         <v>202</v>
@@ -7014,7 +7015,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="109" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
         <v>134</v>
       </c>
@@ -7046,7 +7047,7 @@
         <v>4</v>
       </c>
       <c r="K109" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L109" s="12" t="s">
         <v>202</v>
@@ -7067,7 +7068,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="110" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
         <v>134</v>
       </c>
@@ -7099,7 +7100,7 @@
         <v>4</v>
       </c>
       <c r="K110" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L110" s="12" t="s">
         <v>202</v>
@@ -7120,7 +7121,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="111" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
         <v>134</v>
       </c>
@@ -7152,7 +7153,7 @@
         <v>4</v>
       </c>
       <c r="K111" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L111" s="12" t="s">
         <v>202</v>
@@ -7176,7 +7177,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="112" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
         <v>134</v>
       </c>
@@ -7208,7 +7209,7 @@
         <v>4</v>
       </c>
       <c r="K112" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L112" s="12" t="s">
         <v>202</v>
@@ -7232,7 +7233,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="113" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
         <v>134</v>
       </c>
@@ -7264,7 +7265,7 @@
         <v>4</v>
       </c>
       <c r="K113" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L113" s="12" t="s">
         <v>202</v>
@@ -7282,7 +7283,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="114" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
         <v>134</v>
       </c>
@@ -7314,7 +7315,7 @@
         <v>4</v>
       </c>
       <c r="K114" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L114" s="12" t="s">
         <v>202</v>
@@ -7332,7 +7333,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="115" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
         <v>134</v>
       </c>
@@ -7364,7 +7365,7 @@
         <v>4</v>
       </c>
       <c r="K115" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L115" s="12" t="s">
         <v>202</v>
@@ -7379,7 +7380,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="116" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
         <v>134</v>
       </c>
@@ -7411,7 +7412,7 @@
         <v>4</v>
       </c>
       <c r="K116" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L116" s="12" t="s">
         <v>202</v>
@@ -7432,7 +7433,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="117" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
         <v>134</v>
       </c>
@@ -7464,7 +7465,7 @@
         <v>4</v>
       </c>
       <c r="K117" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L117" s="12" t="s">
         <v>202</v>
@@ -7514,7 +7515,7 @@
         <v>3067</v>
       </c>
       <c r="K118" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L118" s="12" t="s">
         <v>202</v>
@@ -7526,7 +7527,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="119" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
         <v>134</v>
       </c>
@@ -7558,7 +7559,7 @@
         <v>9</v>
       </c>
       <c r="K119" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L119" s="12" t="s">
         <v>202</v>
@@ -7573,7 +7574,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="120" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
         <v>134</v>
       </c>
@@ -7614,7 +7615,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="121" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
         <v>134</v>
       </c>
@@ -7646,7 +7647,7 @@
         <v>4</v>
       </c>
       <c r="K121" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L121" s="12" t="s">
         <v>202</v>
@@ -7661,7 +7662,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="122" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
         <v>134</v>
       </c>
@@ -7693,7 +7694,7 @@
         <v>4</v>
       </c>
       <c r="K122" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L122" s="12" t="s">
         <v>202</v>
@@ -7708,7 +7709,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="123" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
         <v>134</v>
       </c>
@@ -7740,7 +7741,7 @@
         <v>1</v>
       </c>
       <c r="K123" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L123" s="12" t="s">
         <v>202</v>
@@ -7755,7 +7756,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="124" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
         <v>134</v>
       </c>
@@ -7787,7 +7788,7 @@
         <v>2</v>
       </c>
       <c r="K124" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L124" s="12" t="s">
         <v>202</v>
@@ -7805,7 +7806,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="125" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
         <v>134</v>
       </c>
@@ -7837,7 +7838,7 @@
         <v>1</v>
       </c>
       <c r="K125" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L125" s="12" t="s">
         <v>202</v>
@@ -7852,7 +7853,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="126" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
         <v>134</v>
       </c>
@@ -7884,7 +7885,7 @@
         <v>2</v>
       </c>
       <c r="K126" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L126" s="12" t="s">
         <v>202</v>
@@ -7931,7 +7932,7 @@
         <v>3046</v>
       </c>
       <c r="K127" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L127" s="13" t="s">
         <v>202</v>
@@ -7943,7 +7944,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="128" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
         <v>134</v>
       </c>
@@ -7975,7 +7976,7 @@
         <v>3</v>
       </c>
       <c r="K128" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L128" s="12" t="s">
         <v>202</v>
@@ -7996,7 +7997,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="129" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
         <v>134</v>
       </c>
@@ -8028,7 +8029,7 @@
         <v>3</v>
       </c>
       <c r="K129" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L129" s="12" t="s">
         <v>202</v>
@@ -8049,7 +8050,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="130" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
         <v>134</v>
       </c>
@@ -8081,7 +8082,7 @@
         <v>3</v>
       </c>
       <c r="K130" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L130" s="12" t="s">
         <v>202</v>
@@ -8099,7 +8100,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="131" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
         <v>134</v>
       </c>
@@ -8131,7 +8132,7 @@
         <v>3</v>
       </c>
       <c r="K131" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L131" s="12" t="s">
         <v>202</v>
@@ -8149,7 +8150,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="132" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
         <v>134</v>
       </c>
@@ -8181,7 +8182,7 @@
         <v>3</v>
       </c>
       <c r="K132" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L132" s="12" t="s">
         <v>202</v>
@@ -8199,7 +8200,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="133" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
         <v>134</v>
       </c>
@@ -8231,7 +8232,7 @@
         <v>3</v>
       </c>
       <c r="K133" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L133" s="12" t="s">
         <v>202</v>
@@ -8249,7 +8250,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="134" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
         <v>134</v>
       </c>
@@ -8281,7 +8282,7 @@
         <v>3</v>
       </c>
       <c r="K134" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L134" s="12" t="s">
         <v>202</v>
@@ -8296,7 +8297,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="135" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
         <v>134</v>
       </c>
@@ -8328,7 +8329,7 @@
         <v>3</v>
       </c>
       <c r="K135" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L135" s="12" t="s">
         <v>202</v>
@@ -8349,7 +8350,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="136" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
         <v>134</v>
       </c>
@@ -8381,7 +8382,7 @@
         <v>3</v>
       </c>
       <c r="K136" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L136" s="12" t="s">
         <v>202</v>
@@ -8402,7 +8403,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="137" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
         <v>134</v>
       </c>
@@ -8434,7 +8435,7 @@
         <v>3</v>
       </c>
       <c r="K137" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L137" s="12" t="s">
         <v>202</v>
@@ -8452,7 +8453,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="138" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="9" t="s">
         <v>134</v>
       </c>
@@ -8484,7 +8485,7 @@
         <v>3</v>
       </c>
       <c r="K138" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L138" s="13" t="s">
         <v>202</v>
@@ -8517,7 +8518,7 @@
       <c r="AD138" s="13"/>
       <c r="AE138" s="13"/>
     </row>
-    <row r="139" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
         <v>134</v>
       </c>
@@ -8546,7 +8547,7 @@
         <v>3071</v>
       </c>
       <c r="K139" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L139" s="12" t="s">
         <v>202</v>
@@ -8587,7 +8588,7 @@
         <v>3091</v>
       </c>
       <c r="K140" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L140" s="12" t="s">
         <v>202</v>
@@ -8599,7 +8600,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="141" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
         <v>134</v>
       </c>
@@ -8631,7 +8632,7 @@
         <v>3</v>
       </c>
       <c r="K141" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L141" s="12" t="s">
         <v>370</v>
@@ -8640,7 +8641,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="142" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
         <v>134</v>
       </c>
@@ -8672,7 +8673,7 @@
         <v>3</v>
       </c>
       <c r="K142" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L142" s="12" t="s">
         <v>370</v>
@@ -8681,7 +8682,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="143" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
         <v>134</v>
       </c>
@@ -8713,7 +8714,7 @@
         <v>3</v>
       </c>
       <c r="K143" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L143" s="12" t="s">
         <v>370</v>
@@ -8722,7 +8723,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="144" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
         <v>134</v>
       </c>
@@ -8754,7 +8755,7 @@
         <v>3</v>
       </c>
       <c r="K144" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L144" s="12" t="s">
         <v>370</v>
@@ -8763,7 +8764,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="145" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
         <v>134</v>
       </c>
@@ -8804,7 +8805,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="146" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
         <v>134</v>
       </c>
@@ -8845,7 +8846,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="147" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
         <v>134</v>
       </c>
@@ -8886,7 +8887,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="148" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
         <v>134</v>
       </c>
@@ -8927,7 +8928,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="149" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
         <v>134</v>
       </c>
@@ -8968,7 +8969,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="150" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
         <v>134</v>
       </c>
@@ -9009,7 +9010,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="151" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
         <v>134</v>
       </c>
@@ -9038,13 +9039,13 @@
         <v>3097</v>
       </c>
       <c r="K151" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L151" s="12" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="152" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="s">
         <v>134</v>
       </c>
@@ -9082,7 +9083,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="153" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
         <v>134</v>
       </c>
@@ -9120,7 +9121,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="154" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="s">
         <v>134</v>
       </c>
@@ -9158,7 +9159,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="155" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
         <v>134</v>
       </c>
@@ -9196,7 +9197,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="156" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
         <v>134</v>
       </c>
@@ -9234,7 +9235,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="157" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
         <v>134</v>
       </c>
@@ -9272,7 +9273,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="158" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
         <v>134</v>
       </c>
@@ -9301,7 +9302,7 @@
         <v>3097</v>
       </c>
       <c r="K158" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L158" s="12" t="s">
         <v>370</v>
@@ -9339,7 +9340,7 @@
         <v>3</v>
       </c>
       <c r="K159" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L159" s="12" t="s">
         <v>202</v>
@@ -9348,7 +9349,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="160" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
         <v>134</v>
       </c>
@@ -9377,7 +9378,7 @@
         <v>3099</v>
       </c>
       <c r="K160" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L160" s="12" t="s">
         <v>370</v>
@@ -9389,7 +9390,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="161" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
         <v>134</v>
       </c>
@@ -9418,7 +9419,7 @@
         <v>3099</v>
       </c>
       <c r="K161" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L161" s="12" t="s">
         <v>370</v>
@@ -9430,7 +9431,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="162" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
         <v>134</v>
       </c>
@@ -9474,7 +9475,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="163" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
         <v>134</v>
       </c>
@@ -9550,7 +9551,7 @@
         <v>3</v>
       </c>
       <c r="K164" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L164" s="12" t="s">
         <v>202</v>
@@ -9562,7 +9563,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="165" spans="1:31" s="13" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:31" s="13" customFormat="1" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
         <v>134</v>
       </c>
@@ -9592,7 +9593,7 @@
       </c>
       <c r="J165" s="12"/>
       <c r="K165" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L165" s="12" t="s">
         <v>370</v>
@@ -9621,7 +9622,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="166" spans="1:31" s="13" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:31" s="13" customFormat="1" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
         <v>134</v>
       </c>
@@ -9651,7 +9652,7 @@
       </c>
       <c r="J166" s="12"/>
       <c r="K166" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L166" s="12" t="s">
         <v>370</v>
@@ -9680,7 +9681,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="167" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
         <v>134</v>
       </c>
@@ -9724,7 +9725,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="168" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
         <v>134</v>
       </c>
@@ -9768,7 +9769,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="169" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="3" t="s">
         <v>134</v>
       </c>
@@ -9800,7 +9801,7 @@
         <v>5</v>
       </c>
       <c r="K169" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L169" s="12" t="s">
         <v>202</v>
@@ -9815,7 +9816,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="170" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
         <v>134</v>
       </c>
@@ -9847,7 +9848,7 @@
         <v>1</v>
       </c>
       <c r="K170" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L170" s="12" t="s">
         <v>202</v>
@@ -9862,7 +9863,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="171" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="3" t="s">
         <v>134</v>
       </c>
@@ -9894,7 +9895,7 @@
         <v>1</v>
       </c>
       <c r="K171" s="12" t="s">
-        <v>382</v>
+        <v>198</v>
       </c>
       <c r="L171" s="12" t="s">
         <v>202</v>
@@ -9910,7 +9911,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AE171"/>
+  <autoFilter ref="A1:AE171">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="T1_104"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState columnSort="1" ref="K1:T168">
     <sortCondition ref="K1:T1"/>
   </sortState>

</xml_diff>

<commit_message>
Zmiana dla zgłoszenia 144.
W wyniku zgłoszenia 144, uwaga "Nadmiarowo dobrał się tekst "w związku z przeliczeniem kapitału początkowego" bowiem tekst ten dot. przypadków ponownego ustalania emerytury z urzędu a nie na wniosek. " należy wprowadzić zmianę dla tekstu T2a_100 na decyzjach DEC B, DEC B1, DEC B2, DEC C, DEC C1, DEC NSK, DRZ DEC C, DRZ DEC C1: TPR_TRZALPOSTEP = ,2, TRP_KORKAPSKL = ,KKP, TPR_KOREKTAUSTAWA5MARCA = puste
</commit_message>
<xml_diff>
--- a/UEFTA_Teksty.xlsx
+++ b/UEFTA_Teksty.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2155" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2157" uniqueCount="387">
   <si>
     <t>Po ponownym ustaleniu wysokość &lt;NAZWASWIADCZENIAGL&gt; wynosi: 
 &lt;KWOTAKAPITALUPOCZATKOWEGOKOR&gt;/&lt;SREDNIEDALSZETRWANIEZYCIA&gt; = &lt;KWOTAEMERYTURYKOR&gt; zł.</t>
@@ -499,9 +499,6 @@
   </si>
   <si>
     <t>,4,23,80,</t>
-  </si>
-  <si>
-    <t>,KKP, KKPS,</t>
   </si>
   <si>
     <t>DRZ DEC C</t>
@@ -1654,7 +1651,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N1" sqref="N1:N1048576"/>
+      <selection pane="bottomLeft" activeCell="Q120" sqref="Q120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1662,10 +1659,10 @@
     <col min="1" max="1" width="6.5703125" style="3" customWidth="1"/>
     <col min="2" max="2" width="15.42578125" style="3" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="158.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="27" style="3" customWidth="1"/>
     <col min="5" max="5" width="2" style="3" customWidth="1"/>
     <col min="6" max="6" width="39.42578125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" style="3" customWidth="1"/>
     <col min="8" max="8" width="11" style="12" customWidth="1"/>
     <col min="9" max="9" width="14.42578125" style="12" customWidth="1"/>
     <col min="10" max="10" width="8.140625" style="12" customWidth="1"/>
@@ -1676,7 +1673,8 @@
     <col min="15" max="15" width="7.28515625" style="12" customWidth="1"/>
     <col min="16" max="16" width="2.85546875" style="12" customWidth="1"/>
     <col min="17" max="17" width="11.85546875" style="12" customWidth="1"/>
-    <col min="18" max="19" width="4.5703125" style="12" customWidth="1"/>
+    <col min="18" max="18" width="11.28515625" style="12" customWidth="1"/>
+    <col min="19" max="19" width="4.5703125" style="12" customWidth="1"/>
     <col min="20" max="20" width="8.5703125" style="12" bestFit="1" customWidth="1"/>
     <col min="21" max="28" width="3.5703125" style="12" customWidth="1"/>
     <col min="29" max="29" width="3.85546875" style="12" customWidth="1"/>
@@ -1713,7 +1711,7 @@
         <v>134</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>135</v>
@@ -1787,7 +1785,7 @@
         <v>69</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>70</v>
@@ -1832,7 +1830,7 @@
         <v>69</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>70</v>
@@ -1841,7 +1839,7 @@
         <v>2</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>119</v>
@@ -1862,7 +1860,7 @@
         <v>127</v>
       </c>
       <c r="O3" s="14" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AE3" s="15" t="s">
         <v>120</v>
@@ -1879,7 +1877,7 @@
         <v>69</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>70</v>
@@ -1920,7 +1918,7 @@
         <v>69</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>70</v>
@@ -1973,7 +1971,7 @@
         <v>69</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>70</v>
@@ -2034,13 +2032,13 @@
         <v>68</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>70</v>
@@ -2058,7 +2056,7 @@
         <v>3001</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L7" s="12" t="s">
         <v>136</v>
@@ -2070,25 +2068,23 @@
         <v>128</v>
       </c>
       <c r="R7" s="13" t="s">
-        <v>123</v>
+        <v>144</v>
       </c>
       <c r="S7" s="13"/>
-      <c r="AE7" s="13" t="s">
-        <v>120</v>
-      </c>
+      <c r="AE7" s="13"/>
     </row>
     <row r="8" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>70</v>
@@ -2126,13 +2122,13 @@
         <v>68</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>70</v>
@@ -2170,13 +2166,13 @@
         <v>68</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>70</v>
@@ -2226,13 +2222,13 @@
         <v>68</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>70</v>
@@ -2284,13 +2280,13 @@
         <v>68</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>70</v>
@@ -2335,13 +2331,13 @@
         <v>68</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>70</v>
@@ -2393,13 +2389,13 @@
         <v>68</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>70</v>
@@ -2454,13 +2450,13 @@
         <v>68</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>70</v>
@@ -2512,13 +2508,13 @@
         <v>68</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>70</v>
@@ -2563,13 +2559,13 @@
         <v>68</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>70</v>
@@ -2614,13 +2610,13 @@
         <v>68</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>70</v>
@@ -2661,13 +2657,13 @@
         <v>68</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>70</v>
@@ -2714,13 +2710,13 @@
         <v>68</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>70</v>
@@ -2767,13 +2763,13 @@
         <v>68</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>69</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>70</v>
@@ -2830,13 +2826,13 @@
         <v>68</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>70</v>
@@ -2893,13 +2889,13 @@
         <v>68</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>70</v>
@@ -2949,7 +2945,7 @@
         <v>69</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>70</v>
@@ -2990,7 +2986,7 @@
         <v>69</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>70</v>
@@ -3045,13 +3041,13 @@
         <v>68</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>70</v>
@@ -3069,7 +3065,7 @@
         <v>3049</v>
       </c>
       <c r="K26" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L26" s="12" t="s">
         <v>136</v>
@@ -3077,22 +3073,26 @@
       <c r="M26" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="AE26" s="15" t="s">
-        <v>120</v>
-      </c>
+      <c r="N26" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="R26" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="AE26" s="13"/>
     </row>
     <row r="27" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>70</v>
@@ -3134,13 +3134,13 @@
         <v>68</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>70</v>
@@ -3188,7 +3188,7 @@
         <v>69</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>70</v>
@@ -3229,7 +3229,7 @@
         <v>69</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>70</v>
@@ -3284,13 +3284,13 @@
         <v>68</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>70</v>
@@ -3308,7 +3308,7 @@
         <v>3068</v>
       </c>
       <c r="K31" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L31" s="12" t="s">
         <v>136</v>
@@ -3316,22 +3316,26 @@
       <c r="M31" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="AE31" s="15" t="s">
-        <v>120</v>
-      </c>
+      <c r="N31" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="R31" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="AE31" s="13"/>
     </row>
     <row r="32" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>70</v>
@@ -3370,13 +3374,13 @@
         <v>68</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>70</v>
@@ -3421,7 +3425,7 @@
         <v>69</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>70</v>
@@ -3465,7 +3469,7 @@
         <v>69</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>70</v>
@@ -3504,13 +3508,13 @@
         <v>68</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>70</v>
@@ -3528,7 +3532,7 @@
         <v>3003</v>
       </c>
       <c r="K36" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L36" s="12" t="s">
         <v>136</v>
@@ -3539,25 +3543,23 @@
       <c r="N36" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="R36" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="AE36" s="14" t="s">
-        <v>120</v>
-      </c>
+      <c r="R36" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="AE36" s="13"/>
     </row>
     <row r="37" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>70</v>
@@ -3596,13 +3598,13 @@
         <v>68</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>70</v>
@@ -3640,13 +3642,13 @@
         <v>68</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>70</v>
@@ -3693,13 +3695,13 @@
         <v>68</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>70</v>
@@ -3746,13 +3748,13 @@
         <v>68</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>70</v>
@@ -3799,13 +3801,13 @@
         <v>68</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>70</v>
@@ -3866,13 +3868,13 @@
         <v>68</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>70</v>
@@ -3922,13 +3924,13 @@
         <v>68</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>70</v>
@@ -3978,13 +3980,13 @@
         <v>68</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>70</v>
@@ -4028,13 +4030,13 @@
         <v>68</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>70</v>
@@ -4078,13 +4080,13 @@
         <v>68</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>70</v>
@@ -4125,13 +4127,13 @@
         <v>68</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E48" s="5" t="s">
         <v>70</v>
@@ -4178,13 +4180,13 @@
         <v>68</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E49" s="5" t="s">
         <v>70</v>
@@ -4237,7 +4239,7 @@
         <v>69</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E50" s="5" t="s">
         <v>70</v>
@@ -4249,7 +4251,7 @@
         <v>122</v>
       </c>
       <c r="H50" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I50" s="12">
         <v>3056</v>
@@ -4261,7 +4263,7 @@
         <v>136</v>
       </c>
       <c r="M50" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AE50" s="15" t="s">
         <v>120</v>
@@ -4278,7 +4280,7 @@
         <v>69</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E51" s="5" t="s">
         <v>70</v>
@@ -4319,13 +4321,13 @@
         <v>68</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E52" s="5" t="s">
         <v>70</v>
@@ -4337,36 +4339,40 @@
         <v>124</v>
       </c>
       <c r="H52" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I52" s="12">
         <v>3056</v>
       </c>
       <c r="K52" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L52" s="12" t="s">
         <v>136</v>
       </c>
       <c r="M52" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="AE52" s="15" t="s">
-        <v>120</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="N52" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="R52" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="AE52" s="13"/>
     </row>
     <row r="53" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>70</v>
@@ -4407,13 +4413,13 @@
         <v>68</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E54" s="5" t="s">
         <v>70</v>
@@ -4460,7 +4466,7 @@
         <v>69</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E55" s="5" t="s">
         <v>70</v>
@@ -4472,7 +4478,7 @@
         <v>141</v>
       </c>
       <c r="H55" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I55" s="12">
         <v>3033</v>
@@ -4487,7 +4493,7 @@
         <v>136</v>
       </c>
       <c r="M55" s="14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="W55" s="15" t="s">
         <v>132</v>
@@ -4507,7 +4513,7 @@
         <v>69</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E56" s="5" t="s">
         <v>70</v>
@@ -4519,7 +4525,7 @@
         <v>141</v>
       </c>
       <c r="H56" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I56" s="12">
         <v>3033</v>
@@ -4534,7 +4540,7 @@
         <v>136</v>
       </c>
       <c r="M56" s="14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="W56" s="15" t="s">
         <v>120</v>
@@ -4557,7 +4563,7 @@
         <v>69</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E57" s="5" t="s">
         <v>70</v>
@@ -4569,7 +4575,7 @@
         <v>122</v>
       </c>
       <c r="H57" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I57" s="12">
         <v>3058</v>
@@ -4581,7 +4587,7 @@
         <v>136</v>
       </c>
       <c r="M57" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AC57" s="14" t="s">
         <v>120</v>
@@ -4598,7 +4604,7 @@
         <v>69</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E58" s="5" t="s">
         <v>70</v>
@@ -4607,10 +4613,10 @@
         <v>48</v>
       </c>
       <c r="G58" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H58" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I58" s="12">
         <v>3058</v>
@@ -4622,7 +4628,7 @@
         <v>136</v>
       </c>
       <c r="M58" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="U58" s="14" t="s">
         <v>132</v>
@@ -4645,7 +4651,7 @@
         <v>69</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E59" s="5" t="s">
         <v>70</v>
@@ -4654,10 +4660,10 @@
         <v>48</v>
       </c>
       <c r="G59" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H59" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I59" s="12">
         <v>3058</v>
@@ -4669,7 +4675,7 @@
         <v>136</v>
       </c>
       <c r="M59" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="U59" s="14" t="s">
         <v>132</v>
@@ -4692,7 +4698,7 @@
         <v>69</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E60" s="5" t="s">
         <v>70</v>
@@ -4701,10 +4707,10 @@
         <v>48</v>
       </c>
       <c r="G60" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H60" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I60" s="12">
         <v>3058</v>
@@ -4716,7 +4722,7 @@
         <v>136</v>
       </c>
       <c r="M60" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="U60" s="14" t="s">
         <v>120</v>
@@ -4739,7 +4745,7 @@
         <v>69</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E61" s="5" t="s">
         <v>70</v>
@@ -4748,10 +4754,10 @@
         <v>49</v>
       </c>
       <c r="G61" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H61" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I61" s="12">
         <v>3058</v>
@@ -4763,7 +4769,7 @@
         <v>136</v>
       </c>
       <c r="M61" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="U61" s="14" t="s">
         <v>120</v>
@@ -4786,7 +4792,7 @@
         <v>69</v>
       </c>
       <c r="D62" s="16" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E62" s="5" t="s">
         <v>70</v>
@@ -4798,7 +4804,7 @@
         <v>141</v>
       </c>
       <c r="H62" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I62" s="12">
         <v>3047</v>
@@ -4813,7 +4819,7 @@
         <v>136</v>
       </c>
       <c r="M62" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="W62" s="17" t="s">
         <v>132</v>
@@ -4833,7 +4839,7 @@
         <v>69</v>
       </c>
       <c r="D63" s="16" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E63" s="5" t="s">
         <v>70</v>
@@ -4845,7 +4851,7 @@
         <v>141</v>
       </c>
       <c r="H63" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I63" s="12">
         <v>3047</v>
@@ -4860,7 +4866,7 @@
         <v>136</v>
       </c>
       <c r="M63" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="W63" s="17" t="s">
         <v>120</v>
@@ -4883,7 +4889,7 @@
         <v>69</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E64" s="5" t="s">
         <v>70</v>
@@ -4921,7 +4927,7 @@
         <v>69</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E65" s="5" t="s">
         <v>70</v>
@@ -4939,14 +4945,15 @@
         <v>3072</v>
       </c>
       <c r="K65" s="12" t="s">
-        <v>316</v>
-      </c>
-      <c r="R65" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="AE65" s="12" t="s">
-        <v>120</v>
-      </c>
+        <v>315</v>
+      </c>
+      <c r="N65" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="R65" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="AE65" s="13"/>
     </row>
     <row r="66" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
@@ -4959,7 +4966,7 @@
         <v>69</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E66" s="5" t="s">
         <v>70</v>
@@ -4971,7 +4978,7 @@
         <v>122</v>
       </c>
       <c r="H66" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I66" s="12">
         <v>3023</v>
@@ -5003,7 +5010,7 @@
         <v>69</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E67" s="5" t="s">
         <v>70</v>
@@ -5015,7 +5022,7 @@
         <v>3762</v>
       </c>
       <c r="H67" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I67" s="12">
         <v>3023</v>
@@ -5041,13 +5048,13 @@
         <v>68</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E68" s="5" t="s">
         <v>70</v>
@@ -5056,16 +5063,16 @@
         <v>23</v>
       </c>
       <c r="G68" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H68" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I68" s="12">
         <v>3023</v>
       </c>
       <c r="K68" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L68" s="12" t="s">
         <v>136</v>
@@ -5082,13 +5089,13 @@
         <v>68</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E69" s="5" t="s">
         <v>70</v>
@@ -5097,16 +5104,16 @@
         <v>24</v>
       </c>
       <c r="G69" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H69" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I69" s="12">
         <v>3023</v>
       </c>
       <c r="K69" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L69" s="12" t="s">
         <v>136</v>
@@ -5123,13 +5130,13 @@
         <v>68</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E70" s="5" t="s">
         <v>70</v>
@@ -5141,7 +5148,7 @@
         <v>137</v>
       </c>
       <c r="H70" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I70" s="12">
         <v>3023</v>
@@ -5156,7 +5163,7 @@
         <v>136</v>
       </c>
       <c r="M70" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="R70" s="11" t="s">
         <v>138</v>
@@ -5170,13 +5177,13 @@
         <v>68</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E71" s="5" t="s">
         <v>70</v>
@@ -5188,7 +5195,7 @@
         <v>137</v>
       </c>
       <c r="H71" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I71" s="12">
         <v>3023</v>
@@ -5203,7 +5210,7 @@
         <v>136</v>
       </c>
       <c r="M71" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="R71" s="11" t="s">
         <v>144</v>
@@ -5217,13 +5224,13 @@
         <v>68</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E72" s="5" t="s">
         <v>70</v>
@@ -5235,7 +5242,7 @@
         <v>137</v>
       </c>
       <c r="H72" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I72" s="12">
         <v>3023</v>
@@ -5250,7 +5257,7 @@
         <v>136</v>
       </c>
       <c r="M72" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N72" s="11" t="s">
         <v>128</v>
@@ -5267,13 +5274,13 @@
         <v>68</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E73" s="5" t="s">
         <v>70</v>
@@ -5285,7 +5292,7 @@
         <v>137</v>
       </c>
       <c r="H73" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I73" s="12">
         <v>3023</v>
@@ -5300,7 +5307,7 @@
         <v>136</v>
       </c>
       <c r="M73" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N73" s="11" t="s">
         <v>128</v>
@@ -5314,13 +5321,13 @@
         <v>68</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E74" s="5" t="s">
         <v>70</v>
@@ -5332,7 +5339,7 @@
         <v>137</v>
       </c>
       <c r="H74" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I74" s="12">
         <v>3023</v>
@@ -5347,7 +5354,7 @@
         <v>136</v>
       </c>
       <c r="M74" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="R74" s="11" t="s">
         <v>138</v>
@@ -5361,13 +5368,13 @@
         <v>68</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E75" s="5" t="s">
         <v>70</v>
@@ -5379,7 +5386,7 @@
         <v>137</v>
       </c>
       <c r="H75" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I75" s="12">
         <v>3023</v>
@@ -5394,10 +5401,10 @@
         <v>136</v>
       </c>
       <c r="M75" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="R75" s="11" t="s">
         <v>154</v>
-      </c>
-      <c r="R75" s="11" t="s">
-        <v>155</v>
       </c>
       <c r="T75" s="11" t="s">
         <v>120</v>
@@ -5408,13 +5415,13 @@
         <v>68</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E76" s="5" t="s">
         <v>70</v>
@@ -5426,7 +5433,7 @@
         <v>137</v>
       </c>
       <c r="H76" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I76" s="12">
         <v>3023</v>
@@ -5441,7 +5448,7 @@
         <v>136</v>
       </c>
       <c r="M76" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="R76" s="11" t="s">
         <v>144</v>
@@ -5455,13 +5462,13 @@
         <v>68</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C77" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E77" s="5" t="s">
         <v>70</v>
@@ -5473,7 +5480,7 @@
         <v>137</v>
       </c>
       <c r="H77" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I77" s="12">
         <v>3023</v>
@@ -5488,7 +5495,7 @@
         <v>136</v>
       </c>
       <c r="M77" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Z77" s="11" t="s">
         <v>132</v>
@@ -5505,13 +5512,13 @@
         <v>68</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C78" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E78" s="5" t="s">
         <v>70</v>
@@ -5523,7 +5530,7 @@
         <v>137</v>
       </c>
       <c r="H78" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I78" s="12">
         <v>3023</v>
@@ -5538,7 +5545,7 @@
         <v>136</v>
       </c>
       <c r="M78" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Z78" s="11" t="s">
         <v>132</v>
@@ -5555,13 +5562,13 @@
         <v>68</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C79" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E79" s="5" t="s">
         <v>70</v>
@@ -5573,7 +5580,7 @@
         <v>137</v>
       </c>
       <c r="H79" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I79" s="12">
         <v>3023</v>
@@ -5588,7 +5595,7 @@
         <v>136</v>
       </c>
       <c r="M79" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Z79" s="11" t="s">
         <v>120</v>
@@ -5605,13 +5612,13 @@
         <v>68</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C80" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E80" s="5" t="s">
         <v>70</v>
@@ -5623,7 +5630,7 @@
         <v>137</v>
       </c>
       <c r="H80" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I80" s="12">
         <v>3023</v>
@@ -5638,7 +5645,7 @@
         <v>136</v>
       </c>
       <c r="M80" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Z80" s="11" t="s">
         <v>120</v>
@@ -5655,13 +5662,13 @@
         <v>68</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C81" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E81" s="5" t="s">
         <v>70</v>
@@ -5673,7 +5680,7 @@
         <v>137</v>
       </c>
       <c r="H81" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I81" s="12">
         <v>3023</v>
@@ -5688,7 +5695,7 @@
         <v>136</v>
       </c>
       <c r="M81" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AB81" s="11">
         <v>4</v>
@@ -5702,13 +5709,13 @@
         <v>68</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C82" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E82" s="5" t="s">
         <v>70</v>
@@ -5720,7 +5727,7 @@
         <v>137</v>
       </c>
       <c r="H82" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I82" s="12">
         <v>3023</v>
@@ -5735,7 +5742,7 @@
         <v>136</v>
       </c>
       <c r="M82" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Q82" s="11">
         <v>700</v>
@@ -5755,13 +5762,13 @@
         <v>68</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C83" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E83" s="5" t="s">
         <v>70</v>
@@ -5773,7 +5780,7 @@
         <v>137</v>
       </c>
       <c r="H83" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I83" s="12">
         <v>3023</v>
@@ -5788,7 +5795,7 @@
         <v>136</v>
       </c>
       <c r="M83" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Q83" s="11">
         <v>700</v>
@@ -5808,13 +5815,13 @@
         <v>68</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E84" s="5" t="s">
         <v>70</v>
@@ -5826,7 +5833,7 @@
         <v>137</v>
       </c>
       <c r="H84" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I84" s="12">
         <v>3023</v>
@@ -5841,7 +5848,7 @@
         <v>136</v>
       </c>
       <c r="M84" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="V84" s="11" t="s">
         <v>120</v>
@@ -5861,13 +5868,13 @@
         <v>68</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C85" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E85" s="5" t="s">
         <v>70</v>
@@ -5879,7 +5886,7 @@
         <v>137</v>
       </c>
       <c r="H85" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I85" s="12">
         <v>3023</v>
@@ -5894,7 +5901,7 @@
         <v>136</v>
       </c>
       <c r="M85" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="V85" s="11" t="s">
         <v>120</v>
@@ -5914,13 +5921,13 @@
         <v>68</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C86" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E86" s="5" t="s">
         <v>70</v>
@@ -5932,7 +5939,7 @@
         <v>133</v>
       </c>
       <c r="H86" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I86" s="12">
         <v>3023</v>
@@ -5944,7 +5951,7 @@
         <v>136</v>
       </c>
       <c r="M86" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="O86" s="11" t="s">
         <v>120</v>
@@ -5964,13 +5971,13 @@
         <v>68</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C87" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E87" s="5" t="s">
         <v>70</v>
@@ -5982,7 +5989,7 @@
         <v>133</v>
       </c>
       <c r="H87" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I87" s="12">
         <v>3023</v>
@@ -5994,16 +6001,16 @@
         <v>136</v>
       </c>
       <c r="M87" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="O87" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="P87" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="R87" s="11" t="s">
         <v>154</v>
-      </c>
-      <c r="O87" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="P87" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="R87" s="11" t="s">
-        <v>155</v>
       </c>
       <c r="T87" s="11" t="s">
         <v>120</v>
@@ -6014,13 +6021,13 @@
         <v>68</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C88" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E88" s="5" t="s">
         <v>70</v>
@@ -6032,7 +6039,7 @@
         <v>133</v>
       </c>
       <c r="H88" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I88" s="12">
         <v>3023</v>
@@ -6044,7 +6051,7 @@
         <v>136</v>
       </c>
       <c r="M88" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="O88" s="11" t="s">
         <v>120</v>
@@ -6070,7 +6077,7 @@
         <v>69</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E89" s="5" t="s">
         <v>70</v>
@@ -6082,7 +6089,7 @@
         <v>122</v>
       </c>
       <c r="H89" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I89" s="12">
         <v>3042</v>
@@ -6094,7 +6101,7 @@
         <v>136</v>
       </c>
       <c r="M89" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AC89" s="15" t="s">
         <v>120</v>
@@ -6105,13 +6112,13 @@
         <v>68</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C90" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E90" s="5" t="s">
         <v>70</v>
@@ -6123,7 +6130,7 @@
         <v>137</v>
       </c>
       <c r="H90" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I90" s="12">
         <v>3042</v>
@@ -6138,7 +6145,7 @@
         <v>136</v>
       </c>
       <c r="M90" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N90" s="10" t="s">
         <v>128</v>
@@ -6158,13 +6165,13 @@
         <v>68</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C91" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E91" s="5" t="s">
         <v>70</v>
@@ -6176,7 +6183,7 @@
         <v>137</v>
       </c>
       <c r="H91" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I91" s="12">
         <v>3042</v>
@@ -6191,7 +6198,7 @@
         <v>136</v>
       </c>
       <c r="M91" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N91" s="10" t="s">
         <v>128</v>
@@ -6211,13 +6218,13 @@
         <v>68</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C92" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E92" s="5" t="s">
         <v>70</v>
@@ -6229,7 +6236,7 @@
         <v>137</v>
       </c>
       <c r="H92" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I92" s="12">
         <v>3042</v>
@@ -6244,7 +6251,7 @@
         <v>136</v>
       </c>
       <c r="M92" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Z92" s="15" t="s">
         <v>132</v>
@@ -6261,13 +6268,13 @@
         <v>68</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C93" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E93" s="5" t="s">
         <v>70</v>
@@ -6279,7 +6286,7 @@
         <v>137</v>
       </c>
       <c r="H93" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I93" s="12">
         <v>3042</v>
@@ -6294,7 +6301,7 @@
         <v>136</v>
       </c>
       <c r="M93" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Z93" s="15" t="s">
         <v>132</v>
@@ -6311,13 +6318,13 @@
         <v>68</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C94" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D94" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E94" s="5" t="s">
         <v>70</v>
@@ -6329,7 +6336,7 @@
         <v>137</v>
       </c>
       <c r="H94" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I94" s="12">
         <v>3042</v>
@@ -6344,7 +6351,7 @@
         <v>136</v>
       </c>
       <c r="M94" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Z94" s="15" t="s">
         <v>120</v>
@@ -6361,13 +6368,13 @@
         <v>68</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C95" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E95" s="5" t="s">
         <v>70</v>
@@ -6379,7 +6386,7 @@
         <v>137</v>
       </c>
       <c r="H95" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I95" s="12">
         <v>3042</v>
@@ -6394,7 +6401,7 @@
         <v>136</v>
       </c>
       <c r="M95" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Z95" s="15" t="s">
         <v>120</v>
@@ -6411,13 +6418,13 @@
         <v>68</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C96" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E96" s="5" t="s">
         <v>70</v>
@@ -6429,7 +6436,7 @@
         <v>137</v>
       </c>
       <c r="H96" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I96" s="12">
         <v>3042</v>
@@ -6444,7 +6451,7 @@
         <v>136</v>
       </c>
       <c r="M96" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AB96" s="15">
         <v>4</v>
@@ -6458,13 +6465,13 @@
         <v>68</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C97" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E97" s="5" t="s">
         <v>70</v>
@@ -6476,7 +6483,7 @@
         <v>137</v>
       </c>
       <c r="H97" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I97" s="12">
         <v>3042</v>
@@ -6491,10 +6498,10 @@
         <v>136</v>
       </c>
       <c r="M97" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q97" s="14" t="s">
         <v>167</v>
-      </c>
-      <c r="Q97" s="14" t="s">
-        <v>168</v>
       </c>
       <c r="Z97" s="15" t="s">
         <v>132</v>
@@ -6511,13 +6518,13 @@
         <v>68</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C98" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D98" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E98" s="5" t="s">
         <v>70</v>
@@ -6529,7 +6536,7 @@
         <v>137</v>
       </c>
       <c r="H98" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I98" s="12">
         <v>3042</v>
@@ -6544,10 +6551,10 @@
         <v>136</v>
       </c>
       <c r="M98" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q98" s="14" t="s">
         <v>167</v>
-      </c>
-      <c r="Q98" s="14" t="s">
-        <v>168</v>
       </c>
       <c r="Z98" s="15" t="s">
         <v>132</v>
@@ -6564,13 +6571,13 @@
         <v>68</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C99" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E99" s="5" t="s">
         <v>70</v>
@@ -6582,7 +6589,7 @@
         <v>137</v>
       </c>
       <c r="H99" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I99" s="12">
         <v>3042</v>
@@ -6597,7 +6604,7 @@
         <v>136</v>
       </c>
       <c r="M99" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="V99" s="15" t="s">
         <v>120</v>
@@ -6614,13 +6621,13 @@
         <v>68</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C100" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E100" s="5" t="s">
         <v>70</v>
@@ -6632,7 +6639,7 @@
         <v>137</v>
       </c>
       <c r="H100" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I100" s="12">
         <v>3042</v>
@@ -6647,7 +6654,7 @@
         <v>136</v>
       </c>
       <c r="M100" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="V100" s="15" t="s">
         <v>120</v>
@@ -6670,7 +6677,7 @@
         <v>69</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E101" s="5" t="s">
         <v>70</v>
@@ -6682,7 +6689,7 @@
         <v>141</v>
       </c>
       <c r="H101" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I101" s="12">
         <v>3048</v>
@@ -6711,7 +6718,7 @@
         <v>69</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E102" s="5" t="s">
         <v>70</v>
@@ -6723,7 +6730,7 @@
         <v>122</v>
       </c>
       <c r="H102" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I102" s="12">
         <v>3041</v>
@@ -6752,7 +6759,7 @@
         <v>69</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E103" s="5" t="s">
         <v>70</v>
@@ -6764,7 +6771,7 @@
         <v>3762</v>
       </c>
       <c r="H103" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I103" s="12">
         <v>3056</v>
@@ -6776,7 +6783,7 @@
         <v>136</v>
       </c>
       <c r="M103" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="R103" s="14" t="s">
         <v>123</v>
@@ -6790,13 +6797,13 @@
         <v>68</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C104" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E104" s="5" t="s">
         <v>70</v>
@@ -6808,13 +6815,13 @@
         <v>124</v>
       </c>
       <c r="H104" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I104" s="12">
         <v>3041</v>
       </c>
       <c r="K104" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L104" s="12" t="s">
         <v>136</v>
@@ -6825,22 +6832,23 @@
       <c r="N104" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="AE104" s="14" t="s">
-        <v>120</v>
-      </c>
+      <c r="R104" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="AE104" s="13"/>
     </row>
     <row r="105" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C105" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E105" s="5" t="s">
         <v>70</v>
@@ -6852,7 +6860,7 @@
         <v>137</v>
       </c>
       <c r="H105" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I105" s="12">
         <v>3056</v>
@@ -6867,10 +6875,10 @@
         <v>136</v>
       </c>
       <c r="M105" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="R105" s="14" t="s">
         <v>157</v>
-      </c>
-      <c r="R105" s="14" t="s">
-        <v>158</v>
       </c>
       <c r="AE105" s="15" t="s">
         <v>120</v>
@@ -6881,13 +6889,13 @@
         <v>68</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C106" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E106" s="5" t="s">
         <v>70</v>
@@ -6899,7 +6907,7 @@
         <v>137</v>
       </c>
       <c r="H106" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I106" s="12">
         <v>3056</v>
@@ -6914,7 +6922,7 @@
         <v>136</v>
       </c>
       <c r="M106" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="R106" s="14" t="s">
         <v>144</v>
@@ -6928,13 +6936,13 @@
         <v>68</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C107" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D107" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E107" s="5" t="s">
         <v>70</v>
@@ -6946,7 +6954,7 @@
         <v>137</v>
       </c>
       <c r="H107" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I107" s="12">
         <v>3041</v>
@@ -6981,13 +6989,13 @@
         <v>68</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C108" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E108" s="5" t="s">
         <v>70</v>
@@ -6999,7 +7007,7 @@
         <v>137</v>
       </c>
       <c r="H108" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I108" s="12">
         <v>3041</v>
@@ -7034,13 +7042,13 @@
         <v>68</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C109" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D109" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E109" s="5" t="s">
         <v>70</v>
@@ -7052,7 +7060,7 @@
         <v>137</v>
       </c>
       <c r="H109" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I109" s="12">
         <v>3041</v>
@@ -7087,13 +7095,13 @@
         <v>68</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C110" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D110" s="6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E110" s="5" t="s">
         <v>70</v>
@@ -7105,7 +7113,7 @@
         <v>137</v>
       </c>
       <c r="H110" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I110" s="12">
         <v>3041</v>
@@ -7140,13 +7148,13 @@
         <v>68</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C111" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D111" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E111" s="5" t="s">
         <v>70</v>
@@ -7158,7 +7166,7 @@
         <v>137</v>
       </c>
       <c r="H111" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I111" s="12">
         <v>3041</v>
@@ -7196,13 +7204,13 @@
         <v>68</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C112" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D112" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E112" s="5" t="s">
         <v>70</v>
@@ -7214,7 +7222,7 @@
         <v>137</v>
       </c>
       <c r="H112" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I112" s="12">
         <v>3041</v>
@@ -7252,13 +7260,13 @@
         <v>68</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C113" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E113" s="5" t="s">
         <v>70</v>
@@ -7270,7 +7278,7 @@
         <v>137</v>
       </c>
       <c r="H113" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I113" s="12">
         <v>3041</v>
@@ -7302,13 +7310,13 @@
         <v>68</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C114" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D114" s="6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E114" s="5" t="s">
         <v>70</v>
@@ -7320,7 +7328,7 @@
         <v>137</v>
       </c>
       <c r="H114" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I114" s="12">
         <v>3041</v>
@@ -7352,13 +7360,13 @@
         <v>68</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C115" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D115" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E115" s="5" t="s">
         <v>70</v>
@@ -7370,7 +7378,7 @@
         <v>137</v>
       </c>
       <c r="H115" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I115" s="12">
         <v>3041</v>
@@ -7399,13 +7407,13 @@
         <v>68</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C116" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D116" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E116" s="5" t="s">
         <v>70</v>
@@ -7417,7 +7425,7 @@
         <v>137</v>
       </c>
       <c r="H116" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I116" s="12">
         <v>3041</v>
@@ -7452,13 +7460,13 @@
         <v>68</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C117" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D117" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E117" s="5" t="s">
         <v>70</v>
@@ -7470,7 +7478,7 @@
         <v>137</v>
       </c>
       <c r="H117" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I117" s="12">
         <v>3041</v>
@@ -7511,7 +7519,7 @@
         <v>69</v>
       </c>
       <c r="D118" s="6" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E118" s="5" t="s">
         <v>70</v>
@@ -7523,7 +7531,7 @@
         <v>122</v>
       </c>
       <c r="H118" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I118" s="12">
         <v>3067</v>
@@ -7535,7 +7543,7 @@
         <v>136</v>
       </c>
       <c r="M118" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AE118" s="10" t="s">
         <v>120</v>
@@ -7552,7 +7560,7 @@
         <v>69</v>
       </c>
       <c r="D119" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E119" s="5" t="s">
         <v>70</v>
@@ -7564,7 +7572,7 @@
         <v>3762</v>
       </c>
       <c r="H119" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I119" s="12">
         <v>3041</v>
@@ -7593,13 +7601,13 @@
         <v>68</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C120" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D120" s="6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E120" s="5" t="s">
         <v>70</v>
@@ -7611,36 +7619,40 @@
         <v>124</v>
       </c>
       <c r="H120" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I120" s="12">
         <v>3067</v>
       </c>
       <c r="K120" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L120" s="12" t="s">
         <v>136</v>
       </c>
       <c r="M120" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="AE120" s="10" t="s">
-        <v>136</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="N120" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="R120" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="AE120" s="13"/>
     </row>
     <row r="121" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C121" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D121" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E121" s="5" t="s">
         <v>70</v>
@@ -7652,7 +7664,7 @@
         <v>137</v>
       </c>
       <c r="H121" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I121" s="12">
         <v>3041</v>
@@ -7681,13 +7693,13 @@
         <v>68</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C122" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D122" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E122" s="5" t="s">
         <v>70</v>
@@ -7699,7 +7711,7 @@
         <v>137</v>
       </c>
       <c r="H122" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I122" s="12">
         <v>3041</v>
@@ -7734,7 +7746,7 @@
         <v>69</v>
       </c>
       <c r="D123" s="16" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E123" s="5" t="s">
         <v>70</v>
@@ -7746,7 +7758,7 @@
         <v>141</v>
       </c>
       <c r="H123" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I123" s="12">
         <v>3042</v>
@@ -7781,7 +7793,7 @@
         <v>69</v>
       </c>
       <c r="D124" s="16" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E124" s="5" t="s">
         <v>70</v>
@@ -7793,7 +7805,7 @@
         <v>141</v>
       </c>
       <c r="H124" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I124" s="12">
         <v>3042</v>
@@ -7831,7 +7843,7 @@
         <v>69</v>
       </c>
       <c r="D125" s="6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E125" s="5" t="s">
         <v>70</v>
@@ -7843,7 +7855,7 @@
         <v>141</v>
       </c>
       <c r="H125" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I125" s="12">
         <v>3070</v>
@@ -7858,7 +7870,7 @@
         <v>136</v>
       </c>
       <c r="M125" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="W125" s="17" t="s">
         <v>132</v>
@@ -7878,7 +7890,7 @@
         <v>69</v>
       </c>
       <c r="D126" s="6" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E126" s="5" t="s">
         <v>70</v>
@@ -7890,7 +7902,7 @@
         <v>141</v>
       </c>
       <c r="H126" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I126" s="12">
         <v>3070</v>
@@ -7905,7 +7917,7 @@
         <v>136</v>
       </c>
       <c r="M126" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="W126" s="11" t="s">
         <v>120</v>
@@ -7928,7 +7940,7 @@
         <v>69</v>
       </c>
       <c r="D127" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E127" s="5" t="s">
         <v>70</v>
@@ -7940,7 +7952,7 @@
         <v>3000</v>
       </c>
       <c r="H127" s="13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I127" s="13">
         <v>3046</v>
@@ -7952,7 +7964,7 @@
         <v>136</v>
       </c>
       <c r="M127" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AC127" s="15" t="s">
         <v>120</v>
@@ -7963,13 +7975,13 @@
         <v>68</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C128" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D128" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E128" s="5" t="s">
         <v>70</v>
@@ -7981,7 +7993,7 @@
         <v>137</v>
       </c>
       <c r="H128" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I128" s="12">
         <v>3046</v>
@@ -7996,7 +8008,7 @@
         <v>136</v>
       </c>
       <c r="M128" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N128" s="10" t="s">
         <v>128</v>
@@ -8016,13 +8028,13 @@
         <v>68</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C129" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D129" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E129" s="5" t="s">
         <v>70</v>
@@ -8034,7 +8046,7 @@
         <v>137</v>
       </c>
       <c r="H129" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I129" s="12">
         <v>3046</v>
@@ -8049,7 +8061,7 @@
         <v>136</v>
       </c>
       <c r="M129" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N129" s="10" t="s">
         <v>128</v>
@@ -8069,13 +8081,13 @@
         <v>68</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C130" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D130" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E130" s="5" t="s">
         <v>70</v>
@@ -8087,7 +8099,7 @@
         <v>137</v>
       </c>
       <c r="H130" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I130" s="12">
         <v>3046</v>
@@ -8102,7 +8114,7 @@
         <v>136</v>
       </c>
       <c r="M130" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Z130" s="15" t="s">
         <v>132</v>
@@ -8119,13 +8131,13 @@
         <v>68</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C131" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D131" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E131" s="5" t="s">
         <v>70</v>
@@ -8137,7 +8149,7 @@
         <v>137</v>
       </c>
       <c r="H131" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I131" s="12">
         <v>3046</v>
@@ -8152,7 +8164,7 @@
         <v>136</v>
       </c>
       <c r="M131" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Z131" s="15" t="s">
         <v>132</v>
@@ -8169,13 +8181,13 @@
         <v>68</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C132" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D132" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E132" s="5" t="s">
         <v>70</v>
@@ -8187,7 +8199,7 @@
         <v>137</v>
       </c>
       <c r="H132" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I132" s="12">
         <v>3046</v>
@@ -8202,7 +8214,7 @@
         <v>136</v>
       </c>
       <c r="M132" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Z132" s="15" t="s">
         <v>120</v>
@@ -8219,13 +8231,13 @@
         <v>68</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C133" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D133" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E133" s="5" t="s">
         <v>70</v>
@@ -8237,7 +8249,7 @@
         <v>137</v>
       </c>
       <c r="H133" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I133" s="12">
         <v>3046</v>
@@ -8252,7 +8264,7 @@
         <v>136</v>
       </c>
       <c r="M133" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Z133" s="15" t="s">
         <v>120</v>
@@ -8269,13 +8281,13 @@
         <v>68</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C134" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D134" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E134" s="5" t="s">
         <v>70</v>
@@ -8287,7 +8299,7 @@
         <v>137</v>
       </c>
       <c r="H134" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I134" s="12">
         <v>3046</v>
@@ -8302,7 +8314,7 @@
         <v>136</v>
       </c>
       <c r="M134" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AB134" s="15">
         <v>4</v>
@@ -8316,13 +8328,13 @@
         <v>68</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C135" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D135" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E135" s="5" t="s">
         <v>70</v>
@@ -8334,7 +8346,7 @@
         <v>137</v>
       </c>
       <c r="H135" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I135" s="12">
         <v>3046</v>
@@ -8349,10 +8361,10 @@
         <v>136</v>
       </c>
       <c r="M135" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q135" s="14" t="s">
         <v>167</v>
-      </c>
-      <c r="Q135" s="14" t="s">
-        <v>168</v>
       </c>
       <c r="Z135" s="15" t="s">
         <v>132</v>
@@ -8369,13 +8381,13 @@
         <v>68</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C136" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D136" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E136" s="5" t="s">
         <v>70</v>
@@ -8387,7 +8399,7 @@
         <v>137</v>
       </c>
       <c r="H136" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I136" s="12">
         <v>3046</v>
@@ -8402,10 +8414,10 @@
         <v>136</v>
       </c>
       <c r="M136" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q136" s="14" t="s">
         <v>167</v>
-      </c>
-      <c r="Q136" s="14" t="s">
-        <v>168</v>
       </c>
       <c r="Z136" s="15" t="s">
         <v>132</v>
@@ -8422,13 +8434,13 @@
         <v>68</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C137" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D137" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E137" s="5" t="s">
         <v>70</v>
@@ -8440,7 +8452,7 @@
         <v>137</v>
       </c>
       <c r="H137" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I137" s="12">
         <v>3046</v>
@@ -8455,7 +8467,7 @@
         <v>136</v>
       </c>
       <c r="M137" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="V137" s="15" t="s">
         <v>120</v>
@@ -8472,13 +8484,13 @@
         <v>68</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C138" s="9" t="s">
         <v>69</v>
       </c>
       <c r="D138" s="6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E138" s="5" t="s">
         <v>70</v>
@@ -8490,7 +8502,7 @@
         <v>137</v>
       </c>
       <c r="H138" s="13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I138" s="13">
         <v>3046</v>
@@ -8505,7 +8517,7 @@
         <v>136</v>
       </c>
       <c r="M138" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N138" s="13"/>
       <c r="O138" s="13"/>
@@ -8543,7 +8555,7 @@
         <v>69</v>
       </c>
       <c r="D139" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E139" s="5" t="s">
         <v>70</v>
@@ -8555,7 +8567,7 @@
         <v>141</v>
       </c>
       <c r="H139" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I139" s="12">
         <v>3071</v>
@@ -8584,7 +8596,7 @@
         <v>69</v>
       </c>
       <c r="D140" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E140" s="5" t="s">
         <v>70</v>
@@ -8596,7 +8608,7 @@
         <v>122</v>
       </c>
       <c r="H140" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I140" s="12">
         <v>3091</v>
@@ -8608,7 +8620,7 @@
         <v>136</v>
       </c>
       <c r="M140" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AE140" s="15" t="s">
         <v>120</v>
@@ -8619,13 +8631,13 @@
         <v>68</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C141" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D141" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E141" s="5" t="s">
         <v>70</v>
@@ -8634,10 +8646,10 @@
         <v>50</v>
       </c>
       <c r="G141" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H141" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I141" s="12">
         <v>3091</v>
@@ -8649,7 +8661,7 @@
         <v>132</v>
       </c>
       <c r="L141" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="AE141" s="15" t="s">
         <v>120</v>
@@ -8660,13 +8672,13 @@
         <v>68</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C142" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D142" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E142" s="5" t="s">
         <v>70</v>
@@ -8675,10 +8687,10 @@
         <v>51</v>
       </c>
       <c r="G142" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H142" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I142" s="12">
         <v>3091</v>
@@ -8690,7 +8702,7 @@
         <v>132</v>
       </c>
       <c r="L142" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="AE142" s="15" t="s">
         <v>120</v>
@@ -8701,13 +8713,13 @@
         <v>68</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C143" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D143" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E143" s="5" t="s">
         <v>70</v>
@@ -8716,10 +8728,10 @@
         <v>52</v>
       </c>
       <c r="G143" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H143" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I143" s="12">
         <v>3091</v>
@@ -8731,7 +8743,7 @@
         <v>132</v>
       </c>
       <c r="L143" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="AE143" s="15" t="s">
         <v>120</v>
@@ -8742,13 +8754,13 @@
         <v>68</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C144" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D144" s="4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E144" s="5" t="s">
         <v>70</v>
@@ -8757,10 +8769,10 @@
         <v>53</v>
       </c>
       <c r="G144" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H144" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I144" s="12">
         <v>3091</v>
@@ -8772,7 +8784,7 @@
         <v>132</v>
       </c>
       <c r="L144" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="AE144" s="15" t="s">
         <v>120</v>
@@ -8783,13 +8795,13 @@
         <v>68</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C145" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D145" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E145" s="5" t="s">
         <v>70</v>
@@ -8798,10 +8810,10 @@
         <v>54</v>
       </c>
       <c r="G145" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H145" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I145" s="12">
         <v>3091</v>
@@ -8810,10 +8822,10 @@
         <v>4</v>
       </c>
       <c r="K145" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L145" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="AE145" s="15" t="s">
         <v>120</v>
@@ -8824,13 +8836,13 @@
         <v>68</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C146" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D146" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E146" s="5" t="s">
         <v>70</v>
@@ -8839,10 +8851,10 @@
         <v>55</v>
       </c>
       <c r="G146" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H146" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I146" s="12">
         <v>3091</v>
@@ -8851,10 +8863,10 @@
         <v>4</v>
       </c>
       <c r="K146" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L146" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="AE146" s="15" t="s">
         <v>120</v>
@@ -8865,13 +8877,13 @@
         <v>68</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C147" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D147" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E147" s="5" t="s">
         <v>70</v>
@@ -8880,10 +8892,10 @@
         <v>56</v>
       </c>
       <c r="G147" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H147" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I147" s="12">
         <v>3091</v>
@@ -8892,10 +8904,10 @@
         <v>4</v>
       </c>
       <c r="K147" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L147" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="AE147" s="15" t="s">
         <v>120</v>
@@ -8906,13 +8918,13 @@
         <v>68</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C148" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D148" s="4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E148" s="5" t="s">
         <v>70</v>
@@ -8921,10 +8933,10 @@
         <v>57</v>
       </c>
       <c r="G148" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H148" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I148" s="12">
         <v>3091</v>
@@ -8933,10 +8945,10 @@
         <v>4</v>
       </c>
       <c r="K148" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L148" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="AE148" s="15" t="s">
         <v>120</v>
@@ -8947,13 +8959,13 @@
         <v>68</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C149" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D149" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E149" s="5" t="s">
         <v>70</v>
@@ -8962,10 +8974,10 @@
         <v>58</v>
       </c>
       <c r="G149" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H149" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I149" s="12">
         <v>3091</v>
@@ -8974,10 +8986,10 @@
         <v>4</v>
       </c>
       <c r="K149" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L149" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="AE149" s="15" t="s">
         <v>120</v>
@@ -8988,13 +9000,13 @@
         <v>68</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C150" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D150" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E150" s="5" t="s">
         <v>70</v>
@@ -9003,10 +9015,10 @@
         <v>59</v>
       </c>
       <c r="G150" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H150" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I150" s="12">
         <v>3091</v>
@@ -9015,10 +9027,10 @@
         <v>4</v>
       </c>
       <c r="K150" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L150" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="AE150" s="15" t="s">
         <v>120</v>
@@ -9029,13 +9041,13 @@
         <v>68</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C151" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D151" s="16" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E151" s="5" t="s">
         <v>70</v>
@@ -9044,10 +9056,10 @@
         <v>60</v>
       </c>
       <c r="G151" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H151" s="12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I151" s="12">
         <v>3097</v>
@@ -9056,7 +9068,7 @@
         <v>132</v>
       </c>
       <c r="L151" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="152" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -9064,13 +9076,13 @@
         <v>68</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C152" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D152" s="6" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E152" s="5" t="s">
         <v>70</v>
@@ -9079,10 +9091,10 @@
         <v>62</v>
       </c>
       <c r="G152" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="H152" s="12" t="s">
         <v>305</v>
-      </c>
-      <c r="H152" s="12" t="s">
-        <v>306</v>
       </c>
       <c r="I152" s="12">
         <v>3097</v>
@@ -9091,10 +9103,10 @@
         <v>2</v>
       </c>
       <c r="K152" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L152" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="153" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -9102,13 +9114,13 @@
         <v>68</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C153" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D153" s="6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E153" s="5" t="s">
         <v>70</v>
@@ -9117,10 +9129,10 @@
         <v>63</v>
       </c>
       <c r="G153" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="H153" s="12" t="s">
         <v>305</v>
-      </c>
-      <c r="H153" s="12" t="s">
-        <v>306</v>
       </c>
       <c r="I153" s="12">
         <v>3097</v>
@@ -9129,10 +9141,10 @@
         <v>2</v>
       </c>
       <c r="K153" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L153" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="154" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -9140,13 +9152,13 @@
         <v>68</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C154" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D154" s="6" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E154" s="5" t="s">
         <v>70</v>
@@ -9155,10 +9167,10 @@
         <v>64</v>
       </c>
       <c r="G154" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="H154" s="12" t="s">
         <v>305</v>
-      </c>
-      <c r="H154" s="12" t="s">
-        <v>306</v>
       </c>
       <c r="I154" s="12">
         <v>3097</v>
@@ -9167,10 +9179,10 @@
         <v>2</v>
       </c>
       <c r="K154" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L154" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="155" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -9178,13 +9190,13 @@
         <v>68</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C155" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D155" s="6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E155" s="5" t="s">
         <v>70</v>
@@ -9193,10 +9205,10 @@
         <v>65</v>
       </c>
       <c r="G155" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="H155" s="12" t="s">
         <v>305</v>
-      </c>
-      <c r="H155" s="12" t="s">
-        <v>306</v>
       </c>
       <c r="I155" s="12">
         <v>3097</v>
@@ -9205,10 +9217,10 @@
         <v>2</v>
       </c>
       <c r="K155" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L155" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="156" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -9216,13 +9228,13 @@
         <v>68</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C156" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D156" s="6" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E156" s="5" t="s">
         <v>70</v>
@@ -9231,10 +9243,10 @@
         <v>66</v>
       </c>
       <c r="G156" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="H156" s="12" t="s">
         <v>305</v>
-      </c>
-      <c r="H156" s="12" t="s">
-        <v>306</v>
       </c>
       <c r="I156" s="12">
         <v>3097</v>
@@ -9243,10 +9255,10 @@
         <v>2</v>
       </c>
       <c r="K156" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L156" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="157" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -9254,13 +9266,13 @@
         <v>68</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C157" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D157" s="6" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E157" s="5" t="s">
         <v>70</v>
@@ -9269,10 +9281,10 @@
         <v>67</v>
       </c>
       <c r="G157" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="H157" s="12" t="s">
         <v>305</v>
-      </c>
-      <c r="H157" s="12" t="s">
-        <v>306</v>
       </c>
       <c r="I157" s="12">
         <v>3097</v>
@@ -9281,10 +9293,10 @@
         <v>2</v>
       </c>
       <c r="K157" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L157" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="158" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -9292,13 +9304,13 @@
         <v>68</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C158" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D158" s="16" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E158" s="5" t="s">
         <v>70</v>
@@ -9307,10 +9319,10 @@
         <v>61</v>
       </c>
       <c r="G158" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H158" s="12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I158" s="12">
         <v>3097</v>
@@ -9319,7 +9331,7 @@
         <v>132</v>
       </c>
       <c r="L158" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="159" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -9333,7 +9345,7 @@
         <v>69</v>
       </c>
       <c r="D159" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E159" s="5" t="s">
         <v>70</v>
@@ -9345,7 +9357,7 @@
         <v>122</v>
       </c>
       <c r="H159" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I159" s="12">
         <v>3099</v>
@@ -9368,13 +9380,13 @@
         <v>68</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C160" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D160" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E160" s="5" t="s">
         <v>70</v>
@@ -9383,10 +9395,10 @@
         <v>50</v>
       </c>
       <c r="G160" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H160" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I160" s="12">
         <v>3099</v>
@@ -9395,7 +9407,7 @@
         <v>132</v>
       </c>
       <c r="L160" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M160" s="14" t="s">
         <v>146</v>
@@ -9409,13 +9421,13 @@
         <v>68</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C161" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D161" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E161" s="5" t="s">
         <v>70</v>
@@ -9424,10 +9436,10 @@
         <v>51</v>
       </c>
       <c r="G161" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H161" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I161" s="12">
         <v>3099</v>
@@ -9436,7 +9448,7 @@
         <v>132</v>
       </c>
       <c r="L161" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M161" s="14" t="s">
         <v>146</v>
@@ -9450,13 +9462,13 @@
         <v>68</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C162" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D162" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E162" s="5" t="s">
         <v>70</v>
@@ -9465,10 +9477,10 @@
         <v>54</v>
       </c>
       <c r="G162" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H162" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I162" s="12">
         <v>3099</v>
@@ -9477,10 +9489,10 @@
         <v>2</v>
       </c>
       <c r="K162" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L162" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M162" s="14" t="s">
         <v>146</v>
@@ -9494,13 +9506,13 @@
         <v>68</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C163" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D163" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E163" s="5" t="s">
         <v>70</v>
@@ -9509,10 +9521,10 @@
         <v>55</v>
       </c>
       <c r="G163" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H163" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I163" s="12">
         <v>3099</v>
@@ -9521,10 +9533,10 @@
         <v>2</v>
       </c>
       <c r="K163" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L163" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M163" s="14" t="s">
         <v>146</v>
@@ -9544,7 +9556,7 @@
         <v>69</v>
       </c>
       <c r="D164" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E164" s="5" t="s">
         <v>70</v>
@@ -9556,7 +9568,7 @@
         <v>122</v>
       </c>
       <c r="H164" s="12" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="I164" s="12">
         <v>3101</v>
@@ -9571,7 +9583,7 @@
         <v>136</v>
       </c>
       <c r="M164" s="14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AE164" s="15" t="s">
         <v>120</v>
@@ -9582,13 +9594,13 @@
         <v>68</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C165" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D165" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E165" s="5" t="s">
         <v>70</v>
@@ -9597,10 +9609,10 @@
         <v>50</v>
       </c>
       <c r="G165" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H165" s="12" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="I165" s="12">
         <v>3101</v>
@@ -9610,10 +9622,10 @@
         <v>132</v>
       </c>
       <c r="L165" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M165" s="14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="N165" s="12"/>
       <c r="O165" s="12"/>
@@ -9641,13 +9653,13 @@
         <v>68</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C166" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D166" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E166" s="5" t="s">
         <v>70</v>
@@ -9656,10 +9668,10 @@
         <v>51</v>
       </c>
       <c r="G166" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H166" s="19" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="I166" s="12">
         <v>3101</v>
@@ -9669,10 +9681,10 @@
         <v>132</v>
       </c>
       <c r="L166" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M166" s="14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="N166" s="12"/>
       <c r="O166" s="12"/>
@@ -9700,13 +9712,13 @@
         <v>68</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C167" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D167" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E167" s="5" t="s">
         <v>70</v>
@@ -9715,10 +9727,10 @@
         <v>54</v>
       </c>
       <c r="G167" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H167" s="12" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="I167" s="12">
         <v>3101</v>
@@ -9727,13 +9739,13 @@
         <v>3</v>
       </c>
       <c r="K167" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L167" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M167" s="14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AE167" s="15" t="s">
         <v>120</v>
@@ -9744,13 +9756,13 @@
         <v>68</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C168" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D168" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E168" s="5" t="s">
         <v>70</v>
@@ -9759,10 +9771,10 @@
         <v>55</v>
       </c>
       <c r="G168" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H168" s="12" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="I168" s="12">
         <v>3101</v>
@@ -9771,13 +9783,13 @@
         <v>3</v>
       </c>
       <c r="K168" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L168" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M168" s="14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AE168" s="15" t="s">
         <v>120</v>
@@ -9794,7 +9806,7 @@
         <v>69</v>
       </c>
       <c r="D169" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E169" s="5" t="s">
         <v>70</v>
@@ -9806,7 +9818,7 @@
         <v>3762</v>
       </c>
       <c r="H169" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I169" s="12">
         <v>3067</v>
@@ -9821,7 +9833,7 @@
         <v>136</v>
       </c>
       <c r="M169" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="R169" s="10" t="s">
         <v>123</v>
@@ -9835,13 +9847,13 @@
         <v>68</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C170" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D170" s="6" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E170" s="5" t="s">
         <v>70</v>
@@ -9853,7 +9865,7 @@
         <v>137</v>
       </c>
       <c r="H170" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I170" s="12">
         <v>3067</v>
@@ -9868,10 +9880,10 @@
         <v>136</v>
       </c>
       <c r="M170" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="R170" s="10" t="s">
         <v>157</v>
-      </c>
-      <c r="R170" s="10" t="s">
-        <v>158</v>
       </c>
       <c r="AE170" s="10" t="s">
         <v>120</v>
@@ -9882,13 +9894,13 @@
         <v>68</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C171" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D171" s="6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E171" s="5" t="s">
         <v>70</v>
@@ -9900,7 +9912,7 @@
         <v>137</v>
       </c>
       <c r="H171" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I171" s="12">
         <v>3067</v>
@@ -9915,7 +9927,7 @@
         <v>136</v>
       </c>
       <c r="M171" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="R171" s="10" t="s">
         <v>139</v>

</xml_diff>

<commit_message>
Dla tekstu T1_104 w kol "J" (Nr kolejny) ustawiłem wart = 2
http://gitlab/zus-developers/ue_efta/issues/158 uwaga M.Lipiec:  "Ustawa z 5 marca w podstwie prawnej powinna być zaprezentowana jako druga. Pierwsza powinna być ustawa o FUS." Dla tekstu T1_104 należy wprowadzić nr kolejny = 2, a dla tekstu T1_25 nr kolejny = 1
</commit_message>
<xml_diff>
--- a/UEFTA_Teksty.xlsx
+++ b/UEFTA_Teksty.xlsx
@@ -1647,11 +1647,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AE173"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q120" sqref="Q120"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J173" sqref="J173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1802,6 +1803,9 @@
       <c r="I2" s="12">
         <v>3001</v>
       </c>
+      <c r="J2" s="12">
+        <v>2</v>
+      </c>
       <c r="K2" s="12" t="s">
         <v>132</v>
       </c>
@@ -1819,7 +1823,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>68</v>
       </c>
@@ -1866,7 +1870,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>68</v>
       </c>
@@ -1907,7 +1911,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>68</v>
       </c>
@@ -1960,7 +1964,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>68</v>
       </c>
@@ -2027,7 +2031,7 @@
       </c>
       <c r="AE6" s="13"/>
     </row>
-    <row r="7" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>68</v>
       </c>
@@ -2073,7 +2077,7 @@
       <c r="S7" s="13"/>
       <c r="AE7" s="13"/>
     </row>
-    <row r="8" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>68</v>
       </c>
@@ -2117,7 +2121,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>68</v>
       </c>
@@ -2161,7 +2165,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>68</v>
       </c>
@@ -2217,7 +2221,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>68</v>
       </c>
@@ -2275,7 +2279,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>68</v>
       </c>
@@ -2326,7 +2330,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="13" spans="1:31" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" ht="49.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>68</v>
       </c>
@@ -2384,7 +2388,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:31" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" ht="58.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>68</v>
       </c>
@@ -2445,7 +2449,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:31" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" ht="70.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>68</v>
       </c>
@@ -2503,7 +2507,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="16" spans="1:31" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>68</v>
       </c>
@@ -2554,7 +2558,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="17" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>68</v>
       </c>
@@ -2605,7 +2609,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>68</v>
       </c>
@@ -2652,7 +2656,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="19" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>68</v>
       </c>
@@ -2705,7 +2709,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="20" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>68</v>
       </c>
@@ -2758,7 +2762,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="21" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>68</v>
       </c>
@@ -2821,7 +2825,7 @@
       <c r="AD21" s="13"/>
       <c r="AE21" s="13"/>
     </row>
-    <row r="22" spans="1:31" s="13" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31" s="13" customFormat="1" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>68</v>
       </c>
@@ -2884,7 +2888,7 @@
       <c r="AD22" s="12"/>
       <c r="AE22" s="12"/>
     </row>
-    <row r="23" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>68</v>
       </c>
@@ -2962,6 +2966,9 @@
       <c r="I24" s="12">
         <v>3049</v>
       </c>
+      <c r="J24" s="12">
+        <v>2</v>
+      </c>
       <c r="K24" s="12" t="s">
         <v>132</v>
       </c>
@@ -2975,7 +2982,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>68</v>
       </c>
@@ -3036,7 +3043,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="26" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>68</v>
       </c>
@@ -3081,7 +3088,7 @@
       </c>
       <c r="AE26" s="13"/>
     </row>
-    <row r="27" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>68</v>
       </c>
@@ -3129,7 +3136,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="28" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>68</v>
       </c>
@@ -3205,6 +3212,9 @@
       <c r="I29" s="12">
         <v>3068</v>
       </c>
+      <c r="J29" s="12">
+        <v>2</v>
+      </c>
       <c r="K29" s="12" t="s">
         <v>132</v>
       </c>
@@ -3218,7 +3228,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="30" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>68</v>
       </c>
@@ -3279,7 +3289,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="31" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>68</v>
       </c>
@@ -3324,7 +3334,7 @@
       </c>
       <c r="AE31" s="13"/>
     </row>
-    <row r="32" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>68</v>
       </c>
@@ -3369,7 +3379,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="33" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>68</v>
       </c>
@@ -3442,6 +3452,9 @@
       <c r="I34" s="12">
         <v>3003</v>
       </c>
+      <c r="J34" s="12">
+        <v>2</v>
+      </c>
       <c r="K34" s="12" t="s">
         <v>132</v>
       </c>
@@ -3458,7 +3471,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="35" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>68</v>
       </c>
@@ -3503,7 +3516,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="36" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>68</v>
       </c>
@@ -3548,7 +3561,7 @@
       </c>
       <c r="AE36" s="13"/>
     </row>
-    <row r="37" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>68</v>
       </c>
@@ -3593,7 +3606,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="38" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>68</v>
       </c>
@@ -3637,7 +3650,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="39" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>68</v>
       </c>
@@ -3690,7 +3703,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="40" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>68</v>
       </c>
@@ -3743,7 +3756,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="41" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>68</v>
       </c>
@@ -3796,7 +3809,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="42" spans="1:31" s="13" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:31" s="13" customFormat="1" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>68</v>
       </c>
@@ -3863,7 +3876,7 @@
       <c r="AD42" s="12"/>
       <c r="AE42" s="12"/>
     </row>
-    <row r="43" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>68</v>
       </c>
@@ -3919,7 +3932,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="44" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>68</v>
       </c>
@@ -3975,7 +3988,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="45" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>68</v>
       </c>
@@ -4025,7 +4038,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="46" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>68</v>
       </c>
@@ -4075,7 +4088,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="47" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>68</v>
       </c>
@@ -4122,7 +4135,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="48" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>68</v>
       </c>
@@ -4175,7 +4188,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="49" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>68</v>
       </c>
@@ -4256,6 +4269,9 @@
       <c r="I50" s="12">
         <v>3056</v>
       </c>
+      <c r="J50" s="12">
+        <v>2</v>
+      </c>
       <c r="K50" s="12" t="s">
         <v>132</v>
       </c>
@@ -4269,7 +4285,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="51" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>68</v>
       </c>
@@ -4316,7 +4332,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="52" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>68</v>
       </c>
@@ -4361,7 +4377,7 @@
       </c>
       <c r="AE52" s="13"/>
     </row>
-    <row r="53" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>68</v>
       </c>
@@ -4408,7 +4424,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="54" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>68</v>
       </c>
@@ -4455,7 +4471,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="55" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>68</v>
       </c>
@@ -4502,7 +4518,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="56" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>68</v>
       </c>
@@ -4580,6 +4596,9 @@
       <c r="I57" s="12">
         <v>3058</v>
       </c>
+      <c r="J57" s="12">
+        <v>2</v>
+      </c>
       <c r="K57" s="12" t="s">
         <v>132</v>
       </c>
@@ -4593,7 +4612,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="58" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>68</v>
       </c>
@@ -4640,7 +4659,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="59" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>68</v>
       </c>
@@ -4687,7 +4706,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="60" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>68</v>
       </c>
@@ -4734,7 +4753,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="61" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>68</v>
       </c>
@@ -4781,7 +4800,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="62" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>68</v>
       </c>
@@ -4828,7 +4847,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="63" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>68</v>
       </c>
@@ -4906,6 +4925,9 @@
       <c r="I64" s="12">
         <v>3072</v>
       </c>
+      <c r="J64" s="12">
+        <v>2</v>
+      </c>
       <c r="K64" s="12" t="s">
         <v>132</v>
       </c>
@@ -4916,7 +4938,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="65" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>68</v>
       </c>
@@ -4983,6 +5005,9 @@
       <c r="I66" s="12">
         <v>3023</v>
       </c>
+      <c r="J66" s="12">
+        <v>2</v>
+      </c>
       <c r="K66" s="12" t="s">
         <v>132</v>
       </c>
@@ -4999,7 +5024,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="67" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>68</v>
       </c>
@@ -5043,7 +5068,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="68" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>68</v>
       </c>
@@ -5084,7 +5109,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="69" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>68</v>
       </c>
@@ -5125,7 +5150,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="70" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>68</v>
       </c>
@@ -5172,7 +5197,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="71" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>68</v>
       </c>
@@ -5219,7 +5244,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="72" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>68</v>
       </c>
@@ -5269,7 +5294,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="73" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>68</v>
       </c>
@@ -5316,7 +5341,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="74" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>68</v>
       </c>
@@ -5363,7 +5388,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="75" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>68</v>
       </c>
@@ -5410,7 +5435,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="76" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>68</v>
       </c>
@@ -5457,7 +5482,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="77" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>68</v>
       </c>
@@ -5507,7 +5532,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="78" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>68</v>
       </c>
@@ -5557,7 +5582,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="79" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>68</v>
       </c>
@@ -5607,7 +5632,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="80" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>68</v>
       </c>
@@ -5657,7 +5682,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="81" spans="1:29" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:29" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>68</v>
       </c>
@@ -5704,7 +5729,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="82" spans="1:29" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:29" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>68</v>
       </c>
@@ -5757,7 +5782,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="83" spans="1:29" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:29" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>68</v>
       </c>
@@ -5810,7 +5835,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="84" spans="1:29" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:29" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>68</v>
       </c>
@@ -5863,7 +5888,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="85" spans="1:29" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:29" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>68</v>
       </c>
@@ -5916,7 +5941,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="86" spans="1:29" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:29" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>68</v>
       </c>
@@ -5966,7 +5991,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="87" spans="1:29" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:29" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>68</v>
       </c>
@@ -6016,7 +6041,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="88" spans="1:29" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:29" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>68</v>
       </c>
@@ -6094,6 +6119,9 @@
       <c r="I89" s="12">
         <v>3042</v>
       </c>
+      <c r="J89" s="12">
+        <v>2</v>
+      </c>
       <c r="K89" s="12" t="s">
         <v>132</v>
       </c>
@@ -6107,7 +6135,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="90" spans="1:29" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:29" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>68</v>
       </c>
@@ -6160,7 +6188,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="91" spans="1:29" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:29" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>68</v>
       </c>
@@ -6213,7 +6241,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="92" spans="1:29" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:29" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>68</v>
       </c>
@@ -6263,7 +6291,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="93" spans="1:29" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:29" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>68</v>
       </c>
@@ -6313,7 +6341,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="94" spans="1:29" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:29" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>68</v>
       </c>
@@ -6363,7 +6391,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="95" spans="1:29" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:29" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>68</v>
       </c>
@@ -6413,7 +6441,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="96" spans="1:29" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:29" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>68</v>
       </c>
@@ -6460,7 +6488,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="97" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>68</v>
       </c>
@@ -6513,7 +6541,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="98" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>68</v>
       </c>
@@ -6566,7 +6594,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="99" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
         <v>68</v>
       </c>
@@ -6616,7 +6644,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="100" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>68</v>
       </c>
@@ -6666,7 +6694,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="101" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>68</v>
       </c>
@@ -6735,6 +6763,9 @@
       <c r="I102" s="12">
         <v>3041</v>
       </c>
+      <c r="J102" s="12">
+        <v>2</v>
+      </c>
       <c r="K102" s="12" t="s">
         <v>132</v>
       </c>
@@ -6748,7 +6779,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="103" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
         <v>68</v>
       </c>
@@ -6792,7 +6823,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="104" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>68</v>
       </c>
@@ -6837,7 +6868,7 @@
       </c>
       <c r="AE104" s="13"/>
     </row>
-    <row r="105" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
         <v>68</v>
       </c>
@@ -6884,7 +6915,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="106" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
         <v>68</v>
       </c>
@@ -6931,7 +6962,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="107" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
         <v>68</v>
       </c>
@@ -6984,7 +7015,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="108" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
         <v>68</v>
       </c>
@@ -7037,7 +7068,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="109" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
         <v>68</v>
       </c>
@@ -7090,7 +7121,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="110" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
         <v>68</v>
       </c>
@@ -7143,7 +7174,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="111" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
         <v>68</v>
       </c>
@@ -7199,7 +7230,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="112" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
         <v>68</v>
       </c>
@@ -7255,7 +7286,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="113" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
         <v>68</v>
       </c>
@@ -7305,7 +7336,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="114" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
         <v>68</v>
       </c>
@@ -7355,7 +7386,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="115" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
         <v>68</v>
       </c>
@@ -7402,7 +7433,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="116" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
         <v>68</v>
       </c>
@@ -7455,7 +7486,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="117" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
         <v>68</v>
       </c>
@@ -7536,6 +7567,9 @@
       <c r="I118" s="12">
         <v>3067</v>
       </c>
+      <c r="J118" s="12">
+        <v>2</v>
+      </c>
       <c r="K118" s="12" t="s">
         <v>132</v>
       </c>
@@ -7549,7 +7583,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="119" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
         <v>68</v>
       </c>
@@ -7596,7 +7630,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="120" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
         <v>68</v>
       </c>
@@ -7641,7 +7675,7 @@
       </c>
       <c r="AE120" s="13"/>
     </row>
-    <row r="121" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
         <v>68</v>
       </c>
@@ -7688,7 +7722,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
         <v>68</v>
       </c>
@@ -7735,7 +7769,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="123" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
         <v>68</v>
       </c>
@@ -7782,7 +7816,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="124" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
         <v>68</v>
       </c>
@@ -7832,7 +7866,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="125" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
         <v>68</v>
       </c>
@@ -7879,7 +7913,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="126" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
         <v>68</v>
       </c>
@@ -7957,6 +7991,9 @@
       <c r="I127" s="13">
         <v>3046</v>
       </c>
+      <c r="J127" s="12">
+        <v>2</v>
+      </c>
       <c r="K127" s="12" t="s">
         <v>132</v>
       </c>
@@ -7970,7 +8007,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="128" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
         <v>68</v>
       </c>
@@ -8023,7 +8060,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="129" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
         <v>68</v>
       </c>
@@ -8076,7 +8113,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="130" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
         <v>68</v>
       </c>
@@ -8126,7 +8163,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="131" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
         <v>68</v>
       </c>
@@ -8176,7 +8213,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="132" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
         <v>68</v>
       </c>
@@ -8226,7 +8263,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="133" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
         <v>68</v>
       </c>
@@ -8276,7 +8313,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="134" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
         <v>68</v>
       </c>
@@ -8323,7 +8360,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="135" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
         <v>68</v>
       </c>
@@ -8376,7 +8413,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="136" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
         <v>68</v>
       </c>
@@ -8429,7 +8466,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="137" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
         <v>68</v>
       </c>
@@ -8479,7 +8516,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="138" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="9" t="s">
         <v>68</v>
       </c>
@@ -8544,7 +8581,7 @@
       <c r="AD138" s="13"/>
       <c r="AE138" s="13"/>
     </row>
-    <row r="139" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
         <v>68</v>
       </c>
@@ -8613,6 +8650,9 @@
       <c r="I140" s="12">
         <v>3091</v>
       </c>
+      <c r="J140" s="12">
+        <v>2</v>
+      </c>
       <c r="K140" s="12" t="s">
         <v>132</v>
       </c>
@@ -8626,7 +8666,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="141" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
         <v>68</v>
       </c>
@@ -8667,7 +8707,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="142" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
         <v>68</v>
       </c>
@@ -8708,7 +8748,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="143" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
         <v>68</v>
       </c>
@@ -8749,7 +8789,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="144" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
         <v>68</v>
       </c>
@@ -8790,7 +8830,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="145" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
         <v>68</v>
       </c>
@@ -8831,7 +8871,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="146" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
         <v>68</v>
       </c>
@@ -8872,7 +8912,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="147" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
         <v>68</v>
       </c>
@@ -8913,7 +8953,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="148" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
         <v>68</v>
       </c>
@@ -8954,7 +8994,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="149" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
         <v>68</v>
       </c>
@@ -8995,7 +9035,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="150" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
         <v>68</v>
       </c>
@@ -9036,7 +9076,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="151" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
         <v>68</v>
       </c>
@@ -9071,7 +9111,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="152" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="s">
         <v>68</v>
       </c>
@@ -9109,7 +9149,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="153" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
         <v>68</v>
       </c>
@@ -9147,7 +9187,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="154" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="s">
         <v>68</v>
       </c>
@@ -9185,7 +9225,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="155" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
         <v>68</v>
       </c>
@@ -9223,7 +9263,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="156" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
         <v>68</v>
       </c>
@@ -9261,7 +9301,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="157" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
         <v>68</v>
       </c>
@@ -9299,7 +9339,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="158" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
         <v>68</v>
       </c>
@@ -9363,7 +9403,7 @@
         <v>3099</v>
       </c>
       <c r="J159" s="12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K159" s="12" t="s">
         <v>132</v>
@@ -9375,7 +9415,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="160" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
         <v>68</v>
       </c>
@@ -9416,7 +9456,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="161" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
         <v>68</v>
       </c>
@@ -9457,7 +9497,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="162" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
         <v>68</v>
       </c>
@@ -9501,7 +9541,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="163" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
         <v>68</v>
       </c>
@@ -9574,7 +9614,7 @@
         <v>3101</v>
       </c>
       <c r="J164" s="12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K164" s="12" t="s">
         <v>132</v>
@@ -9589,7 +9629,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="165" spans="1:31" s="13" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:31" s="13" customFormat="1" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
         <v>68</v>
       </c>
@@ -9648,7 +9688,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="166" spans="1:31" s="13" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:31" s="13" customFormat="1" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
         <v>68</v>
       </c>
@@ -9707,7 +9747,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="167" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
         <v>68</v>
       </c>
@@ -9751,7 +9791,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="168" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
         <v>68</v>
       </c>
@@ -9795,7 +9835,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="169" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="3" t="s">
         <v>68</v>
       </c>
@@ -9842,7 +9882,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="170" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
         <v>68</v>
       </c>
@@ -9889,7 +9929,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="171" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="3" t="s">
         <v>68</v>
       </c>
@@ -9940,7 +9980,13 @@
       <c r="D173" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AE171"/>
+  <autoFilter ref="A1:AE171">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="T1_104 - (Dz. U. z 2015 r. poz. 552)"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState columnSort="1" ref="K1:T168">
     <sortCondition ref="K1:T1"/>
   </sortState>

</xml_diff>

<commit_message>
Poprawka dotycząca defektu #199.
Poprawiłem literówkę dla Rp-31g (wcześniej było Rp-31-g - a nie ma takiego kodu pisma),
Wystąpienie w rekordzie dla STW_ID_TEKST = 13755.
</commit_message>
<xml_diff>
--- a/UEFTA_Teksty.xlsx
+++ b/UEFTA_Teksty.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2157" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2157" uniqueCount="386">
   <si>
     <t>Po ponownym ustaleniu wysokość &lt;NAZWASWIADCZENIAGL&gt; wynosi: 
 &lt;KWOTAKAPITALUPOCZATKOWEGOKOR&gt;/&lt;SREDNIEDALSZETRWANIEZYCIA&gt; = &lt;KWOTAEMERYTURYKOR&gt; zł.</t>
@@ -970,9 +970,6 @@
   </si>
   <si>
     <t>Rp-31g</t>
-  </si>
-  <si>
-    <t>Rp-31-g</t>
   </si>
   <si>
     <t>Rp-31i</t>
@@ -1651,8 +1648,8 @@
   <dimension ref="A1:AE173"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J173" sqref="J173"/>
+      <pane ySplit="1" topLeftCell="A141" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A158" sqref="A158:XFD158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1660,9 +1657,9 @@
     <col min="1" max="1" width="6.5703125" style="3" customWidth="1"/>
     <col min="2" max="2" width="15.42578125" style="3" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="27" style="3" customWidth="1"/>
+    <col min="4" max="4" width="44.7109375" style="3" customWidth="1"/>
     <col min="5" max="5" width="2" style="3" customWidth="1"/>
-    <col min="6" max="6" width="39.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="78.5703125" style="3" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" style="3" customWidth="1"/>
     <col min="8" max="8" width="11" style="12" customWidth="1"/>
     <col min="9" max="9" width="14.42578125" style="12" customWidth="1"/>
@@ -1712,7 +1709,7 @@
         <v>134</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>135</v>
@@ -1775,7 +1772,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="2" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>68</v>
       </c>
@@ -1786,7 +1783,7 @@
         <v>69</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>70</v>
@@ -1834,7 +1831,7 @@
         <v>69</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>70</v>
@@ -1843,7 +1840,7 @@
         <v>2</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>119</v>
@@ -1864,7 +1861,7 @@
         <v>127</v>
       </c>
       <c r="O3" s="14" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AE3" s="15" t="s">
         <v>120</v>
@@ -1881,7 +1878,7 @@
         <v>69</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>70</v>
@@ -1922,7 +1919,7 @@
         <v>69</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>70</v>
@@ -1975,7 +1972,7 @@
         <v>69</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>70</v>
@@ -2042,7 +2039,7 @@
         <v>69</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>70</v>
@@ -2060,7 +2057,7 @@
         <v>3001</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L7" s="12" t="s">
         <v>136</v>
@@ -2088,7 +2085,7 @@
         <v>69</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>70</v>
@@ -2132,7 +2129,7 @@
         <v>69</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>70</v>
@@ -2176,7 +2173,7 @@
         <v>69</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>70</v>
@@ -2232,7 +2229,7 @@
         <v>69</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>70</v>
@@ -2290,7 +2287,7 @@
         <v>69</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>70</v>
@@ -2341,7 +2338,7 @@
         <v>69</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>70</v>
@@ -2399,7 +2396,7 @@
         <v>69</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>70</v>
@@ -2460,7 +2457,7 @@
         <v>69</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>70</v>
@@ -2518,7 +2515,7 @@
         <v>69</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>70</v>
@@ -2569,7 +2566,7 @@
         <v>69</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>70</v>
@@ -2620,7 +2617,7 @@
         <v>69</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>70</v>
@@ -2667,7 +2664,7 @@
         <v>69</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>70</v>
@@ -2720,7 +2717,7 @@
         <v>69</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>70</v>
@@ -2773,7 +2770,7 @@
         <v>69</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>70</v>
@@ -2836,7 +2833,7 @@
         <v>69</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>70</v>
@@ -2899,7 +2896,7 @@
         <v>69</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>70</v>
@@ -2938,7 +2935,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>68</v>
       </c>
@@ -2949,7 +2946,7 @@
         <v>69</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>70</v>
@@ -2993,7 +2990,7 @@
         <v>69</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>70</v>
@@ -3054,7 +3051,7 @@
         <v>69</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>70</v>
@@ -3072,7 +3069,7 @@
         <v>3049</v>
       </c>
       <c r="K26" s="12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L26" s="12" t="s">
         <v>136</v>
@@ -3099,7 +3096,7 @@
         <v>69</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>70</v>
@@ -3147,7 +3144,7 @@
         <v>69</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>70</v>
@@ -3184,7 +3181,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="29" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>68</v>
       </c>
@@ -3195,7 +3192,7 @@
         <v>69</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>70</v>
@@ -3239,7 +3236,7 @@
         <v>69</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>70</v>
@@ -3300,7 +3297,7 @@
         <v>69</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>70</v>
@@ -3318,7 +3315,7 @@
         <v>3068</v>
       </c>
       <c r="K31" s="12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L31" s="12" t="s">
         <v>136</v>
@@ -3345,7 +3342,7 @@
         <v>69</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>70</v>
@@ -3390,7 +3387,7 @@
         <v>69</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>70</v>
@@ -3424,7 +3421,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="34" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>68</v>
       </c>
@@ -3435,7 +3432,7 @@
         <v>69</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>70</v>
@@ -3482,7 +3479,7 @@
         <v>69</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>70</v>
@@ -3527,7 +3524,7 @@
         <v>69</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>70</v>
@@ -3545,7 +3542,7 @@
         <v>3003</v>
       </c>
       <c r="K36" s="12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L36" s="12" t="s">
         <v>136</v>
@@ -3572,7 +3569,7 @@
         <v>69</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>70</v>
@@ -3617,7 +3614,7 @@
         <v>69</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>70</v>
@@ -3661,7 +3658,7 @@
         <v>69</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>70</v>
@@ -3714,7 +3711,7 @@
         <v>69</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>70</v>
@@ -3767,7 +3764,7 @@
         <v>69</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>70</v>
@@ -3820,7 +3817,7 @@
         <v>69</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>70</v>
@@ -3887,7 +3884,7 @@
         <v>69</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>70</v>
@@ -3943,7 +3940,7 @@
         <v>69</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>70</v>
@@ -3999,7 +3996,7 @@
         <v>69</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>70</v>
@@ -4049,7 +4046,7 @@
         <v>69</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>70</v>
@@ -4099,7 +4096,7 @@
         <v>69</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>70</v>
@@ -4146,7 +4143,7 @@
         <v>69</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E48" s="5" t="s">
         <v>70</v>
@@ -4199,7 +4196,7 @@
         <v>69</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E49" s="5" t="s">
         <v>70</v>
@@ -4241,7 +4238,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="50" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>68</v>
       </c>
@@ -4252,7 +4249,7 @@
         <v>69</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E50" s="5" t="s">
         <v>70</v>
@@ -4296,7 +4293,7 @@
         <v>69</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E51" s="5" t="s">
         <v>70</v>
@@ -4343,7 +4340,7 @@
         <v>69</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E52" s="5" t="s">
         <v>70</v>
@@ -4361,7 +4358,7 @@
         <v>3056</v>
       </c>
       <c r="K52" s="12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L52" s="12" t="s">
         <v>136</v>
@@ -4388,7 +4385,7 @@
         <v>69</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>70</v>
@@ -4435,7 +4432,7 @@
         <v>69</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E54" s="5" t="s">
         <v>70</v>
@@ -4482,7 +4479,7 @@
         <v>69</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E55" s="5" t="s">
         <v>70</v>
@@ -4529,7 +4526,7 @@
         <v>69</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E56" s="5" t="s">
         <v>70</v>
@@ -4568,7 +4565,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>68</v>
       </c>
@@ -4579,7 +4576,7 @@
         <v>69</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E57" s="5" t="s">
         <v>70</v>
@@ -4623,7 +4620,7 @@
         <v>69</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E58" s="5" t="s">
         <v>70</v>
@@ -4670,7 +4667,7 @@
         <v>69</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E59" s="5" t="s">
         <v>70</v>
@@ -4717,7 +4714,7 @@
         <v>69</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E60" s="5" t="s">
         <v>70</v>
@@ -4764,7 +4761,7 @@
         <v>69</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E61" s="5" t="s">
         <v>70</v>
@@ -4811,7 +4808,7 @@
         <v>69</v>
       </c>
       <c r="D62" s="16" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E62" s="5" t="s">
         <v>70</v>
@@ -4858,7 +4855,7 @@
         <v>69</v>
       </c>
       <c r="D63" s="16" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E63" s="5" t="s">
         <v>70</v>
@@ -4897,7 +4894,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>68</v>
       </c>
@@ -4908,7 +4905,7 @@
         <v>69</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E64" s="5" t="s">
         <v>70</v>
@@ -4949,7 +4946,7 @@
         <v>69</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E65" s="5" t="s">
         <v>70</v>
@@ -4967,7 +4964,7 @@
         <v>3072</v>
       </c>
       <c r="K65" s="12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="N65" s="12" t="s">
         <v>128</v>
@@ -4977,7 +4974,7 @@
       </c>
       <c r="AE65" s="13"/>
     </row>
-    <row r="66" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>68</v>
       </c>
@@ -4988,7 +4985,7 @@
         <v>69</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E66" s="5" t="s">
         <v>70</v>
@@ -5035,7 +5032,7 @@
         <v>69</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E67" s="5" t="s">
         <v>70</v>
@@ -5079,7 +5076,7 @@
         <v>69</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E68" s="5" t="s">
         <v>70</v>
@@ -5097,7 +5094,7 @@
         <v>3023</v>
       </c>
       <c r="K68" s="12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L68" s="12" t="s">
         <v>136</v>
@@ -5120,7 +5117,7 @@
         <v>69</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E69" s="5" t="s">
         <v>70</v>
@@ -5138,7 +5135,7 @@
         <v>3023</v>
       </c>
       <c r="K69" s="12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L69" s="12" t="s">
         <v>136</v>
@@ -5161,7 +5158,7 @@
         <v>69</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E70" s="5" t="s">
         <v>70</v>
@@ -5208,7 +5205,7 @@
         <v>69</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E71" s="5" t="s">
         <v>70</v>
@@ -5255,7 +5252,7 @@
         <v>69</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E72" s="5" t="s">
         <v>70</v>
@@ -5305,7 +5302,7 @@
         <v>69</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E73" s="5" t="s">
         <v>70</v>
@@ -5352,7 +5349,7 @@
         <v>69</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E74" s="5" t="s">
         <v>70</v>
@@ -5399,7 +5396,7 @@
         <v>69</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E75" s="5" t="s">
         <v>70</v>
@@ -5446,7 +5443,7 @@
         <v>69</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E76" s="5" t="s">
         <v>70</v>
@@ -5493,7 +5490,7 @@
         <v>69</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E77" s="5" t="s">
         <v>70</v>
@@ -5543,7 +5540,7 @@
         <v>69</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E78" s="5" t="s">
         <v>70</v>
@@ -5593,7 +5590,7 @@
         <v>69</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E79" s="5" t="s">
         <v>70</v>
@@ -5643,7 +5640,7 @@
         <v>69</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E80" s="5" t="s">
         <v>70</v>
@@ -5693,7 +5690,7 @@
         <v>69</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E81" s="5" t="s">
         <v>70</v>
@@ -5740,7 +5737,7 @@
         <v>69</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E82" s="5" t="s">
         <v>70</v>
@@ -5793,7 +5790,7 @@
         <v>69</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E83" s="5" t="s">
         <v>70</v>
@@ -5846,7 +5843,7 @@
         <v>69</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E84" s="5" t="s">
         <v>70</v>
@@ -5899,7 +5896,7 @@
         <v>69</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E85" s="5" t="s">
         <v>70</v>
@@ -5952,7 +5949,7 @@
         <v>69</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E86" s="5" t="s">
         <v>70</v>
@@ -5996,13 +5993,13 @@
         <v>68</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C87" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E87" s="5" t="s">
         <v>70</v>
@@ -6046,13 +6043,13 @@
         <v>68</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C88" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E88" s="5" t="s">
         <v>70</v>
@@ -6091,7 +6088,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="89" spans="1:29" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:29" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>68</v>
       </c>
@@ -6102,7 +6099,7 @@
         <v>69</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E89" s="5" t="s">
         <v>70</v>
@@ -6146,7 +6143,7 @@
         <v>69</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E90" s="5" t="s">
         <v>70</v>
@@ -6199,7 +6196,7 @@
         <v>69</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E91" s="5" t="s">
         <v>70</v>
@@ -6252,7 +6249,7 @@
         <v>69</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E92" s="5" t="s">
         <v>70</v>
@@ -6302,7 +6299,7 @@
         <v>69</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E93" s="5" t="s">
         <v>70</v>
@@ -6352,7 +6349,7 @@
         <v>69</v>
       </c>
       <c r="D94" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E94" s="5" t="s">
         <v>70</v>
@@ -6402,7 +6399,7 @@
         <v>69</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E95" s="5" t="s">
         <v>70</v>
@@ -6452,7 +6449,7 @@
         <v>69</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E96" s="5" t="s">
         <v>70</v>
@@ -6499,7 +6496,7 @@
         <v>69</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E97" s="5" t="s">
         <v>70</v>
@@ -6552,7 +6549,7 @@
         <v>69</v>
       </c>
       <c r="D98" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E98" s="5" t="s">
         <v>70</v>
@@ -6605,7 +6602,7 @@
         <v>69</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E99" s="5" t="s">
         <v>70</v>
@@ -6655,7 +6652,7 @@
         <v>69</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E100" s="5" t="s">
         <v>70</v>
@@ -6705,7 +6702,7 @@
         <v>69</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E101" s="5" t="s">
         <v>70</v>
@@ -6735,7 +6732,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="102" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
         <v>68</v>
       </c>
@@ -6746,7 +6743,7 @@
         <v>69</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E102" s="5" t="s">
         <v>70</v>
@@ -6790,7 +6787,7 @@
         <v>69</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E103" s="5" t="s">
         <v>70</v>
@@ -6834,7 +6831,7 @@
         <v>69</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E104" s="5" t="s">
         <v>70</v>
@@ -6852,7 +6849,7 @@
         <v>3041</v>
       </c>
       <c r="K104" s="12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L104" s="12" t="s">
         <v>136</v>
@@ -6879,7 +6876,7 @@
         <v>69</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E105" s="5" t="s">
         <v>70</v>
@@ -6926,7 +6923,7 @@
         <v>69</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E106" s="5" t="s">
         <v>70</v>
@@ -6973,7 +6970,7 @@
         <v>69</v>
       </c>
       <c r="D107" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E107" s="5" t="s">
         <v>70</v>
@@ -7026,7 +7023,7 @@
         <v>69</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E108" s="5" t="s">
         <v>70</v>
@@ -7079,7 +7076,7 @@
         <v>69</v>
       </c>
       <c r="D109" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E109" s="5" t="s">
         <v>70</v>
@@ -7132,7 +7129,7 @@
         <v>69</v>
       </c>
       <c r="D110" s="6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E110" s="5" t="s">
         <v>70</v>
@@ -7185,7 +7182,7 @@
         <v>69</v>
       </c>
       <c r="D111" s="4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E111" s="5" t="s">
         <v>70</v>
@@ -7241,7 +7238,7 @@
         <v>69</v>
       </c>
       <c r="D112" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E112" s="5" t="s">
         <v>70</v>
@@ -7297,7 +7294,7 @@
         <v>69</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E113" s="5" t="s">
         <v>70</v>
@@ -7347,7 +7344,7 @@
         <v>69</v>
       </c>
       <c r="D114" s="6" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E114" s="5" t="s">
         <v>70</v>
@@ -7397,7 +7394,7 @@
         <v>69</v>
       </c>
       <c r="D115" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E115" s="5" t="s">
         <v>70</v>
@@ -7444,7 +7441,7 @@
         <v>69</v>
       </c>
       <c r="D116" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E116" s="5" t="s">
         <v>70</v>
@@ -7497,7 +7494,7 @@
         <v>69</v>
       </c>
       <c r="D117" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E117" s="5" t="s">
         <v>70</v>
@@ -7539,7 +7536,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="118" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
         <v>68</v>
       </c>
@@ -7550,7 +7547,7 @@
         <v>69</v>
       </c>
       <c r="D118" s="6" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E118" s="5" t="s">
         <v>70</v>
@@ -7594,7 +7591,7 @@
         <v>69</v>
       </c>
       <c r="D119" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E119" s="5" t="s">
         <v>70</v>
@@ -7641,7 +7638,7 @@
         <v>69</v>
       </c>
       <c r="D120" s="6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E120" s="5" t="s">
         <v>70</v>
@@ -7659,7 +7656,7 @@
         <v>3067</v>
       </c>
       <c r="K120" s="12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L120" s="12" t="s">
         <v>136</v>
@@ -7686,7 +7683,7 @@
         <v>69</v>
       </c>
       <c r="D121" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E121" s="5" t="s">
         <v>70</v>
@@ -7733,7 +7730,7 @@
         <v>69</v>
       </c>
       <c r="D122" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E122" s="5" t="s">
         <v>70</v>
@@ -7780,7 +7777,7 @@
         <v>69</v>
       </c>
       <c r="D123" s="16" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E123" s="5" t="s">
         <v>70</v>
@@ -7827,7 +7824,7 @@
         <v>69</v>
       </c>
       <c r="D124" s="16" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E124" s="5" t="s">
         <v>70</v>
@@ -7877,7 +7874,7 @@
         <v>69</v>
       </c>
       <c r="D125" s="6" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E125" s="5" t="s">
         <v>70</v>
@@ -7924,7 +7921,7 @@
         <v>69</v>
       </c>
       <c r="D126" s="6" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E126" s="5" t="s">
         <v>70</v>
@@ -7963,7 +7960,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="127" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
         <v>68</v>
       </c>
@@ -7974,7 +7971,7 @@
         <v>69</v>
       </c>
       <c r="D127" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E127" s="5" t="s">
         <v>70</v>
@@ -8018,7 +8015,7 @@
         <v>69</v>
       </c>
       <c r="D128" s="4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E128" s="5" t="s">
         <v>70</v>
@@ -8071,7 +8068,7 @@
         <v>69</v>
       </c>
       <c r="D129" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E129" s="5" t="s">
         <v>70</v>
@@ -8124,7 +8121,7 @@
         <v>69</v>
       </c>
       <c r="D130" s="4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E130" s="5" t="s">
         <v>70</v>
@@ -8174,7 +8171,7 @@
         <v>69</v>
       </c>
       <c r="D131" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E131" s="5" t="s">
         <v>70</v>
@@ -8224,7 +8221,7 @@
         <v>69</v>
       </c>
       <c r="D132" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E132" s="5" t="s">
         <v>70</v>
@@ -8274,7 +8271,7 @@
         <v>69</v>
       </c>
       <c r="D133" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E133" s="5" t="s">
         <v>70</v>
@@ -8324,7 +8321,7 @@
         <v>69</v>
       </c>
       <c r="D134" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E134" s="5" t="s">
         <v>70</v>
@@ -8371,7 +8368,7 @@
         <v>69</v>
       </c>
       <c r="D135" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E135" s="5" t="s">
         <v>70</v>
@@ -8424,7 +8421,7 @@
         <v>69</v>
       </c>
       <c r="D136" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E136" s="5" t="s">
         <v>70</v>
@@ -8477,7 +8474,7 @@
         <v>69</v>
       </c>
       <c r="D137" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E137" s="5" t="s">
         <v>70</v>
@@ -8527,7 +8524,7 @@
         <v>69</v>
       </c>
       <c r="D138" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E138" s="5" t="s">
         <v>70</v>
@@ -8592,7 +8589,7 @@
         <v>69</v>
       </c>
       <c r="D139" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E139" s="5" t="s">
         <v>70</v>
@@ -8622,7 +8619,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="140" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
         <v>68</v>
       </c>
@@ -8633,7 +8630,7 @@
         <v>69</v>
       </c>
       <c r="D140" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E140" s="5" t="s">
         <v>70</v>
@@ -8666,7 +8663,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="141" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:31" ht="114" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
         <v>68</v>
       </c>
@@ -8677,7 +8674,7 @@
         <v>69</v>
       </c>
       <c r="D141" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E141" s="5" t="s">
         <v>70</v>
@@ -8718,7 +8715,7 @@
         <v>69</v>
       </c>
       <c r="D142" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E142" s="5" t="s">
         <v>70</v>
@@ -8759,7 +8756,7 @@
         <v>69</v>
       </c>
       <c r="D143" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E143" s="5" t="s">
         <v>70</v>
@@ -8800,7 +8797,7 @@
         <v>69</v>
       </c>
       <c r="D144" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E144" s="5" t="s">
         <v>70</v>
@@ -8841,7 +8838,7 @@
         <v>69</v>
       </c>
       <c r="D145" s="4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E145" s="5" t="s">
         <v>70</v>
@@ -8862,7 +8859,7 @@
         <v>4</v>
       </c>
       <c r="K145" s="12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L145" s="12" t="s">
         <v>303</v>
@@ -8882,7 +8879,7 @@
         <v>69</v>
       </c>
       <c r="D146" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E146" s="5" t="s">
         <v>70</v>
@@ -8903,7 +8900,7 @@
         <v>4</v>
       </c>
       <c r="K146" s="12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L146" s="12" t="s">
         <v>303</v>
@@ -8923,7 +8920,7 @@
         <v>69</v>
       </c>
       <c r="D147" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E147" s="5" t="s">
         <v>70</v>
@@ -8944,7 +8941,7 @@
         <v>4</v>
       </c>
       <c r="K147" s="12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L147" s="12" t="s">
         <v>303</v>
@@ -8964,7 +8961,7 @@
         <v>69</v>
       </c>
       <c r="D148" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E148" s="5" t="s">
         <v>70</v>
@@ -8985,7 +8982,7 @@
         <v>4</v>
       </c>
       <c r="K148" s="12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L148" s="12" t="s">
         <v>303</v>
@@ -9005,7 +9002,7 @@
         <v>69</v>
       </c>
       <c r="D149" s="4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E149" s="5" t="s">
         <v>70</v>
@@ -9026,7 +9023,7 @@
         <v>4</v>
       </c>
       <c r="K149" s="12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L149" s="12" t="s">
         <v>303</v>
@@ -9046,7 +9043,7 @@
         <v>69</v>
       </c>
       <c r="D150" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E150" s="5" t="s">
         <v>70</v>
@@ -9067,7 +9064,7 @@
         <v>4</v>
       </c>
       <c r="K150" s="12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L150" s="12" t="s">
         <v>303</v>
@@ -9076,7 +9073,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="151" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:31" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
         <v>68</v>
       </c>
@@ -9087,7 +9084,7 @@
         <v>69</v>
       </c>
       <c r="D151" s="16" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E151" s="5" t="s">
         <v>70</v>
@@ -9122,7 +9119,7 @@
         <v>69</v>
       </c>
       <c r="D152" s="6" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E152" s="5" t="s">
         <v>70</v>
@@ -9143,7 +9140,7 @@
         <v>2</v>
       </c>
       <c r="K152" s="12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L152" s="12" t="s">
         <v>303</v>
@@ -9160,7 +9157,7 @@
         <v>69</v>
       </c>
       <c r="D153" s="6" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E153" s="5" t="s">
         <v>70</v>
@@ -9181,7 +9178,7 @@
         <v>2</v>
       </c>
       <c r="K153" s="12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L153" s="12" t="s">
         <v>303</v>
@@ -9198,7 +9195,7 @@
         <v>69</v>
       </c>
       <c r="D154" s="6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E154" s="5" t="s">
         <v>70</v>
@@ -9219,7 +9216,7 @@
         <v>2</v>
       </c>
       <c r="K154" s="12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L154" s="12" t="s">
         <v>303</v>
@@ -9236,7 +9233,7 @@
         <v>69</v>
       </c>
       <c r="D155" s="6" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E155" s="5" t="s">
         <v>70</v>
@@ -9257,7 +9254,7 @@
         <v>2</v>
       </c>
       <c r="K155" s="12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L155" s="12" t="s">
         <v>303</v>
@@ -9274,7 +9271,7 @@
         <v>69</v>
       </c>
       <c r="D156" s="6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E156" s="5" t="s">
         <v>70</v>
@@ -9295,7 +9292,7 @@
         <v>2</v>
       </c>
       <c r="K156" s="12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L156" s="12" t="s">
         <v>303</v>
@@ -9312,7 +9309,7 @@
         <v>69</v>
       </c>
       <c r="D157" s="6" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E157" s="5" t="s">
         <v>70</v>
@@ -9333,13 +9330,13 @@
         <v>2</v>
       </c>
       <c r="K157" s="12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L157" s="12" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="158" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:31" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
         <v>68</v>
       </c>
@@ -9350,7 +9347,7 @@
         <v>69</v>
       </c>
       <c r="D158" s="16" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E158" s="5" t="s">
         <v>70</v>
@@ -9362,7 +9359,7 @@
         <v>302</v>
       </c>
       <c r="H158" s="12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I158" s="12">
         <v>3097</v>
@@ -9374,7 +9371,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="159" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
         <v>68</v>
       </c>
@@ -9385,7 +9382,7 @@
         <v>69</v>
       </c>
       <c r="D159" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E159" s="5" t="s">
         <v>70</v>
@@ -9397,7 +9394,7 @@
         <v>122</v>
       </c>
       <c r="H159" s="12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I159" s="12">
         <v>3099</v>
@@ -9426,7 +9423,7 @@
         <v>69</v>
       </c>
       <c r="D160" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E160" s="5" t="s">
         <v>70</v>
@@ -9438,7 +9435,7 @@
         <v>302</v>
       </c>
       <c r="H160" s="12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I160" s="12">
         <v>3099</v>
@@ -9467,7 +9464,7 @@
         <v>69</v>
       </c>
       <c r="D161" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E161" s="5" t="s">
         <v>70</v>
@@ -9479,7 +9476,7 @@
         <v>302</v>
       </c>
       <c r="H161" s="12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I161" s="12">
         <v>3099</v>
@@ -9508,7 +9505,7 @@
         <v>69</v>
       </c>
       <c r="D162" s="4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E162" s="5" t="s">
         <v>70</v>
@@ -9520,7 +9517,7 @@
         <v>304</v>
       </c>
       <c r="H162" s="12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I162" s="12">
         <v>3099</v>
@@ -9529,7 +9526,7 @@
         <v>2</v>
       </c>
       <c r="K162" s="12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L162" s="12" t="s">
         <v>303</v>
@@ -9552,7 +9549,7 @@
         <v>69</v>
       </c>
       <c r="D163" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E163" s="5" t="s">
         <v>70</v>
@@ -9564,7 +9561,7 @@
         <v>304</v>
       </c>
       <c r="H163" s="12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I163" s="12">
         <v>3099</v>
@@ -9573,7 +9570,7 @@
         <v>2</v>
       </c>
       <c r="K163" s="12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L163" s="12" t="s">
         <v>303</v>
@@ -9585,7 +9582,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="164" spans="1:31" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
         <v>68</v>
       </c>
@@ -9596,7 +9593,7 @@
         <v>69</v>
       </c>
       <c r="D164" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E164" s="5" t="s">
         <v>70</v>
@@ -9608,7 +9605,7 @@
         <v>122</v>
       </c>
       <c r="H164" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I164" s="12">
         <v>3101</v>
@@ -9623,7 +9620,7 @@
         <v>136</v>
       </c>
       <c r="M164" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AE164" s="15" t="s">
         <v>120</v>
@@ -9640,7 +9637,7 @@
         <v>69</v>
       </c>
       <c r="D165" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E165" s="5" t="s">
         <v>70</v>
@@ -9652,7 +9649,7 @@
         <v>302</v>
       </c>
       <c r="H165" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I165" s="12">
         <v>3101</v>
@@ -9665,7 +9662,7 @@
         <v>303</v>
       </c>
       <c r="M165" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="N165" s="12"/>
       <c r="O165" s="12"/>
@@ -9699,7 +9696,7 @@
         <v>69</v>
       </c>
       <c r="D166" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E166" s="5" t="s">
         <v>70</v>
@@ -9711,7 +9708,7 @@
         <v>302</v>
       </c>
       <c r="H166" s="19" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I166" s="12">
         <v>3101</v>
@@ -9724,7 +9721,7 @@
         <v>303</v>
       </c>
       <c r="M166" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="N166" s="12"/>
       <c r="O166" s="12"/>
@@ -9758,7 +9755,7 @@
         <v>69</v>
       </c>
       <c r="D167" s="4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E167" s="5" t="s">
         <v>70</v>
@@ -9770,7 +9767,7 @@
         <v>304</v>
       </c>
       <c r="H167" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I167" s="12">
         <v>3101</v>
@@ -9779,13 +9776,13 @@
         <v>3</v>
       </c>
       <c r="K167" s="12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L167" s="12" t="s">
         <v>303</v>
       </c>
       <c r="M167" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AE167" s="15" t="s">
         <v>120</v>
@@ -9802,7 +9799,7 @@
         <v>69</v>
       </c>
       <c r="D168" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E168" s="5" t="s">
         <v>70</v>
@@ -9814,7 +9811,7 @@
         <v>304</v>
       </c>
       <c r="H168" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I168" s="12">
         <v>3101</v>
@@ -9823,13 +9820,13 @@
         <v>3</v>
       </c>
       <c r="K168" s="12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L168" s="12" t="s">
         <v>303</v>
       </c>
       <c r="M168" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AE168" s="15" t="s">
         <v>120</v>
@@ -9846,7 +9843,7 @@
         <v>69</v>
       </c>
       <c r="D169" s="6" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E169" s="5" t="s">
         <v>70</v>
@@ -9893,7 +9890,7 @@
         <v>69</v>
       </c>
       <c r="D170" s="6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E170" s="5" t="s">
         <v>70</v>
@@ -9929,7 +9926,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="171" spans="1:31" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:31" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="3" t="s">
         <v>68</v>
       </c>
@@ -9940,7 +9937,7 @@
         <v>69</v>
       </c>
       <c r="D171" s="6" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E171" s="5" t="s">
         <v>70</v>
@@ -9981,9 +9978,15 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:AE171">
-    <filterColumn colId="3">
+    <filterColumn colId="6">
       <filters>
-        <filter val="T1_104 - (Dz. U. z 2015 r. poz. 552)"/>
+        <filter val="3038"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="7">
+      <filters>
+        <filter val="Rp-31g"/>
+        <filter val="Rp-31-g"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
new line, long -, ...
</commit_message>
<xml_diff>
--- a/UEFTA_Teksty.xlsx
+++ b/UEFTA_Teksty.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="15" windowWidth="23415" windowHeight="9960" tabRatio="165"/>
+    <workbookView xWindow="3750" yWindow="15" windowWidth="23415" windowHeight="9960" tabRatio="165"/>
   </bookViews>
   <sheets>
     <sheet name="toSOS_S_TEKSTOW" sheetId="1" r:id="rId1"/>
@@ -962,27 +962,9 @@
     <t>T1_104 - (Dz. U. z 2015 r. poz. 552)</t>
   </si>
   <si>
-    <t>T148_49 - Po przelicz. KP, kwota ponownie oblicz. i zwal. KP - na Pana koncie wynosi …</t>
-  </si>
-  <si>
-    <t>T16_66 - Art. 55a - ... prawo do wcześn. em. zostanie przywrócone w przyp. wycofania wniosku …</t>
-  </si>
-  <si>
-    <t>T2_151 - Art. 26a - W związku z przyznaniem emerytury w powsz. wieku em. … prawo do em. wcześn. ustaje z dniem …</t>
-  </si>
-  <si>
-    <t>T2_152 - Art. 26a - W związku z obliczeniem emerytury w powsz. wieku em. … prawo do em. wcześn. ustaje z dniem …</t>
-  </si>
-  <si>
     <t>T2a_100 - Art 174 ust. 2a i 185a - w związku z przeliczeniem kapitału początkowego</t>
   </si>
   <si>
-    <t>T8_159 - Art 174 ust. 2a i 185a - Po ponownym ustaleniu wysokość … wynosi: SKL + KAP / ŚDTŻ</t>
-  </si>
-  <si>
-    <t>T8_160 - Art 174 ust. 2a i 185a - Po ponownym ustaleniu wysokość … wynosi: KAP / ŚDTZ</t>
-  </si>
-  <si>
     <t>T8_161 - Art. 26 ust. 5 i 6 - ŚDTŻ korzystniejsze [w dniu zgłoszenia wniosku] niż [w dniu osiągn. powsz. w. em.]</t>
   </si>
   <si>
@@ -1007,75 +989,33 @@
     <t>T8_168 - Art. 26 ust. 5 i 6 - ŚDTŻ korzystniejsze [w dniu zgłoszenia wniosku] niż [w dniu spełnienia warunków]</t>
   </si>
   <si>
-    <t>T8_169 - Art. 26 ust. 5 i 6 - ŚDTŻ … w dniu spełnienia warunków</t>
-  </si>
-  <si>
     <t>T8_170 - Art. 26 ust. 5 i 6 - ŚDTŻ korzystniejsze [w dniu 1.01.2009 r.] niż [w dniu zgłoszenia wniosku]</t>
   </si>
   <si>
     <t>T8_171 - Art. 26 ust. 5 i 6 - ŚDTŻ korzystniejsze [w dniu zgłoszenia wniosku] niż [w dniu 1.01.2009 r.]</t>
   </si>
   <si>
-    <t>T88_147 - Art. 55a - Podstawę obliczenia emerytury stanowi … kwota składek + KP</t>
-  </si>
-  <si>
-    <t>T88_148 - Art. 55a - Podstawę obliczenia emerytury stanowi … kwota składek</t>
-  </si>
-  <si>
-    <t>T88_149 - Art. 55a - Podstawę obliczenia emerytury stanowi … KP</t>
-  </si>
-  <si>
     <t>T16_67 - Art. 110a - Ponownego ustalenia em. dokonano ... może nastąpić wyłącznie jeden raz.</t>
   </si>
   <si>
     <t>T16_68 - Art. 110a - spełnia Pan warunki do ponownego ust. em na podst. Art. 110.</t>
   </si>
   <si>
-    <t xml:space="preserve">T10b_66 - Art. 26 ust. 5 i 6 - Do ustalenia wys. okr. em. przyjęto ŚDTŻ … w dniu zgłoszenia wniosku o em. … korzystniejsze od … w dniu osiągn. powsz. w. em. </t>
-  </si>
-  <si>
-    <t>T10b_67 - Art. 26 ust. 5 i 6 - Do ustalenia wys. okr. em. przyjęto ŚDTŻ … w dniu osiągn. powsz. w. em. … korzystniejsze od … w dniu zgłoszenia wniosku o em.</t>
-  </si>
-  <si>
-    <t>T10b_68 - Art. 26 ust. 5 i 6 - Do ustalenia wys. okr. em. przyjęto ŚDTŻ … w dniu osiągn. powsz. w. em. … korzystniejsze od … wypłata zawiesz. renty z tyt. niezd. do pracy</t>
-  </si>
-  <si>
-    <t>T10b_69 - Art. 26 ust. 5 i 6 - Do ustalenia wys. okr. em. przyjęto ŚDTŻ … wypłata zawiesz. renty z tyt. niezd. do pracy … korzystniejsze od … osiągn. powsz. w. em.</t>
-  </si>
-  <si>
     <t>T16_68 - Art. 110a - spełnia Pan/i warunki do ponownego ust. em na podst. Art. 110.</t>
   </si>
   <si>
-    <t>T148_50 - Po przelicz. KP, kwota ponownie oblicz. i zwal. KP - na koncie osoby zmarłej wynosi …</t>
-  </si>
-  <si>
     <t>T2b_55 - Art. 174 ust. 2a i Art. 185a - ponownie ustala wysokość</t>
   </si>
   <si>
     <t>T3_211 - Art. 174 ust. 2a i Art. 185a - renty rodzinnej</t>
   </si>
   <si>
-    <t>T8_172 - Art 174 ust. 2a i 185a - Po ponownym ustaleniu … wysokość świadcz. osoby zmarłej … wynosi: SKL + KAP / ŚDTŻ</t>
-  </si>
-  <si>
-    <t>T8_173 - Art 174 ust. 2a i 185a - Po ponownym ustaleniu … wysokość świadcz. osoby zmarłej … wynosi: KAP / ŚDTŻ</t>
-  </si>
-  <si>
     <t>T8_174 - Art. 26 ust. 5 i 6 - ŚDTŻ korzystniejsze [w dniu osiągn. wieku os. zm.] niż [w dniu zgłoszenia wniosku]</t>
   </si>
   <si>
     <t>T8_175 - Art. 26 ust. 5 i 6 - ŚDTŻ korzystniejsze [w dniu osiągn. wieku] niż [w dniu zgonu]</t>
   </si>
   <si>
-    <t>T8_176 - Art. 55 i 55a - Po ponownym ustaleniu … wysokość świadcz. osoby zmarłej … wynosi: SKL + KAP - POBR.EM. / ŚDTŻ</t>
-  </si>
-  <si>
-    <t>T8_177 - Art. 55 i 55a - Po ponownym ustaleniu … wysokość świadcz. osoby zmarłej … wynosi: SKL - POBR.EM. / ŚDTŻ</t>
-  </si>
-  <si>
-    <t>T8_178 - Art. 55 i 55a - Po ponownym ustaleniu … wysokość świadcz. osoby zmarłej … wynosi: KAP - POBR.EM. / ŚDTŻ</t>
-  </si>
-  <si>
     <t>T8_179 - Art. 26 ust. 5 i 6 - ŚDTŻ korzystniejsze [w dniu zgonu] niż [w dniu osiągn. wieku]</t>
   </si>
   <si>
@@ -1088,9 +1028,6 @@
     <t>T8_182 - Art. 26 ust. 5 i 6 - ŚDTŻ korzystniejsze [w dniu zgonu] niż [w dniu spełnienia warunków]</t>
   </si>
   <si>
-    <t>T8_183 - Art. 26 ust. 5 i 6 - ŚDTŻ … w dniu spełnienia warunków - dla osoby zmarłej</t>
-  </si>
-  <si>
     <t>T8_184 - Art. 26 ust. 5 i 6 - ŚDTŻ korzystniejsze [w dniu nast. po wieku] niż [w dniu zgonu]</t>
   </si>
   <si>
@@ -1103,48 +1040,9 @@
     <t>T8_187 - Art. 26 ust. 5 i 6 - ŚDTŻ korzystniejsze [w dniu zgonu] niż [w dniu 01.01.2009 r.]</t>
   </si>
   <si>
-    <t>T88_150 - Art. 55a - Podstawę obliczenia emerytury osoby zmarłej stanowi … kwota składek + KP</t>
-  </si>
-  <si>
-    <t>T88_151 - Art. 55a - Podstawę obliczenia emerytury osoby zmarłej stanowi … kwota składek</t>
-  </si>
-  <si>
-    <t>T88_152 - Art. 55a - Podstawę obliczenia emerytury osoby zmarłej stanowi … KP</t>
-  </si>
-  <si>
-    <t>T16_69 - Art. 110a - Ponownego ustalenia em. osoby zmarłej dokonano … może nastąpić wyłącznie jeden raz.</t>
-  </si>
-  <si>
-    <t>T8_163 - Art. 26 ust. 5 i 6 - z urzędu ŚDTŻ … w dniu osiągn. powsz. w. em. … korzystniejsze od … wypłata zawiesz. renty z tyt. niezd. do pracy</t>
-  </si>
-  <si>
-    <t>T50_449 - Zgodnie z art. 174 ust. 2a ... przy ustalaniu KP okresy urlopów lub niewyk. pracy oblicza się przyj. 1,3% PW …</t>
-  </si>
-  <si>
-    <t>T50_450 - Zgodnie z art. 185a … poprzez dodanie do okresów nieskładk. okresów studiów wyższ. w wymiarze 1/3 okr. składk.</t>
-  </si>
-  <si>
-    <t>T50_451 - Art. 55a - Wprowadzony ustawą … umożliwia ponowne obliczenie, z zast. art. 55 … osobie, która miała ustalone prawo do em. wcześn. i kontynuowała ubezp.</t>
-  </si>
-  <si>
-    <t>T50_452 - Art. 26 ust. 6 - Wysokość em. podlega ponownemu ustaleniu … jeżeli obowiązywała inna tablica ŚDTŻ …</t>
-  </si>
-  <si>
-    <t>T54_698 - Art. 55 i 55a - nie kontynuował/a Pan/i ubezp. … po osiągn. powsz. w. em. … brak podstaw do oblicz.</t>
-  </si>
-  <si>
-    <t>T54_699 - Art. 55 i 55a - emerytura została przyznana przed dniem 1 stycznia 2009 r., a zatem brak jest podstaw do obliczenia …</t>
-  </si>
-  <si>
     <t>T54_700 - Art. 55 i 55a - emerytura nie została przyznana na podstawie art. 27 ustawy emerytalnej, a zatem brak jest podstaw</t>
   </si>
   <si>
-    <t>T54_701 - wniosek o emeryturę zgłosił Pan(i) w miesiącu, w którym obowiązywała ta sama tablica ŚDTŻ …</t>
-  </si>
-  <si>
-    <t>T50_453 - Zgodnie z art. 110a … dotyczy wyłącznie em. i może nastąpić wyłącznie jeden raz</t>
-  </si>
-  <si>
     <t>T54_699 - Art. 110a - ponowne ustalenie świadczenia dotyczy wyłącznie emerytury</t>
   </si>
   <si>
@@ -1152,18 +1050,6 @@
   </si>
   <si>
     <t>T54_701 - Art. 110a - nowo ustalony wskaźnik wysokości podstawy wymiaru emerytury nie przekracza 250%</t>
-  </si>
-  <si>
-    <t>T54_702 - Art. 110a - do ponownego ustalenia … wskazano wynagrodzenia przyjęte do ostatnio obliczonej podstawy wymiaru</t>
-  </si>
-  <si>
-    <t>T54_703 - Art. 110a - do ponownego ustalenia podstawy wymiaru emerytury nie wskazano wynagrodzeń …</t>
-  </si>
-  <si>
-    <t>T54_704 - Art. 110a - nie podlegał/a Pan/i ubezp. społecz. … po przyznaniu em. … brak podstaw do ponownego przel.</t>
-  </si>
-  <si>
-    <t>T50_454 - Art. 110a - Wysokość emerytury podlega ponownemu ustaleniu … gdy zostały spełnione warunki …</t>
   </si>
   <si>
     <t>Zakład informuje, że prawo do wcześniejszej emerytury zostanie przywrócone w przypadku wycofania wniosku o emeryturę przyznaną na podstawie niniejszej decyzji. Wycofanie wniosku o emeryturę możliwe jest do dnia uprawomocnienia się decyzji, tj. w przypadku niezłożenia odwołania do sądu - w terminie miesiąca od dnia doręczenia decyzji.</t>
@@ -1210,6 +1096,120 @@
   </si>
   <si>
     <t>- nie podlegał&lt;A&gt; &lt;PANPANISWIADCZENIOBIORCA&gt; ubezpieczeniu społecznemu - ubezpieczeniom emerytalnemu i rentowym po przyznaniu emerytury, a zatem brak jest podstaw do ponownego obliczenia emerytury w myśl art. 110a ustawy emerytalnej</t>
+  </si>
+  <si>
+    <t>T148_49 - Po przelicz. KP, kwota ponownie oblicz. i zwal. KP - na Pana koncie wynosi ...</t>
+  </si>
+  <si>
+    <t>T16_66 - Art. 55a - ... prawo do wcześn. em. zostanie przywrócone w przyp. wycofania wniosku ...</t>
+  </si>
+  <si>
+    <t>T2_151 - Art. 26a - W związku z przyznaniem emerytury w powsz. wieku em. ... prawo do em. wcześn. ustaje z dniem ...</t>
+  </si>
+  <si>
+    <t>T2_152 - Art. 26a - W związku z obliczeniem emerytury w powsz. wieku em. ... prawo do em. wcześn. ustaje z dniem ...</t>
+  </si>
+  <si>
+    <t>T8_159 - Art 174 ust. 2a i 185a - Po ponownym ustaleniu wysokość ... wynosi: SKL + KAP / ŚDTŻ</t>
+  </si>
+  <si>
+    <t>T8_160 - Art 174 ust. 2a i 185a - Po ponownym ustaleniu wysokość ... wynosi: KAP / ŚDTZ</t>
+  </si>
+  <si>
+    <t>T8_169 - Art. 26 ust. 5 i 6 - ŚDTŻ ... w dniu spełnienia warunków</t>
+  </si>
+  <si>
+    <t>T88_147 - Art. 55a - Podstawę obliczenia emerytury stanowi ... kwota składek + KP</t>
+  </si>
+  <si>
+    <t>T88_148 - Art. 55a - Podstawę obliczenia emerytury stanowi ... kwota składek</t>
+  </si>
+  <si>
+    <t>T88_149 - Art. 55a - Podstawę obliczenia emerytury stanowi ... KP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T10b_66 - Art. 26 ust. 5 i 6 - Do ustalenia wys. okr. em. przyjęto ŚDTŻ ... w dniu zgłoszenia wniosku o em. ... korzystniejsze od ... w dniu osiągn. powsz. w. em. </t>
+  </si>
+  <si>
+    <t>T10b_67 - Art. 26 ust. 5 i 6 - Do ustalenia wys. okr. em. przyjęto ŚDTŻ ... w dniu osiągn. powsz. w. em. ... korzystniejsze od ... w dniu zgłoszenia wniosku o em.</t>
+  </si>
+  <si>
+    <t>T10b_68 - Art. 26 ust. 5 i 6 - Do ustalenia wys. okr. em. przyjęto ŚDTŻ ... w dniu osiągn. powsz. w. em. ... korzystniejsze od ... wypłata zawiesz. renty z tyt. niezd. do pracy</t>
+  </si>
+  <si>
+    <t>T10b_69 - Art. 26 ust. 5 i 6 - Do ustalenia wys. okr. em. przyjęto ŚDTŻ ... wypłata zawiesz. renty z tyt. niezd. do pracy ... korzystniejsze od ... osiągn. powsz. w. em.</t>
+  </si>
+  <si>
+    <t>T148_50 - Po przelicz. KP, kwota ponownie oblicz. i zwal. KP - na koncie osoby zmarłej wynosi ...</t>
+  </si>
+  <si>
+    <t>T8_172 - Art 174 ust. 2a i 185a - Po ponownym ustaleniu ... wysokość świadcz. osoby zmarłej ... wynosi: SKL + KAP / ŚDTŻ</t>
+  </si>
+  <si>
+    <t>T8_173 - Art 174 ust. 2a i 185a - Po ponownym ustaleniu ... wysokość świadcz. osoby zmarłej ... wynosi: KAP / ŚDTŻ</t>
+  </si>
+  <si>
+    <t>T8_176 - Art. 55 i 55a - Po ponownym ustaleniu ... wysokość świadcz. osoby zmarłej ... wynosi: SKL + KAP - POBR.EM. / ŚDTŻ</t>
+  </si>
+  <si>
+    <t>T8_177 - Art. 55 i 55a - Po ponownym ustaleniu ... wysokość świadcz. osoby zmarłej ... wynosi: SKL - POBR.EM. / ŚDTŻ</t>
+  </si>
+  <si>
+    <t>T8_178 - Art. 55 i 55a - Po ponownym ustaleniu ... wysokość świadcz. osoby zmarłej ... wynosi: KAP - POBR.EM. / ŚDTŻ</t>
+  </si>
+  <si>
+    <t>T8_183 - Art. 26 ust. 5 i 6 - ŚDTŻ ... w dniu spełnienia warunków - dla osoby zmarłej</t>
+  </si>
+  <si>
+    <t>T88_150 - Art. 55a - Podstawę obliczenia emerytury osoby zmarłej stanowi ... kwota składek + KP</t>
+  </si>
+  <si>
+    <t>T88_151 - Art. 55a - Podstawę obliczenia emerytury osoby zmarłej stanowi ... kwota składek</t>
+  </si>
+  <si>
+    <t>T88_152 - Art. 55a - Podstawę obliczenia emerytury osoby zmarłej stanowi ... KP</t>
+  </si>
+  <si>
+    <t>T16_69 - Art. 110a - Ponownego ustalenia em. osoby zmarłej dokonano ... może nastąpić wyłącznie jeden raz.</t>
+  </si>
+  <si>
+    <t>T8_163 - Art. 26 ust. 5 i 6 - z urzędu ŚDTŻ ... w dniu osiągn. powsz. w. em. ... korzystniejsze od ... wypłata zawiesz. renty z tyt. niezd. do pracy</t>
+  </si>
+  <si>
+    <t>T50_449 - Zgodnie z art. 174 ust. 2a ... przy ustalaniu KP okresy urlopów lub niewyk. pracy oblicza się przyj. 1,3% PW ...</t>
+  </si>
+  <si>
+    <t>T50_450 - Zgodnie z art. 185a ... poprzez dodanie do okresów nieskładk. okresów studiów wyższ. w wymiarze 1/3 okr. składk.</t>
+  </si>
+  <si>
+    <t>T50_451 - Art. 55a - Wprowadzony ustawą ... umożliwia ponowne obliczenie, z zast. art. 55 ... osobie, która miała ustalone prawo do em. wcześn. i kontynuowała ubezp.</t>
+  </si>
+  <si>
+    <t>T50_452 - Art. 26 ust. 6 - Wysokość em. podlega ponownemu ustaleniu ... jeżeli obowiązywała inna tablica ŚDTŻ ...</t>
+  </si>
+  <si>
+    <t>T54_698 - Art. 55 i 55a - nie kontynuował/a Pan/i ubezp. ... po osiągn. powsz. w. em. ... brak podstaw do oblicz.</t>
+  </si>
+  <si>
+    <t>T54_699 - Art. 55 i 55a - emerytura została przyznana przed dniem 1 stycznia 2009 r., a zatem brak jest podstaw do obliczenia ...</t>
+  </si>
+  <si>
+    <t>T54_701 - wniosek o emeryturę zgłosił Pan(i) w miesiącu, w którym obowiązywała ta sama tablica ŚDTŻ ...</t>
+  </si>
+  <si>
+    <t>T50_453 - Zgodnie z art. 110a ... dotyczy wyłącznie em. i może nastąpić wyłącznie jeden raz</t>
+  </si>
+  <si>
+    <t>T54_702 - Art. 110a - do ponownego ustalenia ... wskazano wynagrodzenia przyjęte do ostatnio obliczonej podstawy wymiaru</t>
+  </si>
+  <si>
+    <t>T54_703 - Art. 110a - do ponownego ustalenia podstawy wymiaru emerytury nie wskazano wynagrodzeń ...</t>
+  </si>
+  <si>
+    <t>T54_704 - Art. 110a - nie podlegał/a Pan/i ubezp. społecz. ... po przyznaniu em. ... brak podstaw do ponownego przel.</t>
+  </si>
+  <si>
+    <t>T50_454 - Art. 110a - Wysokość emerytury podlega ponownemu ustaleniu ... gdy zostały spełnione warunki ...</t>
   </si>
 </sst>
 </file>
@@ -1648,7 +1648,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1830,7 +1830,7 @@
         <v>57</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>304</v>
+        <v>348</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>58</v>
@@ -1877,13 +1877,13 @@
         <v>57</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>305</v>
+        <v>349</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>58</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>372</v>
+        <v>334</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>129</v>
@@ -1918,7 +1918,7 @@
         <v>57</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>306</v>
+        <v>350</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>58</v>
@@ -1971,7 +1971,7 @@
         <v>57</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>307</v>
+        <v>351</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>58</v>
@@ -2038,13 +2038,13 @@
         <v>57</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>58</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>373</v>
+        <v>335</v>
       </c>
       <c r="G7" s="7" t="s">
         <v>112</v>
@@ -2084,7 +2084,7 @@
         <v>57</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>309</v>
+        <v>352</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>58</v>
@@ -2128,7 +2128,7 @@
         <v>57</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>310</v>
+        <v>353</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>58</v>
@@ -2172,7 +2172,7 @@
         <v>57</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>58</v>
@@ -2228,7 +2228,7 @@
         <v>57</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>58</v>
@@ -2286,7 +2286,7 @@
         <v>57</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>58</v>
@@ -2337,7 +2337,7 @@
         <v>57</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>58</v>
@@ -2395,7 +2395,7 @@
         <v>57</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>58</v>
@@ -2456,7 +2456,7 @@
         <v>57</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>58</v>
@@ -2514,7 +2514,7 @@
         <v>57</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>58</v>
@@ -2565,7 +2565,7 @@
         <v>57</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>58</v>
@@ -2616,7 +2616,7 @@
         <v>57</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>319</v>
+        <v>354</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>58</v>
@@ -2663,7 +2663,7 @@
         <v>57</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>58</v>
@@ -2716,7 +2716,7 @@
         <v>57</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>58</v>
@@ -2769,7 +2769,7 @@
         <v>57</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>322</v>
+        <v>355</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>58</v>
@@ -2832,7 +2832,7 @@
         <v>57</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>323</v>
+        <v>356</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>58</v>
@@ -2895,7 +2895,7 @@
         <v>57</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>324</v>
+        <v>357</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>58</v>
@@ -2989,7 +2989,7 @@
         <v>57</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>304</v>
+        <v>348</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>58</v>
@@ -3050,13 +3050,13 @@
         <v>57</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>58</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>373</v>
+        <v>335</v>
       </c>
       <c r="G26" s="7" t="s">
         <v>112</v>
@@ -3095,7 +3095,7 @@
         <v>57</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>309</v>
+        <v>352</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>58</v>
@@ -3143,7 +3143,7 @@
         <v>57</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>310</v>
+        <v>353</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>58</v>
@@ -3235,7 +3235,7 @@
         <v>57</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>304</v>
+        <v>348</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>58</v>
@@ -3296,13 +3296,13 @@
         <v>57</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>58</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>373</v>
+        <v>335</v>
       </c>
       <c r="G31" s="7" t="s">
         <v>112</v>
@@ -3341,7 +3341,7 @@
         <v>57</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>309</v>
+        <v>352</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>58</v>
@@ -3386,7 +3386,7 @@
         <v>57</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>310</v>
+        <v>353</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>58</v>
@@ -3478,7 +3478,7 @@
         <v>57</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>304</v>
+        <v>348</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>58</v>
@@ -3523,13 +3523,13 @@
         <v>57</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>58</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>373</v>
+        <v>335</v>
       </c>
       <c r="G36" s="7" t="s">
         <v>112</v>
@@ -3568,7 +3568,7 @@
         <v>57</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>309</v>
+        <v>352</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>58</v>
@@ -3613,7 +3613,7 @@
         <v>57</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>310</v>
+        <v>353</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>58</v>
@@ -3657,7 +3657,7 @@
         <v>57</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>58</v>
@@ -3710,7 +3710,7 @@
         <v>57</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>58</v>
@@ -3763,7 +3763,7 @@
         <v>57</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>58</v>
@@ -3816,7 +3816,7 @@
         <v>57</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>58</v>
@@ -3883,7 +3883,7 @@
         <v>57</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>58</v>
@@ -3939,7 +3939,7 @@
         <v>57</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>58</v>
@@ -3995,7 +3995,7 @@
         <v>57</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>58</v>
@@ -4045,7 +4045,7 @@
         <v>57</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>58</v>
@@ -4095,7 +4095,7 @@
         <v>57</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>319</v>
+        <v>354</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>58</v>
@@ -4142,7 +4142,7 @@
         <v>57</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="E48" s="5" t="s">
         <v>58</v>
@@ -4195,7 +4195,7 @@
         <v>57</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="E49" s="5" t="s">
         <v>58</v>
@@ -4292,7 +4292,7 @@
         <v>57</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>304</v>
+        <v>348</v>
       </c>
       <c r="E51" s="5" t="s">
         <v>58</v>
@@ -4339,13 +4339,13 @@
         <v>57</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="E52" s="5" t="s">
         <v>58</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>373</v>
+        <v>335</v>
       </c>
       <c r="G52" s="7" t="s">
         <v>112</v>
@@ -4384,7 +4384,7 @@
         <v>57</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>309</v>
+        <v>352</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>58</v>
@@ -4431,7 +4431,7 @@
         <v>57</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>310</v>
+        <v>353</v>
       </c>
       <c r="E54" s="5" t="s">
         <v>58</v>
@@ -4478,7 +4478,7 @@
         <v>57</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
       <c r="E55" s="5" t="s">
         <v>58</v>
@@ -4525,7 +4525,7 @@
         <v>57</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="E56" s="5" t="s">
         <v>58</v>
@@ -4619,7 +4619,7 @@
         <v>57</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>327</v>
+        <v>358</v>
       </c>
       <c r="E58" s="5" t="s">
         <v>58</v>
@@ -4666,7 +4666,7 @@
         <v>57</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>328</v>
+        <v>359</v>
       </c>
       <c r="E59" s="5" t="s">
         <v>58</v>
@@ -4713,7 +4713,7 @@
         <v>57</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>329</v>
+        <v>360</v>
       </c>
       <c r="E60" s="5" t="s">
         <v>58</v>
@@ -4760,7 +4760,7 @@
         <v>57</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>330</v>
+        <v>361</v>
       </c>
       <c r="E61" s="5" t="s">
         <v>58</v>
@@ -4807,7 +4807,7 @@
         <v>57</v>
       </c>
       <c r="D62" s="16" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
       <c r="E62" s="5" t="s">
         <v>58</v>
@@ -4854,7 +4854,7 @@
         <v>57</v>
       </c>
       <c r="D63" s="16" t="s">
-        <v>331</v>
+        <v>317</v>
       </c>
       <c r="E63" s="5" t="s">
         <v>58</v>
@@ -4945,13 +4945,13 @@
         <v>57</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="E65" s="5" t="s">
         <v>58</v>
       </c>
       <c r="F65" s="6" t="s">
-        <v>373</v>
+        <v>335</v>
       </c>
       <c r="G65" s="7" t="s">
         <v>112</v>
@@ -5031,7 +5031,7 @@
         <v>57</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>332</v>
+        <v>362</v>
       </c>
       <c r="E67" s="5" t="s">
         <v>58</v>
@@ -5075,7 +5075,7 @@
         <v>57</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
       <c r="E68" s="5" t="s">
         <v>58</v>
@@ -5116,7 +5116,7 @@
         <v>57</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>334</v>
+        <v>319</v>
       </c>
       <c r="E69" s="5" t="s">
         <v>58</v>
@@ -5157,13 +5157,13 @@
         <v>57</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>335</v>
+        <v>363</v>
       </c>
       <c r="E70" s="5" t="s">
         <v>58</v>
       </c>
       <c r="F70" s="6" t="s">
-        <v>374</v>
+        <v>336</v>
       </c>
       <c r="G70" s="7" t="s">
         <v>125</v>
@@ -5204,13 +5204,13 @@
         <v>57</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>336</v>
+        <v>364</v>
       </c>
       <c r="E71" s="5" t="s">
         <v>58</v>
       </c>
       <c r="F71" s="6" t="s">
-        <v>375</v>
+        <v>337</v>
       </c>
       <c r="G71" s="7" t="s">
         <v>125</v>
@@ -5251,7 +5251,7 @@
         <v>57</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>337</v>
+        <v>320</v>
       </c>
       <c r="E72" s="5" t="s">
         <v>58</v>
@@ -5301,7 +5301,7 @@
         <v>57</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>338</v>
+        <v>321</v>
       </c>
       <c r="E73" s="5" t="s">
         <v>58</v>
@@ -5348,13 +5348,13 @@
         <v>57</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>339</v>
+        <v>365</v>
       </c>
       <c r="E74" s="5" t="s">
         <v>58</v>
       </c>
       <c r="F74" s="6" t="s">
-        <v>376</v>
+        <v>338</v>
       </c>
       <c r="G74" s="7" t="s">
         <v>125</v>
@@ -5395,13 +5395,13 @@
         <v>57</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>340</v>
+        <v>366</v>
       </c>
       <c r="E75" s="5" t="s">
         <v>58</v>
       </c>
       <c r="F75" s="6" t="s">
-        <v>377</v>
+        <v>339</v>
       </c>
       <c r="G75" s="7" t="s">
         <v>125</v>
@@ -5442,13 +5442,13 @@
         <v>57</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>341</v>
+        <v>367</v>
       </c>
       <c r="E76" s="5" t="s">
         <v>58</v>
       </c>
       <c r="F76" s="6" t="s">
-        <v>378</v>
+        <v>340</v>
       </c>
       <c r="G76" s="7" t="s">
         <v>125</v>
@@ -5489,7 +5489,7 @@
         <v>57</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>342</v>
+        <v>322</v>
       </c>
       <c r="E77" s="5" t="s">
         <v>58</v>
@@ -5539,7 +5539,7 @@
         <v>57</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>343</v>
+        <v>323</v>
       </c>
       <c r="E78" s="5" t="s">
         <v>58</v>
@@ -5589,7 +5589,7 @@
         <v>57</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>344</v>
+        <v>324</v>
       </c>
       <c r="E79" s="5" t="s">
         <v>58</v>
@@ -5639,7 +5639,7 @@
         <v>57</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>345</v>
+        <v>325</v>
       </c>
       <c r="E80" s="5" t="s">
         <v>58</v>
@@ -5689,7 +5689,7 @@
         <v>57</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>346</v>
+        <v>368</v>
       </c>
       <c r="E81" s="5" t="s">
         <v>58</v>
@@ -5736,7 +5736,7 @@
         <v>57</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>347</v>
+        <v>326</v>
       </c>
       <c r="E82" s="5" t="s">
         <v>58</v>
@@ -5789,7 +5789,7 @@
         <v>57</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>348</v>
+        <v>327</v>
       </c>
       <c r="E83" s="5" t="s">
         <v>58</v>
@@ -5842,7 +5842,7 @@
         <v>57</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>349</v>
+        <v>328</v>
       </c>
       <c r="E84" s="5" t="s">
         <v>58</v>
@@ -5895,7 +5895,7 @@
         <v>57</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>350</v>
+        <v>329</v>
       </c>
       <c r="E85" s="5" t="s">
         <v>58</v>
@@ -5948,7 +5948,7 @@
         <v>57</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>351</v>
+        <v>369</v>
       </c>
       <c r="E86" s="5" t="s">
         <v>58</v>
@@ -5998,7 +5998,7 @@
         <v>57</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>352</v>
+        <v>370</v>
       </c>
       <c r="E87" s="5" t="s">
         <v>58</v>
@@ -6048,7 +6048,7 @@
         <v>57</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>353</v>
+        <v>371</v>
       </c>
       <c r="E88" s="5" t="s">
         <v>58</v>
@@ -6142,7 +6142,7 @@
         <v>57</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>337</v>
+        <v>320</v>
       </c>
       <c r="E90" s="5" t="s">
         <v>58</v>
@@ -6195,7 +6195,7 @@
         <v>57</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>338</v>
+        <v>321</v>
       </c>
       <c r="E91" s="5" t="s">
         <v>58</v>
@@ -6248,7 +6248,7 @@
         <v>57</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>342</v>
+        <v>322</v>
       </c>
       <c r="E92" s="5" t="s">
         <v>58</v>
@@ -6298,7 +6298,7 @@
         <v>57</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>343</v>
+        <v>323</v>
       </c>
       <c r="E93" s="5" t="s">
         <v>58</v>
@@ -6348,7 +6348,7 @@
         <v>57</v>
       </c>
       <c r="D94" s="4" t="s">
-        <v>344</v>
+        <v>324</v>
       </c>
       <c r="E94" s="5" t="s">
         <v>58</v>
@@ -6398,7 +6398,7 @@
         <v>57</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>345</v>
+        <v>325</v>
       </c>
       <c r="E95" s="5" t="s">
         <v>58</v>
@@ -6448,7 +6448,7 @@
         <v>57</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>346</v>
+        <v>368</v>
       </c>
       <c r="E96" s="5" t="s">
         <v>58</v>
@@ -6495,7 +6495,7 @@
         <v>57</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>347</v>
+        <v>326</v>
       </c>
       <c r="E97" s="5" t="s">
         <v>58</v>
@@ -6548,7 +6548,7 @@
         <v>57</v>
       </c>
       <c r="D98" s="4" t="s">
-        <v>348</v>
+        <v>327</v>
       </c>
       <c r="E98" s="5" t="s">
         <v>58</v>
@@ -6601,7 +6601,7 @@
         <v>57</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>349</v>
+        <v>328</v>
       </c>
       <c r="E99" s="5" t="s">
         <v>58</v>
@@ -6651,7 +6651,7 @@
         <v>57</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>350</v>
+        <v>329</v>
       </c>
       <c r="E100" s="5" t="s">
         <v>58</v>
@@ -6701,7 +6701,7 @@
         <v>57</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>354</v>
+        <v>372</v>
       </c>
       <c r="E101" s="5" t="s">
         <v>58</v>
@@ -6786,7 +6786,7 @@
         <v>57</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>304</v>
+        <v>348</v>
       </c>
       <c r="E103" s="5" t="s">
         <v>58</v>
@@ -6830,13 +6830,13 @@
         <v>57</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="E104" s="5" t="s">
         <v>58</v>
       </c>
       <c r="F104" s="6" t="s">
-        <v>373</v>
+        <v>335</v>
       </c>
       <c r="G104" s="7" t="s">
         <v>112</v>
@@ -6875,7 +6875,7 @@
         <v>57</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>309</v>
+        <v>352</v>
       </c>
       <c r="E105" s="5" t="s">
         <v>58</v>
@@ -6922,7 +6922,7 @@
         <v>57</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>310</v>
+        <v>353</v>
       </c>
       <c r="E106" s="5" t="s">
         <v>58</v>
@@ -6969,7 +6969,7 @@
         <v>57</v>
       </c>
       <c r="D107" s="4" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="E107" s="5" t="s">
         <v>58</v>
@@ -7022,7 +7022,7 @@
         <v>57</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="E108" s="5" t="s">
         <v>58</v>
@@ -7075,7 +7075,7 @@
         <v>57</v>
       </c>
       <c r="D109" s="4" t="s">
-        <v>355</v>
+        <v>373</v>
       </c>
       <c r="E109" s="5" t="s">
         <v>58</v>
@@ -7128,7 +7128,7 @@
         <v>57</v>
       </c>
       <c r="D110" s="6" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="E110" s="5" t="s">
         <v>58</v>
@@ -7181,7 +7181,7 @@
         <v>57</v>
       </c>
       <c r="D111" s="4" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="E111" s="5" t="s">
         <v>58</v>
@@ -7237,7 +7237,7 @@
         <v>57</v>
       </c>
       <c r="D112" s="4" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="E112" s="5" t="s">
         <v>58</v>
@@ -7293,7 +7293,7 @@
         <v>57</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="E113" s="5" t="s">
         <v>58</v>
@@ -7343,7 +7343,7 @@
         <v>57</v>
       </c>
       <c r="D114" s="6" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="E114" s="5" t="s">
         <v>58</v>
@@ -7393,7 +7393,7 @@
         <v>57</v>
       </c>
       <c r="D115" s="4" t="s">
-        <v>319</v>
+        <v>354</v>
       </c>
       <c r="E115" s="5" t="s">
         <v>58</v>
@@ -7440,7 +7440,7 @@
         <v>57</v>
       </c>
       <c r="D116" s="4" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="E116" s="5" t="s">
         <v>58</v>
@@ -7493,7 +7493,7 @@
         <v>57</v>
       </c>
       <c r="D117" s="4" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="E117" s="5" t="s">
         <v>58</v>
@@ -7590,7 +7590,7 @@
         <v>57</v>
       </c>
       <c r="D119" s="4" t="s">
-        <v>304</v>
+        <v>348</v>
       </c>
       <c r="E119" s="5" t="s">
         <v>58</v>
@@ -7637,13 +7637,13 @@
         <v>57</v>
       </c>
       <c r="D120" s="6" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="E120" s="5" t="s">
         <v>58</v>
       </c>
       <c r="F120" s="6" t="s">
-        <v>373</v>
+        <v>335</v>
       </c>
       <c r="G120" s="7" t="s">
         <v>112</v>
@@ -7682,7 +7682,7 @@
         <v>57</v>
       </c>
       <c r="D121" s="4" t="s">
-        <v>309</v>
+        <v>352</v>
       </c>
       <c r="E121" s="5" t="s">
         <v>58</v>
@@ -7729,7 +7729,7 @@
         <v>57</v>
       </c>
       <c r="D122" s="4" t="s">
-        <v>310</v>
+        <v>353</v>
       </c>
       <c r="E122" s="5" t="s">
         <v>58</v>
@@ -7776,7 +7776,7 @@
         <v>57</v>
       </c>
       <c r="D123" s="16" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
       <c r="E123" s="5" t="s">
         <v>58</v>
@@ -7823,7 +7823,7 @@
         <v>57</v>
       </c>
       <c r="D124" s="16" t="s">
-        <v>331</v>
+        <v>317</v>
       </c>
       <c r="E124" s="5" t="s">
         <v>58</v>
@@ -7873,7 +7873,7 @@
         <v>57</v>
       </c>
       <c r="D125" s="6" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
       <c r="E125" s="5" t="s">
         <v>58</v>
@@ -7920,7 +7920,7 @@
         <v>57</v>
       </c>
       <c r="D126" s="6" t="s">
-        <v>331</v>
+        <v>317</v>
       </c>
       <c r="E126" s="5" t="s">
         <v>58</v>
@@ -8014,7 +8014,7 @@
         <v>57</v>
       </c>
       <c r="D128" s="4" t="s">
-        <v>337</v>
+        <v>320</v>
       </c>
       <c r="E128" s="5" t="s">
         <v>58</v>
@@ -8067,7 +8067,7 @@
         <v>57</v>
       </c>
       <c r="D129" s="4" t="s">
-        <v>338</v>
+        <v>321</v>
       </c>
       <c r="E129" s="5" t="s">
         <v>58</v>
@@ -8120,7 +8120,7 @@
         <v>57</v>
       </c>
       <c r="D130" s="4" t="s">
-        <v>342</v>
+        <v>322</v>
       </c>
       <c r="E130" s="5" t="s">
         <v>58</v>
@@ -8170,7 +8170,7 @@
         <v>57</v>
       </c>
       <c r="D131" s="4" t="s">
-        <v>343</v>
+        <v>323</v>
       </c>
       <c r="E131" s="5" t="s">
         <v>58</v>
@@ -8220,7 +8220,7 @@
         <v>57</v>
       </c>
       <c r="D132" s="4" t="s">
-        <v>344</v>
+        <v>324</v>
       </c>
       <c r="E132" s="5" t="s">
         <v>58</v>
@@ -8270,7 +8270,7 @@
         <v>57</v>
       </c>
       <c r="D133" s="4" t="s">
-        <v>345</v>
+        <v>325</v>
       </c>
       <c r="E133" s="5" t="s">
         <v>58</v>
@@ -8320,7 +8320,7 @@
         <v>57</v>
       </c>
       <c r="D134" s="4" t="s">
-        <v>346</v>
+        <v>368</v>
       </c>
       <c r="E134" s="5" t="s">
         <v>58</v>
@@ -8367,7 +8367,7 @@
         <v>57</v>
       </c>
       <c r="D135" s="4" t="s">
-        <v>347</v>
+        <v>326</v>
       </c>
       <c r="E135" s="5" t="s">
         <v>58</v>
@@ -8420,7 +8420,7 @@
         <v>57</v>
       </c>
       <c r="D136" s="4" t="s">
-        <v>348</v>
+        <v>327</v>
       </c>
       <c r="E136" s="5" t="s">
         <v>58</v>
@@ -8473,7 +8473,7 @@
         <v>57</v>
       </c>
       <c r="D137" s="6" t="s">
-        <v>349</v>
+        <v>328</v>
       </c>
       <c r="E137" s="5" t="s">
         <v>58</v>
@@ -8523,7 +8523,7 @@
         <v>57</v>
       </c>
       <c r="D138" s="6" t="s">
-        <v>350</v>
+        <v>329</v>
       </c>
       <c r="E138" s="5" t="s">
         <v>58</v>
@@ -8588,7 +8588,7 @@
         <v>57</v>
       </c>
       <c r="D139" s="4" t="s">
-        <v>354</v>
+        <v>372</v>
       </c>
       <c r="E139" s="5" t="s">
         <v>58</v>
@@ -8673,7 +8673,7 @@
         <v>57</v>
       </c>
       <c r="D141" s="4" t="s">
-        <v>356</v>
+        <v>374</v>
       </c>
       <c r="E141" s="5" t="s">
         <v>58</v>
@@ -8714,7 +8714,7 @@
         <v>57</v>
       </c>
       <c r="D142" s="4" t="s">
-        <v>357</v>
+        <v>375</v>
       </c>
       <c r="E142" s="5" t="s">
         <v>58</v>
@@ -8755,13 +8755,13 @@
         <v>57</v>
       </c>
       <c r="D143" s="4" t="s">
-        <v>358</v>
+        <v>376</v>
       </c>
       <c r="E143" s="5" t="s">
         <v>58</v>
       </c>
       <c r="F143" s="6" t="s">
-        <v>379</v>
+        <v>341</v>
       </c>
       <c r="G143" s="7" t="s">
         <v>290</v>
@@ -8796,7 +8796,7 @@
         <v>57</v>
       </c>
       <c r="D144" s="4" t="s">
-        <v>359</v>
+        <v>377</v>
       </c>
       <c r="E144" s="5" t="s">
         <v>58</v>
@@ -8837,13 +8837,13 @@
         <v>57</v>
       </c>
       <c r="D145" s="4" t="s">
-        <v>380</v>
+        <v>342</v>
       </c>
       <c r="E145" s="5" t="s">
         <v>58</v>
       </c>
       <c r="F145" s="6" t="s">
-        <v>381</v>
+        <v>343</v>
       </c>
       <c r="G145" s="7" t="s">
         <v>292</v>
@@ -8878,13 +8878,13 @@
         <v>57</v>
       </c>
       <c r="D146" s="4" t="s">
-        <v>382</v>
+        <v>344</v>
       </c>
       <c r="E146" s="5" t="s">
         <v>58</v>
       </c>
       <c r="F146" s="6" t="s">
-        <v>383</v>
+        <v>345</v>
       </c>
       <c r="G146" s="7" t="s">
         <v>292</v>
@@ -8919,7 +8919,7 @@
         <v>57</v>
       </c>
       <c r="D147" s="4" t="s">
-        <v>360</v>
+        <v>378</v>
       </c>
       <c r="E147" s="5" t="s">
         <v>58</v>
@@ -8960,7 +8960,7 @@
         <v>57</v>
       </c>
       <c r="D148" s="4" t="s">
-        <v>361</v>
+        <v>379</v>
       </c>
       <c r="E148" s="5" t="s">
         <v>58</v>
@@ -9001,13 +9001,13 @@
         <v>57</v>
       </c>
       <c r="D149" s="4" t="s">
-        <v>362</v>
+        <v>330</v>
       </c>
       <c r="E149" s="5" t="s">
         <v>58</v>
       </c>
       <c r="F149" s="6" t="s">
-        <v>384</v>
+        <v>346</v>
       </c>
       <c r="G149" s="7" t="s">
         <v>292</v>
@@ -9042,7 +9042,7 @@
         <v>57</v>
       </c>
       <c r="D150" s="4" t="s">
-        <v>363</v>
+        <v>380</v>
       </c>
       <c r="E150" s="5" t="s">
         <v>58</v>
@@ -9083,7 +9083,7 @@
         <v>57</v>
       </c>
       <c r="D151" s="16" t="s">
-        <v>364</v>
+        <v>381</v>
       </c>
       <c r="E151" s="5" t="s">
         <v>58</v>
@@ -9118,7 +9118,7 @@
         <v>57</v>
       </c>
       <c r="D152" s="6" t="s">
-        <v>365</v>
+        <v>331</v>
       </c>
       <c r="E152" s="5" t="s">
         <v>58</v>
@@ -9156,7 +9156,7 @@
         <v>57</v>
       </c>
       <c r="D153" s="6" t="s">
-        <v>366</v>
+        <v>332</v>
       </c>
       <c r="E153" s="5" t="s">
         <v>58</v>
@@ -9194,7 +9194,7 @@
         <v>57</v>
       </c>
       <c r="D154" s="6" t="s">
-        <v>367</v>
+        <v>333</v>
       </c>
       <c r="E154" s="5" t="s">
         <v>58</v>
@@ -9232,7 +9232,7 @@
         <v>57</v>
       </c>
       <c r="D155" s="6" t="s">
-        <v>368</v>
+        <v>382</v>
       </c>
       <c r="E155" s="5" t="s">
         <v>58</v>
@@ -9270,7 +9270,7 @@
         <v>57</v>
       </c>
       <c r="D156" s="6" t="s">
-        <v>369</v>
+        <v>383</v>
       </c>
       <c r="E156" s="5" t="s">
         <v>58</v>
@@ -9308,13 +9308,13 @@
         <v>57</v>
       </c>
       <c r="D157" s="6" t="s">
-        <v>370</v>
+        <v>384</v>
       </c>
       <c r="E157" s="5" t="s">
         <v>58</v>
       </c>
       <c r="F157" s="18" t="s">
-        <v>385</v>
+        <v>347</v>
       </c>
       <c r="G157" s="7" t="s">
         <v>292</v>
@@ -9346,7 +9346,7 @@
         <v>57</v>
       </c>
       <c r="D158" s="16" t="s">
-        <v>371</v>
+        <v>385</v>
       </c>
       <c r="E158" s="5" t="s">
         <v>58</v>
@@ -9422,7 +9422,7 @@
         <v>57</v>
       </c>
       <c r="D160" s="4" t="s">
-        <v>356</v>
+        <v>374</v>
       </c>
       <c r="E160" s="5" t="s">
         <v>58</v>
@@ -9463,7 +9463,7 @@
         <v>57</v>
       </c>
       <c r="D161" s="4" t="s">
-        <v>357</v>
+        <v>375</v>
       </c>
       <c r="E161" s="5" t="s">
         <v>58</v>
@@ -9504,13 +9504,13 @@
         <v>57</v>
       </c>
       <c r="D162" s="4" t="s">
-        <v>380</v>
+        <v>342</v>
       </c>
       <c r="E162" s="5" t="s">
         <v>58</v>
       </c>
       <c r="F162" s="6" t="s">
-        <v>381</v>
+        <v>343</v>
       </c>
       <c r="G162" s="7" t="s">
         <v>292</v>
@@ -9548,13 +9548,13 @@
         <v>57</v>
       </c>
       <c r="D163" s="4" t="s">
-        <v>382</v>
+        <v>344</v>
       </c>
       <c r="E163" s="5" t="s">
         <v>58</v>
       </c>
       <c r="F163" s="6" t="s">
-        <v>383</v>
+        <v>345</v>
       </c>
       <c r="G163" s="7" t="s">
         <v>292</v>
@@ -9636,7 +9636,7 @@
         <v>57</v>
       </c>
       <c r="D165" s="4" t="s">
-        <v>356</v>
+        <v>374</v>
       </c>
       <c r="E165" s="5" t="s">
         <v>58</v>
@@ -9695,7 +9695,7 @@
         <v>57</v>
       </c>
       <c r="D166" s="4" t="s">
-        <v>357</v>
+        <v>375</v>
       </c>
       <c r="E166" s="5" t="s">
         <v>58</v>
@@ -9754,13 +9754,13 @@
         <v>57</v>
       </c>
       <c r="D167" s="4" t="s">
-        <v>380</v>
+        <v>342</v>
       </c>
       <c r="E167" s="5" t="s">
         <v>58</v>
       </c>
       <c r="F167" s="6" t="s">
-        <v>381</v>
+        <v>343</v>
       </c>
       <c r="G167" s="7" t="s">
         <v>292</v>
@@ -9798,13 +9798,13 @@
         <v>57</v>
       </c>
       <c r="D168" s="4" t="s">
-        <v>382</v>
+        <v>344</v>
       </c>
       <c r="E168" s="5" t="s">
         <v>58</v>
       </c>
       <c r="F168" s="6" t="s">
-        <v>383</v>
+        <v>345</v>
       </c>
       <c r="G168" s="7" t="s">
         <v>292</v>
@@ -9842,7 +9842,7 @@
         <v>57</v>
       </c>
       <c r="D169" s="6" t="s">
-        <v>304</v>
+        <v>348</v>
       </c>
       <c r="E169" s="5" t="s">
         <v>58</v>
@@ -9889,7 +9889,7 @@
         <v>57</v>
       </c>
       <c r="D170" s="6" t="s">
-        <v>309</v>
+        <v>352</v>
       </c>
       <c r="E170" s="5" t="s">
         <v>58</v>
@@ -9936,7 +9936,7 @@
         <v>57</v>
       </c>
       <c r="D171" s="6" t="s">
-        <v>310</v>
+        <v>353</v>
       </c>
       <c r="E171" s="5" t="s">
         <v>58</v>

</xml_diff>

<commit_message>
dodana obsluga parametrow istniejacych tekstow i tektow pisma; dodane generowanie skryptu delete -'skasuj to co dodales'
</commit_message>
<xml_diff>
--- a/UEFTA_Teksty.xlsx
+++ b/UEFTA_Teksty.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="6540" yWindow="15" windowWidth="13950" windowHeight="7725" tabRatio="369"/>
+    <workbookView xWindow="7470" yWindow="15" windowWidth="13950" windowHeight="7725" tabRatio="419"/>
   </bookViews>
   <sheets>
     <sheet name="toSOS_S_TEKSTOW" sheetId="1" r:id="rId1"/>
@@ -12,14 +12,14 @@
     <sheet name="parametry" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">toSOS_S_TEKSTOW!$A$1:$AE$175</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">toSOS_S_TEKSTOW!$A$1:$AE$176</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1963" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1985" uniqueCount="516">
   <si>
     <t>Po ponownym ustaleniu wysokość &lt;NAZWASWIADCZENIAGL&gt; wynosi: 
 &lt;KWOTAKAPITALUPOCZATKOWEGOKOR&gt;/&lt;SREDNIEDALSZETRWANIEZYCIA&gt; = &lt;KWOTAEMERYTURYKOR&gt; zł.</t>
@@ -1586,13 +1586,22 @@
     <t>48062</t>
   </si>
   <si>
-    <t>T2b_2</t>
-  </si>
-  <si>
     <t>3534</t>
   </si>
   <si>
     <t>48057</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T2b_2 </t>
+  </si>
+  <si>
+    <t>272</t>
+  </si>
+  <si>
+    <t>273</t>
+  </si>
+  <si>
+    <t>274</t>
   </si>
 </sst>
 </file>
@@ -2037,21 +2046,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE176"/>
+  <dimension ref="A1:AE178"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A170" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E176" sqref="E176"/>
+      <selection pane="bottomLeft" activeCell="D186" sqref="D186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.5703125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="27.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="27.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="40.5703125" style="3" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" style="3" customWidth="1"/>
     <col min="8" max="8" width="11" style="12" customWidth="1"/>
     <col min="9" max="9" width="14.42578125" style="12" customWidth="1"/>
@@ -9612,6 +9621,12 @@
       <c r="AE173" s="14"/>
     </row>
     <row r="174" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A174" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="B174" s="3" t="s">
+        <v>513</v>
+      </c>
       <c r="C174" s="3" t="s">
         <v>506</v>
       </c>
@@ -9633,25 +9648,25 @@
       <c r="K174" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="M174" s="12" t="s">
-        <v>89</v>
-      </c>
       <c r="AE174" s="12" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
     </row>
     <row r="175" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A175" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="B175" s="3" t="s">
+        <v>513</v>
+      </c>
       <c r="C175" s="3" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>507</v>
-      </c>
-      <c r="E175" s="3" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="G175" s="3" t="s">
-        <v>92</v>
+        <v>502</v>
       </c>
       <c r="H175" s="12" t="s">
         <v>88</v>
@@ -9670,14 +9685,20 @@
       </c>
     </row>
     <row r="176" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A176" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="B176" s="3" t="s">
+        <v>514</v>
+      </c>
       <c r="C176" s="3" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="E176" s="3" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="G176" s="3" t="s">
         <v>92</v>
@@ -9695,8 +9716,72 @@
         <v>73</v>
       </c>
     </row>
+    <row r="177" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A177" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="B177" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="C177" s="3" t="s">
+        <v>508</v>
+      </c>
+      <c r="D177" s="3" t="s">
+        <v>507</v>
+      </c>
+      <c r="G177" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H177" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="I177" s="12">
+        <v>3003</v>
+      </c>
+      <c r="K177" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="M177" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="AE177" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="178" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A178" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="B178" s="3" t="s">
+        <v>515</v>
+      </c>
+      <c r="C178" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="D178" s="3" t="s">
+        <v>512</v>
+      </c>
+      <c r="E178" s="3" t="s">
+        <v>511</v>
+      </c>
+      <c r="G178" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H178" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="I178" s="12">
+        <v>3003</v>
+      </c>
+      <c r="K178" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE178" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:AE175"/>
+  <autoFilter ref="A1:AE176"/>
   <sortState columnSort="1" ref="K1:T168">
     <sortCondition ref="K1:T1"/>
   </sortState>

</xml_diff>

<commit_message>
use of .config file, counters, ...
</commit_message>
<xml_diff>
--- a/UEFTA_Teksty.xlsx
+++ b/UEFTA_Teksty.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="7470" yWindow="15" windowWidth="13950" windowHeight="7725" tabRatio="419"/>
+    <workbookView xWindow="8400" yWindow="15" windowWidth="13950" windowHeight="7725" tabRatio="465"/>
   </bookViews>
   <sheets>
     <sheet name="toSOS_S_TEKSTOW" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1985" uniqueCount="516">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2165" uniqueCount="567">
   <si>
     <t>Po ponownym ustaleniu wysokość &lt;NAZWASWIADCZENIAGL&gt; wynosi: 
 &lt;KWOTAKAPITALUPOCZATKOWEGOKOR&gt;/&lt;SREDNIEDALSZETRWANIEZYCIA&gt; = &lt;KWOTAEMERYTURYKOR&gt; zł.</t>
@@ -1603,17 +1603,178 @@
   <si>
     <t>274</t>
   </si>
+  <si>
+    <t>48241</t>
+  </si>
+  <si>
+    <t>4960</t>
+  </si>
+  <si>
+    <t>4961</t>
+  </si>
+  <si>
+    <t>4962</t>
+  </si>
+  <si>
+    <t>48242</t>
+  </si>
+  <si>
+    <t>48243</t>
+  </si>
+  <si>
+    <t>12467</t>
+  </si>
+  <si>
+    <t>12468</t>
+  </si>
+  <si>
+    <t>12469</t>
+  </si>
+  <si>
+    <t>8836</t>
+  </si>
+  <si>
+    <t>8837</t>
+  </si>
+  <si>
+    <t>8838</t>
+  </si>
+  <si>
+    <t>12763</t>
+  </si>
+  <si>
+    <t>12764</t>
+  </si>
+  <si>
+    <t>12765</t>
+  </si>
+  <si>
+    <t>5572</t>
+  </si>
+  <si>
+    <t>5573</t>
+  </si>
+  <si>
+    <t>13621</t>
+  </si>
+  <si>
+    <t>13622</t>
+  </si>
+  <si>
+    <t>T8_29</t>
+  </si>
+  <si>
+    <t>T8_30</t>
+  </si>
+  <si>
+    <t>T8_31</t>
+  </si>
+  <si>
+    <t>5546</t>
+  </si>
+  <si>
+    <t>5547</t>
+  </si>
+  <si>
+    <t>5548</t>
+  </si>
+  <si>
+    <t>46703</t>
+  </si>
+  <si>
+    <t>46704</t>
+  </si>
+  <si>
+    <t>46705</t>
+  </si>
+  <si>
+    <t>4645</t>
+  </si>
+  <si>
+    <t>4646</t>
+  </si>
+  <si>
+    <t>4647</t>
+  </si>
+  <si>
+    <t>275</t>
+  </si>
+  <si>
+    <t>276</t>
+  </si>
+  <si>
+    <t>277</t>
+  </si>
+  <si>
+    <t>278</t>
+  </si>
+  <si>
+    <t>279</t>
+  </si>
+  <si>
+    <t>280</t>
+  </si>
+  <si>
+    <t>281</t>
+  </si>
+  <si>
+    <t>282</t>
+  </si>
+  <si>
+    <t>283</t>
+  </si>
+  <si>
+    <t>284</t>
+  </si>
+  <si>
+    <t>285</t>
+  </si>
+  <si>
+    <t>286</t>
+  </si>
+  <si>
+    <t>287</t>
+  </si>
+  <si>
+    <t>288</t>
+  </si>
+  <si>
+    <t>289</t>
+  </si>
+  <si>
+    <t>290</t>
+  </si>
+  <si>
+    <t>291</t>
+  </si>
+  <si>
+    <t>292</t>
+  </si>
+  <si>
+    <t>293</t>
+  </si>
+  <si>
+    <t>294</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1654,6 +1815,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1672,78 +1840,82 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="3"/>
+    <cellStyle name="Normal 3" xfId="2"/>
     <cellStyle name="Normalny 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2046,11 +2218,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE178"/>
+  <dimension ref="A1:AE198"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A170" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D186" sqref="D186"/>
+      <pane ySplit="1" topLeftCell="A182" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D201" sqref="D201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2058,26 +2230,25 @@
     <col min="1" max="1" width="6.5703125" style="3" customWidth="1"/>
     <col min="2" max="2" width="7.5703125" style="3" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="27.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" style="3" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="40.5703125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" style="3" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" style="3" customWidth="1"/>
     <col min="8" max="8" width="11" style="12" customWidth="1"/>
     <col min="9" max="9" width="14.42578125" style="12" customWidth="1"/>
-    <col min="10" max="10" width="8.140625" style="12" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" style="12" customWidth="1"/>
+    <col min="10" max="10" width="3.7109375" style="12" customWidth="1"/>
+    <col min="11" max="11" width="5" style="12" customWidth="1"/>
     <col min="12" max="12" width="7.7109375" style="12" customWidth="1"/>
-    <col min="13" max="13" width="15.7109375" style="12" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" style="12" customWidth="1"/>
     <col min="14" max="14" width="4.28515625" style="12" customWidth="1"/>
-    <col min="15" max="15" width="7.28515625" style="12" customWidth="1"/>
+    <col min="15" max="15" width="4.140625" style="12" customWidth="1"/>
     <col min="16" max="16" width="2.85546875" style="12" customWidth="1"/>
-    <col min="17" max="17" width="11.85546875" style="12" customWidth="1"/>
-    <col min="18" max="18" width="11.28515625" style="12" customWidth="1"/>
+    <col min="17" max="18" width="5.28515625" style="12" customWidth="1"/>
     <col min="19" max="19" width="4.5703125" style="12" customWidth="1"/>
-    <col min="20" max="20" width="8.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="3.7109375" style="12" customWidth="1"/>
     <col min="21" max="28" width="3.5703125" style="12" customWidth="1"/>
     <col min="29" max="29" width="3.85546875" style="12" customWidth="1"/>
-    <col min="30" max="30" width="5.42578125" style="12" customWidth="1"/>
+    <col min="30" max="30" width="4.42578125" style="12" customWidth="1"/>
     <col min="31" max="31" width="4.140625" style="12" customWidth="1"/>
     <col min="32" max="16384" width="9.140625" style="12"/>
   </cols>
@@ -9780,6 +9951,697 @@
         <v>73</v>
       </c>
     </row>
+    <row r="179" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A179" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="B179" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="C179" s="3" t="s">
+        <v>517</v>
+      </c>
+      <c r="D179" s="3" t="s">
+        <v>484</v>
+      </c>
+      <c r="E179" s="3" t="s">
+        <v>516</v>
+      </c>
+      <c r="G179" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H179" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="I179" s="12">
+        <v>3003</v>
+      </c>
+      <c r="J179" s="12">
+        <v>1</v>
+      </c>
+      <c r="K179" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE179" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="180" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A180" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="B180" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="C180" s="3" t="s">
+        <v>518</v>
+      </c>
+      <c r="D180" s="3" t="s">
+        <v>485</v>
+      </c>
+      <c r="E180" s="3" t="s">
+        <v>520</v>
+      </c>
+      <c r="G180" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H180" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="I180" s="12">
+        <v>3003</v>
+      </c>
+      <c r="J180" s="12">
+        <v>1</v>
+      </c>
+      <c r="K180" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE180" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="181" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A181" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="B181" s="3" t="s">
+        <v>549</v>
+      </c>
+      <c r="C181" s="3" t="s">
+        <v>519</v>
+      </c>
+      <c r="D181" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="E181" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="G181" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H181" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="I181" s="12">
+        <v>3003</v>
+      </c>
+      <c r="J181" s="12">
+        <v>1</v>
+      </c>
+      <c r="K181" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE181" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="182" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A182" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="B182" s="3" t="s">
+        <v>550</v>
+      </c>
+      <c r="C182" s="3" t="s">
+        <v>517</v>
+      </c>
+      <c r="D182" s="3" t="s">
+        <v>484</v>
+      </c>
+      <c r="E182" s="3" t="s">
+        <v>522</v>
+      </c>
+      <c r="G182" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H182" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="I182" s="12">
+        <v>3056</v>
+      </c>
+      <c r="J182" s="12">
+        <v>1</v>
+      </c>
+      <c r="K182" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE182" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="183" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A183" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="B183" s="3" t="s">
+        <v>551</v>
+      </c>
+      <c r="C183" s="3" t="s">
+        <v>518</v>
+      </c>
+      <c r="D183" s="3" t="s">
+        <v>485</v>
+      </c>
+      <c r="E183" s="3" t="s">
+        <v>523</v>
+      </c>
+      <c r="G183" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H183" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="I183" s="12">
+        <v>3056</v>
+      </c>
+      <c r="J183" s="12">
+        <v>1</v>
+      </c>
+      <c r="K183" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE183" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="184" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A184" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="B184" s="3" t="s">
+        <v>552</v>
+      </c>
+      <c r="C184" s="3" t="s">
+        <v>519</v>
+      </c>
+      <c r="D184" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="E184" s="3" t="s">
+        <v>524</v>
+      </c>
+      <c r="G184" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H184" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="I184" s="12">
+        <v>3056</v>
+      </c>
+      <c r="J184" s="12">
+        <v>1</v>
+      </c>
+      <c r="K184" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE184" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="185" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A185" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="B185" s="3" t="s">
+        <v>553</v>
+      </c>
+      <c r="C185" s="3" t="s">
+        <v>517</v>
+      </c>
+      <c r="D185" s="3" t="s">
+        <v>484</v>
+      </c>
+      <c r="E185" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="G185" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H185" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="I185" s="12">
+        <v>3041</v>
+      </c>
+      <c r="J185" s="12">
+        <v>1</v>
+      </c>
+      <c r="K185" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE185" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="186" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A186" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="B186" s="3" t="s">
+        <v>554</v>
+      </c>
+      <c r="C186" s="3" t="s">
+        <v>518</v>
+      </c>
+      <c r="D186" s="3" t="s">
+        <v>485</v>
+      </c>
+      <c r="E186" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="G186" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H186" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="I186" s="12">
+        <v>3041</v>
+      </c>
+      <c r="J186" s="12">
+        <v>1</v>
+      </c>
+      <c r="K186" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE186" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="187" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A187" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="B187" s="3" t="s">
+        <v>555</v>
+      </c>
+      <c r="C187" s="3" t="s">
+        <v>519</v>
+      </c>
+      <c r="D187" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="E187" s="3" t="s">
+        <v>527</v>
+      </c>
+      <c r="G187" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H187" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="I187" s="12">
+        <v>3041</v>
+      </c>
+      <c r="J187" s="12">
+        <v>1</v>
+      </c>
+      <c r="K187" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE187" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="188" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A188" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="B188" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="C188" s="3" t="s">
+        <v>517</v>
+      </c>
+      <c r="D188" s="3" t="s">
+        <v>484</v>
+      </c>
+      <c r="E188" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="G188" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H188" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="I188" s="12">
+        <v>3067</v>
+      </c>
+      <c r="J188" s="12">
+        <v>1</v>
+      </c>
+      <c r="K188" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE188" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="189" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A189" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="B189" s="3" t="s">
+        <v>557</v>
+      </c>
+      <c r="C189" s="3" t="s">
+        <v>518</v>
+      </c>
+      <c r="D189" s="3" t="s">
+        <v>485</v>
+      </c>
+      <c r="E189" s="3" t="s">
+        <v>529</v>
+      </c>
+      <c r="G189" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H189" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="I189" s="12">
+        <v>3067</v>
+      </c>
+      <c r="J189" s="12">
+        <v>1</v>
+      </c>
+      <c r="K189" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE189" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="190" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A190" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="B190" s="3" t="s">
+        <v>558</v>
+      </c>
+      <c r="C190" s="3" t="s">
+        <v>519</v>
+      </c>
+      <c r="D190" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="E190" s="3" t="s">
+        <v>530</v>
+      </c>
+      <c r="G190" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H190" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="I190" s="12">
+        <v>3067</v>
+      </c>
+      <c r="J190" s="12">
+        <v>1</v>
+      </c>
+      <c r="K190" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE190" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="191" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A191" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="B191" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="C191" s="3" t="s">
+        <v>531</v>
+      </c>
+      <c r="D191" s="3" t="s">
+        <v>482</v>
+      </c>
+      <c r="E191" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="G191" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H191" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="I191" s="12">
+        <v>3072</v>
+      </c>
+      <c r="J191" s="12">
+        <v>1</v>
+      </c>
+      <c r="K191" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE191" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="192" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A192" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="B192" s="3" t="s">
+        <v>560</v>
+      </c>
+      <c r="C192" s="3" t="s">
+        <v>532</v>
+      </c>
+      <c r="D192" s="3" t="s">
+        <v>483</v>
+      </c>
+      <c r="E192" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="G192" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H192" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="I192" s="12">
+        <v>3072</v>
+      </c>
+      <c r="J192" s="12">
+        <v>1</v>
+      </c>
+      <c r="K192" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE192" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="193" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A193" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="B193" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="C193" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="D193" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="E193" s="3" t="s">
+        <v>541</v>
+      </c>
+      <c r="G193" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H193" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="I193" s="12">
+        <v>3001</v>
+      </c>
+      <c r="J193" s="12">
+        <v>1</v>
+      </c>
+      <c r="K193" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE193" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="194" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A194" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="B194" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="C194" s="3" t="s">
+        <v>539</v>
+      </c>
+      <c r="D194" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="E194" s="3" t="s">
+        <v>542</v>
+      </c>
+      <c r="G194" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H194" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="I194" s="12">
+        <v>3001</v>
+      </c>
+      <c r="J194" s="12">
+        <v>1</v>
+      </c>
+      <c r="K194" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE194" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="195" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A195" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="B195" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="C195" s="3" t="s">
+        <v>540</v>
+      </c>
+      <c r="D195" s="3" t="s">
+        <v>537</v>
+      </c>
+      <c r="E195" s="3" t="s">
+        <v>543</v>
+      </c>
+      <c r="G195" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H195" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="I195" s="12">
+        <v>3001</v>
+      </c>
+      <c r="J195" s="12">
+        <v>1</v>
+      </c>
+      <c r="K195" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE195" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="196" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A196" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="B196" s="3" t="s">
+        <v>564</v>
+      </c>
+      <c r="C196" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="D196" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="E196" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="G196" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H196" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="I196" s="12">
+        <v>3049</v>
+      </c>
+      <c r="K196" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE196" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="197" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A197" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="B197" s="3" t="s">
+        <v>565</v>
+      </c>
+      <c r="C197" s="3" t="s">
+        <v>539</v>
+      </c>
+      <c r="D197" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="E197" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="G197" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H197" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="I197" s="12">
+        <v>3049</v>
+      </c>
+      <c r="K197" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE197" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="198" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A198" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="B198" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="C198" s="3" t="s">
+        <v>540</v>
+      </c>
+      <c r="D198" s="3" t="s">
+        <v>537</v>
+      </c>
+      <c r="E198" s="3" t="s">
+        <v>546</v>
+      </c>
+      <c r="G198" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H198" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="I198" s="12">
+        <v>3049</v>
+      </c>
+      <c r="K198" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE198" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:AE176"/>
   <sortState columnSort="1" ref="K1:T168">
@@ -9794,11 +10656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B9" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="topRight" activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection sqref="A1:L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>